<commit_message>
Calcular componentes adicionales de terremoto
</commit_message>
<xml_diff>
--- a/prototipo_pcr/inputs/insumos.xlsx
+++ b/prototipo_pcr/inputs/insumos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebatoec/Library/CloudStorage/OneDrive-SharedLibraries-SegurosSuramericana,S.A/Proyecto féniX - féniX/01 IFRS17/02 Entregables Procesos/05 Reservas/03 PCR CP/03 Tecnología/01 Prototipo/prototipo_pcr/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCF92922-4B95-AD4E-85E3-BC84D6413675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC42E67-7DA1-2342-97B9-902C865173C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17440" tabRatio="959" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17440" tabRatio="959" firstSheet="5" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="param_contabilidad" sheetId="6" r:id="rId1"/>
@@ -1496,9 +1496,6 @@
     <t>activo</t>
   </si>
   <si>
-    <t>gasto_total_terremoto</t>
-  </si>
-  <si>
     <t>terremoto</t>
   </si>
   <si>
@@ -1517,13 +1514,16 @@
     <t>expedicion_otros</t>
   </si>
   <si>
-    <t>factor_pprr_terremoto</t>
+    <t>TERREMOTO</t>
   </si>
   <si>
-    <t>valor del gasto total asociado a la producción emitida de terremoto</t>
+    <t>terremoto_factor_pprr</t>
   </si>
   <si>
-    <t>TERREMOTO</t>
+    <t>terremoto_nota_tecnica</t>
+  </si>
+  <si>
+    <t>valor del gasto total de nota tecnica asociado a la produccion emitida de terremoto</t>
   </si>
 </sst>
 </file>
@@ -2094,8 +2094,8 @@
   </sheetPr>
   <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2513,15 +2513,15 @@
         <v>1</v>
       </c>
       <c r="I14" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>352</v>
+        <v>360</v>
       </c>
       <c r="B15" t="s">
-        <v>352</v>
+        <v>360</v>
       </c>
       <c r="C15" t="s">
         <v>102</v>
@@ -2542,7 +2542,7 @@
         <v>1</v>
       </c>
       <c r="I15" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -2571,15 +2571,15 @@
         <v>1</v>
       </c>
       <c r="I16" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>352</v>
+        <v>360</v>
       </c>
       <c r="B17" t="s">
-        <v>352</v>
+        <v>360</v>
       </c>
       <c r="C17" t="s">
         <v>102</v>
@@ -2600,7 +2600,7 @@
         <v>1</v>
       </c>
       <c r="I17" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -4707,13 +4707,13 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A12977D-9D3C-784D-BA64-82A8AADC1B2E}">
-  <sheetPr filterMode="1">
+  <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
   <dimension ref="A1:I261"/>
   <sheetViews>
-    <sheetView zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A141" zoomScale="112" zoomScaleNormal="73" workbookViewId="0">
+      <selection activeCell="B156" sqref="B156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4912,7 +4912,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="51" t="s">
         <v>59</v>
       </c>
@@ -4964,7 +4964,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="51" t="s">
         <v>59</v>
       </c>
@@ -5172,7 +5172,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="51" t="s">
         <v>59</v>
       </c>
@@ -5354,7 +5354,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="51" t="s">
         <v>60</v>
       </c>
@@ -5536,7 +5536,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="51" t="s">
         <v>61</v>
       </c>
@@ -5562,7 +5562,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="51" t="s">
         <v>59</v>
       </c>
@@ -5588,7 +5588,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="51" t="s">
         <v>60</v>
       </c>
@@ -5614,7 +5614,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="51" t="s">
         <v>61</v>
       </c>
@@ -5640,7 +5640,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="51" t="s">
         <v>59</v>
       </c>
@@ -5666,7 +5666,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="51" t="s">
         <v>60</v>
       </c>
@@ -5692,7 +5692,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="51" t="s">
         <v>61</v>
       </c>
@@ -5952,7 +5952,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="51" t="s">
         <v>59</v>
       </c>
@@ -6134,7 +6134,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="51" t="s">
         <v>60</v>
       </c>
@@ -6316,7 +6316,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="62" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="51" t="s">
         <v>61</v>
       </c>
@@ -6342,7 +6342,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="63" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="51" t="s">
         <v>59</v>
       </c>
@@ -6368,7 +6368,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="51" t="s">
         <v>60</v>
       </c>
@@ -6394,7 +6394,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="51" t="s">
         <v>61</v>
       </c>
@@ -6420,7 +6420,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="66" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" s="51" t="s">
         <v>59</v>
       </c>
@@ -6446,7 +6446,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="67" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" s="51" t="s">
         <v>60</v>
       </c>
@@ -6472,7 +6472,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="68" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" s="51" t="s">
         <v>61</v>
       </c>
@@ -6732,7 +6732,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="78" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" s="51" t="s">
         <v>59</v>
       </c>
@@ -6914,7 +6914,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="85" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" s="51" t="s">
         <v>60</v>
       </c>
@@ -7096,7 +7096,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" s="51" t="s">
         <v>61</v>
       </c>
@@ -7122,7 +7122,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="93" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" s="51" t="s">
         <v>59</v>
       </c>
@@ -7148,7 +7148,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="94" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" s="51" t="s">
         <v>60</v>
       </c>
@@ -7174,7 +7174,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="95" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" s="51" t="s">
         <v>61</v>
       </c>
@@ -7200,7 +7200,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="96" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" s="51" t="s">
         <v>59</v>
       </c>
@@ -7226,7 +7226,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="97" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" s="51" t="s">
         <v>60</v>
       </c>
@@ -7252,7 +7252,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="98" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" s="51" t="s">
         <v>61</v>
       </c>
@@ -7512,7 +7512,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="108" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" s="51" t="s">
         <v>59</v>
       </c>
@@ -7694,7 +7694,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="115" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" s="51" t="s">
         <v>60</v>
       </c>
@@ -7876,7 +7876,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="122" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A122" s="51" t="s">
         <v>61</v>
       </c>
@@ -7902,7 +7902,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="123" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A123" s="51" t="s">
         <v>59</v>
       </c>
@@ -7928,7 +7928,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="124" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A124" s="51" t="s">
         <v>60</v>
       </c>
@@ -7954,7 +7954,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="125" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A125" s="51" t="s">
         <v>61</v>
       </c>
@@ -7980,7 +7980,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="126" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A126" s="51" t="s">
         <v>59</v>
       </c>
@@ -8006,7 +8006,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="127" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A127" s="51" t="s">
         <v>60</v>
       </c>
@@ -8032,7 +8032,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="128" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A128" s="51" t="s">
         <v>61</v>
       </c>
@@ -8292,7 +8292,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="138" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A138" s="51" t="s">
         <v>59</v>
       </c>
@@ -8318,7 +8318,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="139" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A139" s="51" t="s">
         <v>59</v>
       </c>
@@ -8344,7 +8344,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="140" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A140" s="51" t="s">
         <v>59</v>
       </c>
@@ -8552,7 +8552,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="148" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A148" s="51" t="s">
         <v>59</v>
       </c>
@@ -8578,7 +8578,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="149" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A149" s="51" t="s">
         <v>59</v>
       </c>
@@ -8604,7 +8604,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="150" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A150" s="51" t="s">
         <v>59</v>
       </c>
@@ -8812,7 +8812,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="158" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A158" s="51" t="s">
         <v>59</v>
       </c>
@@ -8994,7 +8994,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="165" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A165" s="51" t="s">
         <v>60</v>
       </c>
@@ -9176,7 +9176,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="172" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A172" s="51" t="s">
         <v>61</v>
       </c>
@@ -9202,7 +9202,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="173" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A173" s="51" t="s">
         <v>59</v>
       </c>
@@ -9228,7 +9228,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="174" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A174" s="51" t="s">
         <v>60</v>
       </c>
@@ -9254,7 +9254,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="175" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A175" s="51" t="s">
         <v>61</v>
       </c>
@@ -9280,7 +9280,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="176" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A176" s="51" t="s">
         <v>59</v>
       </c>
@@ -9306,7 +9306,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="177" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A177" s="51" t="s">
         <v>60</v>
       </c>
@@ -9332,7 +9332,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="178" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A178" s="51" t="s">
         <v>61</v>
       </c>
@@ -9592,7 +9592,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="188" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A188" s="51" t="s">
         <v>59</v>
       </c>
@@ -9618,7 +9618,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="189" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A189" s="51" t="s">
         <v>59</v>
       </c>
@@ -9644,7 +9644,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="190" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A190" s="51" t="s">
         <v>59</v>
       </c>
@@ -9852,7 +9852,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="198" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A198" s="51" t="s">
         <v>59</v>
       </c>
@@ -10034,7 +10034,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="205" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A205" s="51" t="s">
         <v>60</v>
       </c>
@@ -10216,7 +10216,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="212" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A212" s="51" t="s">
         <v>61</v>
       </c>
@@ -10242,7 +10242,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="213" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A213" s="51" t="s">
         <v>59</v>
       </c>
@@ -10268,7 +10268,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="214" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A214" s="51" t="s">
         <v>60</v>
       </c>
@@ -10294,7 +10294,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="215" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A215" s="51" t="s">
         <v>61</v>
       </c>
@@ -10320,7 +10320,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="216" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A216" s="51" t="s">
         <v>59</v>
       </c>
@@ -10346,7 +10346,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="217" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A217" s="51" t="s">
         <v>60</v>
       </c>
@@ -10372,7 +10372,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="218" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A218" s="51" t="s">
         <v>61</v>
       </c>
@@ -10632,7 +10632,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="228" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A228" s="51" t="s">
         <v>59</v>
       </c>
@@ -10658,7 +10658,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="229" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A229" s="51" t="s">
         <v>59</v>
       </c>
@@ -10684,7 +10684,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="230" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A230" s="51" t="s">
         <v>59</v>
       </c>
@@ -10892,7 +10892,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="238" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A238" s="51" t="s">
         <v>59</v>
       </c>
@@ -11074,7 +11074,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="245" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A245" s="51" t="s">
         <v>60</v>
       </c>
@@ -11256,7 +11256,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="252" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A252" s="51" t="s">
         <v>61</v>
       </c>
@@ -11282,7 +11282,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="253" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A253" s="51" t="s">
         <v>59</v>
       </c>
@@ -11308,7 +11308,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="254" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A254" s="51" t="s">
         <v>60</v>
       </c>
@@ -11334,7 +11334,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="255" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A255" s="51" t="s">
         <v>61</v>
       </c>
@@ -11360,7 +11360,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="256" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A256" s="51" t="s">
         <v>59</v>
       </c>
@@ -11386,7 +11386,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="257" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A257" s="51" t="s">
         <v>60</v>
       </c>
@@ -11412,7 +11412,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="258" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A258" s="51" t="s">
         <v>61</v>
       </c>
@@ -11517,13 +11517,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I261" xr:uid="{8A12977D-9D3C-784D-BA64-82A8AADC1B2E}">
-    <filterColumn colId="5">
-      <filters>
-        <filter val="0"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:I261" xr:uid="{8A12977D-9D3C-784D-BA64-82A8AADC1B2E}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <legacyDrawing r:id="rId1"/>
@@ -12863,8 +12857,8 @@
   </sheetPr>
   <dimension ref="A1:I209"/>
   <sheetViews>
-    <sheetView topLeftCell="A195" zoomScale="150" workbookViewId="0">
-      <selection activeCell="G198" sqref="G198"/>
+    <sheetView topLeftCell="A202" zoomScale="150" workbookViewId="0">
+      <selection activeCell="G207" sqref="G207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12876,7 +12870,7 @@
     <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -12903,10 +12897,10 @@
         <v>15</v>
       </c>
       <c r="H1" s="5" t="s">
+        <v>354</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>355</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -12932,7 +12926,7 @@
         <v>8</v>
       </c>
       <c r="H2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I2">
         <v>0.1</v>
@@ -12961,7 +12955,7 @@
         <v>47</v>
       </c>
       <c r="H3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I3">
         <v>0.2</v>
@@ -12990,7 +12984,7 @@
         <v>8</v>
       </c>
       <c r="H4" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I4">
         <v>1.1000000000000001</v>
@@ -13019,7 +13013,7 @@
         <v>8</v>
       </c>
       <c r="H5" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I5">
         <v>0.13</v>
@@ -13048,7 +13042,7 @@
         <v>8</v>
       </c>
       <c r="H6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I6">
         <v>0.15</v>
@@ -13077,7 +13071,7 @@
         <v>8</v>
       </c>
       <c r="H7" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I7">
         <v>0.7</v>
@@ -13106,7 +13100,7 @@
         <v>8</v>
       </c>
       <c r="H8" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I8">
         <v>0.1</v>
@@ -13135,7 +13129,7 @@
         <v>47</v>
       </c>
       <c r="H9" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I9">
         <v>0.2</v>
@@ -13164,7 +13158,7 @@
         <v>8</v>
       </c>
       <c r="H10" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I10">
         <v>1.1000000000000001</v>
@@ -13193,7 +13187,7 @@
         <v>8</v>
       </c>
       <c r="H11" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I11">
         <v>0.13</v>
@@ -13222,7 +13216,7 @@
         <v>8</v>
       </c>
       <c r="H12" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I12">
         <v>0.15</v>
@@ -13251,7 +13245,7 @@
         <v>8</v>
       </c>
       <c r="H13" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I13">
         <v>0.7</v>
@@ -13280,7 +13274,7 @@
         <v>8</v>
       </c>
       <c r="H14" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I14">
         <v>0.1</v>
@@ -13309,7 +13303,7 @@
         <v>47</v>
       </c>
       <c r="H15" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I15">
         <v>0.2</v>
@@ -13338,7 +13332,7 @@
         <v>8</v>
       </c>
       <c r="H16" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I16">
         <v>1.1000000000000001</v>
@@ -13367,7 +13361,7 @@
         <v>8</v>
       </c>
       <c r="H17" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I17">
         <v>0.13</v>
@@ -13396,7 +13390,7 @@
         <v>8</v>
       </c>
       <c r="H18" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I18">
         <v>0.15</v>
@@ -13425,7 +13419,7 @@
         <v>8</v>
       </c>
       <c r="H19" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I19">
         <v>0.7</v>
@@ -13454,7 +13448,7 @@
         <v>8</v>
       </c>
       <c r="H20" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I20">
         <v>0.1</v>
@@ -13483,7 +13477,7 @@
         <v>47</v>
       </c>
       <c r="H21" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I21">
         <v>0.2</v>
@@ -13512,7 +13506,7 @@
         <v>8</v>
       </c>
       <c r="H22" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I22">
         <v>1.1000000000000001</v>
@@ -13541,7 +13535,7 @@
         <v>8</v>
       </c>
       <c r="H23" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I23">
         <v>0.13</v>
@@ -13570,7 +13564,7 @@
         <v>8</v>
       </c>
       <c r="H24" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I24">
         <v>0.15</v>
@@ -13599,7 +13593,7 @@
         <v>8</v>
       </c>
       <c r="H25" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I25">
         <v>0.7</v>
@@ -13628,7 +13622,7 @@
         <v>8</v>
       </c>
       <c r="H26" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I26">
         <v>0</v>
@@ -13657,7 +13651,7 @@
         <v>8</v>
       </c>
       <c r="H27" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I27">
         <v>0</v>
@@ -13686,7 +13680,7 @@
         <v>8</v>
       </c>
       <c r="H28" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I28">
         <v>0</v>
@@ -13715,7 +13709,7 @@
         <v>8</v>
       </c>
       <c r="H29" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I29">
         <v>0</v>
@@ -13744,7 +13738,7 @@
         <v>8</v>
       </c>
       <c r="H30" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I30">
         <v>0.1</v>
@@ -13773,7 +13767,7 @@
         <v>47</v>
       </c>
       <c r="H31" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I31">
         <v>0.2</v>
@@ -13802,7 +13796,7 @@
         <v>8</v>
       </c>
       <c r="H32" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I32">
         <v>1.1000000000000001</v>
@@ -13831,7 +13825,7 @@
         <v>8</v>
       </c>
       <c r="H33" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I33">
         <v>0.13</v>
@@ -13860,7 +13854,7 @@
         <v>8</v>
       </c>
       <c r="H34" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I34">
         <v>0.15</v>
@@ -13889,7 +13883,7 @@
         <v>8</v>
       </c>
       <c r="H35" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I35">
         <v>0.7</v>
@@ -13918,7 +13912,7 @@
         <v>8</v>
       </c>
       <c r="H36" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I36">
         <v>0.1</v>
@@ -13947,7 +13941,7 @@
         <v>47</v>
       </c>
       <c r="H37" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I37">
         <v>0.2</v>
@@ -13976,7 +13970,7 @@
         <v>8</v>
       </c>
       <c r="H38" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I38">
         <v>1.1000000000000001</v>
@@ -14005,7 +13999,7 @@
         <v>8</v>
       </c>
       <c r="H39" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I39">
         <v>0.13</v>
@@ -14034,7 +14028,7 @@
         <v>8</v>
       </c>
       <c r="H40" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I40">
         <v>0.15</v>
@@ -14063,7 +14057,7 @@
         <v>8</v>
       </c>
       <c r="H41" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I41">
         <v>0.7</v>
@@ -14092,7 +14086,7 @@
         <v>8</v>
       </c>
       <c r="H42" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I42">
         <v>0.1</v>
@@ -14121,7 +14115,7 @@
         <v>47</v>
       </c>
       <c r="H43" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I43">
         <v>0.2</v>
@@ -14150,7 +14144,7 @@
         <v>8</v>
       </c>
       <c r="H44" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I44">
         <v>1.1000000000000001</v>
@@ -14179,7 +14173,7 @@
         <v>8</v>
       </c>
       <c r="H45" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I45">
         <v>0.13</v>
@@ -14208,7 +14202,7 @@
         <v>8</v>
       </c>
       <c r="H46" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I46">
         <v>0.15</v>
@@ -14237,7 +14231,7 @@
         <v>8</v>
       </c>
       <c r="H47" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I47">
         <v>0.7</v>
@@ -14266,7 +14260,7 @@
         <v>8</v>
       </c>
       <c r="H48" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I48">
         <v>0.1</v>
@@ -14295,7 +14289,7 @@
         <v>47</v>
       </c>
       <c r="H49" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I49">
         <v>0.2</v>
@@ -14324,7 +14318,7 @@
         <v>8</v>
       </c>
       <c r="H50" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I50">
         <v>1.1000000000000001</v>
@@ -14353,7 +14347,7 @@
         <v>8</v>
       </c>
       <c r="H51" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I51">
         <v>0.13</v>
@@ -14382,7 +14376,7 @@
         <v>8</v>
       </c>
       <c r="H52" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I52">
         <v>0.15</v>
@@ -14411,7 +14405,7 @@
         <v>8</v>
       </c>
       <c r="H53" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I53">
         <v>0.7</v>
@@ -14440,7 +14434,7 @@
         <v>8</v>
       </c>
       <c r="H54" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I54">
         <v>0</v>
@@ -14469,7 +14463,7 @@
         <v>8</v>
       </c>
       <c r="H55" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I55">
         <v>0</v>
@@ -14498,7 +14492,7 @@
         <v>8</v>
       </c>
       <c r="H56" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I56">
         <v>0</v>
@@ -14527,7 +14521,7 @@
         <v>8</v>
       </c>
       <c r="H57" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I57">
         <v>0</v>
@@ -14556,7 +14550,7 @@
         <v>8</v>
       </c>
       <c r="H58" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I58">
         <v>0.1</v>
@@ -14585,7 +14579,7 @@
         <v>47</v>
       </c>
       <c r="H59" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I59">
         <v>0.2</v>
@@ -14614,7 +14608,7 @@
         <v>8</v>
       </c>
       <c r="H60" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I60">
         <v>1.1000000000000001</v>
@@ -14643,7 +14637,7 @@
         <v>8</v>
       </c>
       <c r="H61" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I61">
         <v>0.13</v>
@@ -14672,7 +14666,7 @@
         <v>8</v>
       </c>
       <c r="H62" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I62">
         <v>0.15</v>
@@ -14701,7 +14695,7 @@
         <v>8</v>
       </c>
       <c r="H63" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I63">
         <v>0.7</v>
@@ -14730,7 +14724,7 @@
         <v>8</v>
       </c>
       <c r="H64" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I64">
         <v>0.1</v>
@@ -14759,7 +14753,7 @@
         <v>47</v>
       </c>
       <c r="H65" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I65">
         <v>0.2</v>
@@ -14788,7 +14782,7 @@
         <v>8</v>
       </c>
       <c r="H66" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I66">
         <v>1.1000000000000001</v>
@@ -14817,7 +14811,7 @@
         <v>8</v>
       </c>
       <c r="H67" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I67">
         <v>0.13</v>
@@ -14846,7 +14840,7 @@
         <v>8</v>
       </c>
       <c r="H68" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I68">
         <v>0.15</v>
@@ -14875,7 +14869,7 @@
         <v>8</v>
       </c>
       <c r="H69" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I69">
         <v>0.7</v>
@@ -14904,7 +14898,7 @@
         <v>8</v>
       </c>
       <c r="H70" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I70">
         <v>0.1</v>
@@ -14933,7 +14927,7 @@
         <v>47</v>
       </c>
       <c r="H71" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I71">
         <v>0.2</v>
@@ -14962,7 +14956,7 @@
         <v>8</v>
       </c>
       <c r="H72" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I72">
         <v>1.1000000000000001</v>
@@ -14991,7 +14985,7 @@
         <v>8</v>
       </c>
       <c r="H73" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I73">
         <v>0.13</v>
@@ -15020,7 +15014,7 @@
         <v>8</v>
       </c>
       <c r="H74" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I74">
         <v>0.15</v>
@@ -15049,7 +15043,7 @@
         <v>8</v>
       </c>
       <c r="H75" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I75">
         <v>0.7</v>
@@ -15078,7 +15072,7 @@
         <v>8</v>
       </c>
       <c r="H76" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I76">
         <v>0.1</v>
@@ -15107,7 +15101,7 @@
         <v>47</v>
       </c>
       <c r="H77" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I77">
         <v>0.2</v>
@@ -15136,7 +15130,7 @@
         <v>8</v>
       </c>
       <c r="H78" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I78">
         <v>1.1000000000000001</v>
@@ -15165,7 +15159,7 @@
         <v>8</v>
       </c>
       <c r="H79" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I79">
         <v>0.13</v>
@@ -15194,7 +15188,7 @@
         <v>8</v>
       </c>
       <c r="H80" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I80">
         <v>0.15</v>
@@ -15223,7 +15217,7 @@
         <v>8</v>
       </c>
       <c r="H81" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I81">
         <v>0.7</v>
@@ -15252,7 +15246,7 @@
         <v>8</v>
       </c>
       <c r="H82" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I82">
         <v>0.15</v>
@@ -15281,7 +15275,7 @@
         <v>8</v>
       </c>
       <c r="H83" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I83">
         <v>0.15</v>
@@ -15310,7 +15304,7 @@
         <v>8</v>
       </c>
       <c r="H84" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I84">
         <v>0.16</v>
@@ -15339,7 +15333,7 @@
         <v>8</v>
       </c>
       <c r="H85" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I85">
         <v>0.16500000000000001</v>
@@ -15368,7 +15362,7 @@
         <v>8</v>
       </c>
       <c r="H86" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I86">
         <v>0.5</v>
@@ -15397,7 +15391,7 @@
         <v>47</v>
       </c>
       <c r="H87" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I87">
         <v>0.1</v>
@@ -15426,7 +15420,7 @@
         <v>8</v>
       </c>
       <c r="H88" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I88">
         <v>0.6</v>
@@ -15455,7 +15449,7 @@
         <v>8</v>
       </c>
       <c r="H89" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I89">
         <v>7.0000000000000007E-2</v>
@@ -15484,7 +15478,7 @@
         <v>8</v>
       </c>
       <c r="H90" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I90">
         <v>0.8</v>
@@ -15513,7 +15507,7 @@
         <v>8</v>
       </c>
       <c r="H91" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I91">
         <v>0.3</v>
@@ -15542,7 +15536,7 @@
         <v>8</v>
       </c>
       <c r="H92" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I92">
         <v>0.5</v>
@@ -15571,7 +15565,7 @@
         <v>47</v>
       </c>
       <c r="H93" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I93">
         <v>0.1</v>
@@ -15600,7 +15594,7 @@
         <v>8</v>
       </c>
       <c r="H94" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I94">
         <v>0.6</v>
@@ -15629,7 +15623,7 @@
         <v>8</v>
       </c>
       <c r="H95" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I95">
         <v>7.0000000000000007E-2</v>
@@ -15658,7 +15652,7 @@
         <v>8</v>
       </c>
       <c r="H96" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I96">
         <v>0.8</v>
@@ -15687,7 +15681,7 @@
         <v>8</v>
       </c>
       <c r="H97" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I97">
         <v>0.3</v>
@@ -15716,7 +15710,7 @@
         <v>8</v>
       </c>
       <c r="H98" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I98">
         <v>0.5</v>
@@ -15745,7 +15739,7 @@
         <v>47</v>
       </c>
       <c r="H99" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I99">
         <v>0.1</v>
@@ -15774,7 +15768,7 @@
         <v>8</v>
       </c>
       <c r="H100" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I100">
         <v>0.6</v>
@@ -15803,7 +15797,7 @@
         <v>8</v>
       </c>
       <c r="H101" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I101">
         <v>7.0000000000000007E-2</v>
@@ -15832,7 +15826,7 @@
         <v>8</v>
       </c>
       <c r="H102" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I102">
         <v>0.8</v>
@@ -15861,7 +15855,7 @@
         <v>8</v>
       </c>
       <c r="H103" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I103">
         <v>0.3</v>
@@ -15890,7 +15884,7 @@
         <v>8</v>
       </c>
       <c r="H104" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I104">
         <v>0.5</v>
@@ -15919,7 +15913,7 @@
         <v>47</v>
       </c>
       <c r="H105" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I105">
         <v>0.1</v>
@@ -15948,7 +15942,7 @@
         <v>8</v>
       </c>
       <c r="H106" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I106">
         <v>0.6</v>
@@ -15977,7 +15971,7 @@
         <v>8</v>
       </c>
       <c r="H107" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I107">
         <v>7.0000000000000007E-2</v>
@@ -16006,7 +16000,7 @@
         <v>8</v>
       </c>
       <c r="H108" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I108">
         <v>0.8</v>
@@ -16035,7 +16029,7 @@
         <v>8</v>
       </c>
       <c r="H109" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I109">
         <v>0.3</v>
@@ -16064,7 +16058,7 @@
         <v>8</v>
       </c>
       <c r="H110" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I110">
         <v>0.21</v>
@@ -16093,7 +16087,7 @@
         <v>8</v>
       </c>
       <c r="H111" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I111">
         <v>0.2</v>
@@ -16122,7 +16116,7 @@
         <v>8</v>
       </c>
       <c r="H112" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I112">
         <v>0.23</v>
@@ -16151,7 +16145,7 @@
         <v>8</v>
       </c>
       <c r="H113" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I113">
         <v>0.22</v>
@@ -16180,7 +16174,7 @@
         <v>8</v>
       </c>
       <c r="H114" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I114">
         <v>0.5</v>
@@ -16209,7 +16203,7 @@
         <v>47</v>
       </c>
       <c r="H115" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I115">
         <v>0.1</v>
@@ -16238,7 +16232,7 @@
         <v>8</v>
       </c>
       <c r="H116" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I116">
         <v>0.6</v>
@@ -16267,7 +16261,7 @@
         <v>8</v>
       </c>
       <c r="H117" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I117">
         <v>7.0000000000000007E-2</v>
@@ -16296,7 +16290,7 @@
         <v>8</v>
       </c>
       <c r="H118" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I118">
         <v>0.8</v>
@@ -16325,7 +16319,7 @@
         <v>8</v>
       </c>
       <c r="H119" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I119">
         <v>0.3</v>
@@ -16354,7 +16348,7 @@
         <v>8</v>
       </c>
       <c r="H120" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I120">
         <v>0.5</v>
@@ -16383,7 +16377,7 @@
         <v>47</v>
       </c>
       <c r="H121" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I121">
         <v>0.1</v>
@@ -16412,7 +16406,7 @@
         <v>8</v>
       </c>
       <c r="H122" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I122">
         <v>0.6</v>
@@ -16441,7 +16435,7 @@
         <v>8</v>
       </c>
       <c r="H123" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I123">
         <v>7.0000000000000007E-2</v>
@@ -16470,7 +16464,7 @@
         <v>8</v>
       </c>
       <c r="H124" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I124">
         <v>0.8</v>
@@ -16499,7 +16493,7 @@
         <v>8</v>
       </c>
       <c r="H125" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I125">
         <v>0.3</v>
@@ -16528,7 +16522,7 @@
         <v>8</v>
       </c>
       <c r="H126" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I126">
         <v>0.5</v>
@@ -16557,7 +16551,7 @@
         <v>47</v>
       </c>
       <c r="H127" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I127">
         <v>0.1</v>
@@ -16586,7 +16580,7 @@
         <v>8</v>
       </c>
       <c r="H128" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I128">
         <v>0.6</v>
@@ -16615,7 +16609,7 @@
         <v>8</v>
       </c>
       <c r="H129" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I129">
         <v>7.0000000000000007E-2</v>
@@ -16644,7 +16638,7 @@
         <v>8</v>
       </c>
       <c r="H130" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I130">
         <v>0.8</v>
@@ -16673,7 +16667,7 @@
         <v>8</v>
       </c>
       <c r="H131" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I131">
         <v>0.3</v>
@@ -16702,7 +16696,7 @@
         <v>8</v>
       </c>
       <c r="H132" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I132">
         <v>0.5</v>
@@ -16731,7 +16725,7 @@
         <v>47</v>
       </c>
       <c r="H133" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I133">
         <v>0.1</v>
@@ -16760,7 +16754,7 @@
         <v>8</v>
       </c>
       <c r="H134" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I134">
         <v>0.6</v>
@@ -16789,7 +16783,7 @@
         <v>8</v>
       </c>
       <c r="H135" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I135">
         <v>7.0000000000000007E-2</v>
@@ -16818,7 +16812,7 @@
         <v>8</v>
       </c>
       <c r="H136" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I136">
         <v>0.8</v>
@@ -16847,7 +16841,7 @@
         <v>8</v>
       </c>
       <c r="H137" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I137">
         <v>0.3</v>
@@ -16876,7 +16870,7 @@
         <v>8</v>
       </c>
       <c r="H138" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I138">
         <v>0.11</v>
@@ -16905,7 +16899,7 @@
         <v>8</v>
       </c>
       <c r="H139" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I139">
         <v>0.13</v>
@@ -16934,7 +16928,7 @@
         <v>8</v>
       </c>
       <c r="H140" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I140">
         <v>0.14000000000000001</v>
@@ -16963,7 +16957,7 @@
         <v>8</v>
       </c>
       <c r="H141" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I141">
         <v>0.14000000000000001</v>
@@ -16992,7 +16986,7 @@
         <v>8</v>
       </c>
       <c r="H142" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I142">
         <v>0.5</v>
@@ -17021,7 +17015,7 @@
         <v>47</v>
       </c>
       <c r="H143" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I143">
         <v>0.1</v>
@@ -17050,7 +17044,7 @@
         <v>8</v>
       </c>
       <c r="H144" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I144">
         <v>0.6</v>
@@ -17079,7 +17073,7 @@
         <v>8</v>
       </c>
       <c r="H145" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I145">
         <v>7.0000000000000007E-2</v>
@@ -17108,7 +17102,7 @@
         <v>8</v>
       </c>
       <c r="H146" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I146">
         <v>0.8</v>
@@ -17137,7 +17131,7 @@
         <v>8</v>
       </c>
       <c r="H147" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I147">
         <v>0.3</v>
@@ -17166,7 +17160,7 @@
         <v>8</v>
       </c>
       <c r="H148" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I148">
         <v>0.5</v>
@@ -17195,7 +17189,7 @@
         <v>47</v>
       </c>
       <c r="H149" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I149">
         <v>0.1</v>
@@ -17224,7 +17218,7 @@
         <v>8</v>
       </c>
       <c r="H150" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I150">
         <v>0.6</v>
@@ -17253,7 +17247,7 @@
         <v>8</v>
       </c>
       <c r="H151" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I151">
         <v>7.0000000000000007E-2</v>
@@ -17282,7 +17276,7 @@
         <v>8</v>
       </c>
       <c r="H152" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I152">
         <v>0.8</v>
@@ -17311,7 +17305,7 @@
         <v>8</v>
       </c>
       <c r="H153" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I153">
         <v>0.3</v>
@@ -17340,7 +17334,7 @@
         <v>8</v>
       </c>
       <c r="H154" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I154">
         <v>0.5</v>
@@ -17369,7 +17363,7 @@
         <v>47</v>
       </c>
       <c r="H155" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I155">
         <v>0.1</v>
@@ -17398,7 +17392,7 @@
         <v>8</v>
       </c>
       <c r="H156" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I156">
         <v>0.6</v>
@@ -17427,7 +17421,7 @@
         <v>8</v>
       </c>
       <c r="H157" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I157">
         <v>7.0000000000000007E-2</v>
@@ -17456,7 +17450,7 @@
         <v>8</v>
       </c>
       <c r="H158" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I158">
         <v>0.8</v>
@@ -17485,7 +17479,7 @@
         <v>8</v>
       </c>
       <c r="H159" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I159">
         <v>0.3</v>
@@ -17514,7 +17508,7 @@
         <v>8</v>
       </c>
       <c r="H160" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I160">
         <v>0.5</v>
@@ -17543,7 +17537,7 @@
         <v>47</v>
       </c>
       <c r="H161" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I161">
         <v>0.1</v>
@@ -17572,7 +17566,7 @@
         <v>8</v>
       </c>
       <c r="H162" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I162">
         <v>0.6</v>
@@ -17601,7 +17595,7 @@
         <v>8</v>
       </c>
       <c r="H163" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I163">
         <v>7.0000000000000007E-2</v>
@@ -17630,7 +17624,7 @@
         <v>8</v>
       </c>
       <c r="H164" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I164">
         <v>0.8</v>
@@ -17659,7 +17653,7 @@
         <v>8</v>
       </c>
       <c r="H165" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I165">
         <v>0.3</v>
@@ -17688,7 +17682,7 @@
         <v>8</v>
       </c>
       <c r="H166" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I166">
         <v>0.11</v>
@@ -17717,7 +17711,7 @@
         <v>8</v>
       </c>
       <c r="H167" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I167">
         <v>0.13</v>
@@ -17746,7 +17740,7 @@
         <v>8</v>
       </c>
       <c r="H168" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I168">
         <v>0.14000000000000001</v>
@@ -17775,7 +17769,7 @@
         <v>8</v>
       </c>
       <c r="H169" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I169">
         <v>0.14000000000000001</v>
@@ -17833,7 +17827,7 @@
         <v>8</v>
       </c>
       <c r="H171" t="s">
-        <v>352</v>
+        <v>360</v>
       </c>
       <c r="I171">
         <v>0.11</v>
@@ -17862,7 +17856,7 @@
         <v>8</v>
       </c>
       <c r="H172" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I172">
         <v>0.04</v>
@@ -17891,7 +17885,7 @@
         <v>8</v>
       </c>
       <c r="H173" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I173">
         <v>0.04</v>
@@ -17949,7 +17943,7 @@
         <v>8</v>
       </c>
       <c r="H175" t="s">
-        <v>352</v>
+        <v>360</v>
       </c>
       <c r="I175">
         <v>0.11</v>
@@ -17978,7 +17972,7 @@
         <v>8</v>
       </c>
       <c r="H176" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I176">
         <v>0.04</v>
@@ -18007,7 +18001,7 @@
         <v>8</v>
       </c>
       <c r="H177" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I177">
         <v>0.04</v>
@@ -18036,7 +18030,7 @@
         <v>8</v>
       </c>
       <c r="H178" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I178">
         <v>0.04</v>
@@ -18065,7 +18059,7 @@
         <v>8</v>
       </c>
       <c r="H179" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I179">
         <v>0.04</v>
@@ -18123,7 +18117,7 @@
         <v>8</v>
       </c>
       <c r="H181" t="s">
-        <v>352</v>
+        <v>360</v>
       </c>
       <c r="I181">
         <v>0.11</v>
@@ -18152,7 +18146,7 @@
         <v>8</v>
       </c>
       <c r="H182" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I182">
         <v>0.04</v>
@@ -18181,7 +18175,7 @@
         <v>8</v>
       </c>
       <c r="H183" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I183">
         <v>0.04</v>
@@ -18239,7 +18233,7 @@
         <v>8</v>
       </c>
       <c r="H185" t="s">
-        <v>352</v>
+        <v>360</v>
       </c>
       <c r="I185">
         <v>0.11</v>
@@ -18268,7 +18262,7 @@
         <v>8</v>
       </c>
       <c r="H186" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I186">
         <v>0.04</v>
@@ -18297,7 +18291,7 @@
         <v>8</v>
       </c>
       <c r="H187" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I187">
         <v>0.04</v>
@@ -18326,7 +18320,7 @@
         <v>8</v>
       </c>
       <c r="H188" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I188">
         <v>0.04</v>
@@ -18355,7 +18349,7 @@
         <v>8</v>
       </c>
       <c r="H189" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I189">
         <v>0.04</v>
@@ -18413,7 +18407,7 @@
         <v>8</v>
       </c>
       <c r="H191" t="s">
-        <v>352</v>
+        <v>360</v>
       </c>
       <c r="I191">
         <v>0.11</v>
@@ -18442,7 +18436,7 @@
         <v>8</v>
       </c>
       <c r="H192" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I192">
         <v>0.04</v>
@@ -18471,7 +18465,7 @@
         <v>8</v>
       </c>
       <c r="H193" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I193">
         <v>0.04</v>
@@ -18529,7 +18523,7 @@
         <v>8</v>
       </c>
       <c r="H195" t="s">
-        <v>352</v>
+        <v>360</v>
       </c>
       <c r="I195">
         <v>0.11</v>
@@ -18558,7 +18552,7 @@
         <v>8</v>
       </c>
       <c r="H196" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I196">
         <v>0.04</v>
@@ -18587,7 +18581,7 @@
         <v>8</v>
       </c>
       <c r="H197" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I197">
         <v>0.04</v>
@@ -18616,7 +18610,7 @@
         <v>8</v>
       </c>
       <c r="H198" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I198">
         <v>0.04</v>
@@ -18645,7 +18639,7 @@
         <v>8</v>
       </c>
       <c r="H199" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I199">
         <v>0.04</v>
@@ -18703,7 +18697,7 @@
         <v>8</v>
       </c>
       <c r="H201" t="s">
-        <v>352</v>
+        <v>360</v>
       </c>
       <c r="I201">
         <v>0.11</v>
@@ -18732,7 +18726,7 @@
         <v>8</v>
       </c>
       <c r="H202" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I202">
         <v>0.04</v>
@@ -18761,7 +18755,7 @@
         <v>8</v>
       </c>
       <c r="H203" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I203">
         <v>0.04</v>
@@ -18819,7 +18813,7 @@
         <v>8</v>
       </c>
       <c r="H205" t="s">
-        <v>352</v>
+        <v>360</v>
       </c>
       <c r="I205">
         <v>0.11</v>
@@ -18848,7 +18842,7 @@
         <v>8</v>
       </c>
       <c r="H206" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I206">
         <v>0.04</v>
@@ -18877,7 +18871,7 @@
         <v>8</v>
       </c>
       <c r="H207" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I207">
         <v>0.04</v>
@@ -18906,7 +18900,7 @@
         <v>8</v>
       </c>
       <c r="H208" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I208">
         <v>0.04</v>
@@ -18935,7 +18929,7 @@
         <v>8</v>
       </c>
       <c r="H209" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I209">
         <v>0.04</v>
@@ -40089,8 +40083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3AB633E-9AEE-C044-8F09-ED4F88978E4B}">
   <dimension ref="A1:T19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15:G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -41234,7 +41228,7 @@
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B19" s="10" t="s">
         <v>71</v>
@@ -41252,7 +41246,7 @@
         <v>5340312414</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="H19" s="10">
         <v>425544224</v>
@@ -43224,15 +43218,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101003456B0730C78B347BD7589BC061D6E7A" ma:contentTypeVersion="12" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="63fa1c64418ad5e2c432e8a28af753ff">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7ab8c0d4-f18b-4fef-b649-c77d178c2495" xmlns:ns3="65efab6e-20b9-465e-9733-f0c2ab732419" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0084d3678d80c20d937c1596fa80271a" ns2:_="" ns3:_="">
     <xsd:import namespace="7ab8c0d4-f18b-4fef-b649-c77d178c2495"/>
@@ -43433,6 +43418,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE50E33B-922F-4D33-8831-2DF5BA7F11F6}">
   <ds:schemaRefs>
@@ -43451,14 +43445,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C685BDB-1785-4A39-A308-4CA166889A49}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52F4FD56-548C-4109-A8A9-EE1A91F5144E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -43477,6 +43463,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C685BDB-1785-4A39-A308-4CA166889A49}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{3c0bd4fe-1111-4d13-8e0c-7c33b9eb7581}" enabled="0" method="" siteId="{3c0bd4fe-1111-4d13-8e0c-7c33b9eb7581}" removed="1"/>

</xml_diff>

<commit_message>
se agrega el campo tipo_reasegurador requerido en el input
</commit_message>
<xml_diff>
--- a/prototipo_pcr/inputs/insumos.xlsx
+++ b/prototipo_pcr/inputs/insumos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10720"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://suramericana.sharepoint.com/sites/TraNIFF/Shared Documents/féniX/01 IFRS17/02 Entregables Procesos/05 Reservas/03 PCR CP/03 Tecnología/01 Prototipo/prototipo_pcr/inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://suramericana.sharepoint.com/sites/TraNIFF/Shared Documents/féniX/01 IFRS17/02 Entregables Procesos/05 Reservas/03 PCR CP/03 Tecnología/01 Prototipo/prototipo_pcr/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="13_ncr:1_{3EC42E67-7DA1-2342-97B9-902C865173C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1DE600D3-C7BD-3A47-AEE0-2C19F62B5897}"/>
+  <xr:revisionPtr revIDLastSave="56" documentId="13_ncr:1_{3EC42E67-7DA1-2342-97B9-902C865173C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F9D48AAA-EDA1-974C-ACE0-096C1979C70D}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17440" tabRatio="959" firstSheet="5" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" tabRatio="959" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="param_contabilidad" sheetId="6" r:id="rId1"/>
@@ -25,17 +25,16 @@
     <sheet name="seguimiento_rea_noprop" sheetId="19" r:id="rId10"/>
     <sheet name="map_bt" sheetId="20" r:id="rId11"/>
     <sheet name="tipo_seguro" sheetId="21" r:id="rId12"/>
-    <sheet name="homologacion" sheetId="26" r:id="rId13"/>
-    <sheet name="cuenta_cobrar_directo" sheetId="23" r:id="rId14"/>
-    <sheet name="cuenta_corriente_rea" sheetId="25" r:id="rId15"/>
+    <sheet name="cuenta_cobrar_directo" sheetId="23" r:id="rId13"/>
+    <sheet name="cuenta_corriente_rea" sheetId="25" r:id="rId14"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">comision_rea!$A$1:$U$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">comision_rea!$A$1:$V$9</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">map_bt!$A$1:$I$261</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">param_contabilidad!$A$1:$I$34</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">porc_descuento!$A$1:$K$17</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">produccion_directo!$A$1:$T$18</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">produccion_rea!$A$1:$X$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">produccion_rea!$A$1:$Y$10</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">tipo_seguro!$A$1:$C$61</definedName>
   </definedNames>
   <calcPr calcId="191028" iterate="1"/>
@@ -225,7 +224,7 @@
     <author>Priscilla Andrea Palacios Ruiz</author>
   </authors>
   <commentList>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{D9B7D91C-F7E6-7049-88D7-306E8176ED0D}">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{D9B7D91C-F7E6-7049-88D7-306E8176ED0D}">
       <text>
         <r>
           <rPr>
@@ -238,7 +237,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{1A1486ED-68D5-E44F-B774-F7614417A941}">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{1A1486ED-68D5-E44F-B774-F7614417A941}">
       <text>
         <r>
           <rPr>
@@ -252,7 +251,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{41D4138C-3A2B-764D-A151-DBB640FDE563}">
+    <comment ref="S1" authorId="0" shapeId="0" xr:uid="{41D4138C-3A2B-764D-A151-DBB640FDE563}">
       <text>
         <r>
           <rPr>
@@ -276,7 +275,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y1" authorId="0" shapeId="0" xr:uid="{615C3EE8-58D0-244B-A8A9-61E48533A4E2}">
+    <comment ref="Z1" authorId="0" shapeId="0" xr:uid="{615C3EE8-58D0-244B-A8A9-61E48533A4E2}">
       <text>
         <r>
           <rPr>
@@ -299,7 +298,7 @@
     <author>Priscilla Andrea Palacios Ruiz</author>
   </authors>
   <commentList>
-    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{16C83569-8856-3941-A083-484460776B6E}">
+    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{16C83569-8856-3941-A083-484460776B6E}">
       <text>
         <r>
           <rPr>
@@ -312,7 +311,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V1" authorId="0" shapeId="0" xr:uid="{E92E6D44-20CF-CB40-B52F-ADAAD919B98A}">
+    <comment ref="W1" authorId="0" shapeId="0" xr:uid="{E92E6D44-20CF-CB40-B52F-ADAAD919B98A}">
       <text>
         <r>
           <rPr>
@@ -346,7 +345,7 @@
     <author>Priscilla Andrea Palacios Ruiz</author>
   </authors>
   <commentList>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{1770F033-91D7-0047-BD15-7694292C6393}">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{1770F033-91D7-0047-BD15-7694292C6393}">
       <text>
         <r>
           <rPr>
@@ -359,7 +358,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{C8C07976-3C72-1D44-9A79-A6697E245BBC}">
+    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{C8C07976-3C72-1D44-9A79-A6697E245BBC}">
       <text>
         <r>
           <rPr>
@@ -461,7 +460,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7239" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7264" uniqueCount="365">
   <si>
     <t>tipo_insumo</t>
   </si>
@@ -1545,6 +1544,18 @@
   <si>
     <t>cuenta_pagar_costo_rea</t>
   </si>
+  <si>
+    <t>tipo_reasegurador</t>
+  </si>
+  <si>
+    <t>tipo_reaesegurador</t>
+  </si>
+  <si>
+    <t>INT</t>
+  </si>
+  <si>
+    <t>EXT</t>
+  </si>
 </sst>
 </file>
 
@@ -3881,7 +3892,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:A31"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4732,7 +4743,7 @@
   </sheetPr>
   <dimension ref="A1:I261"/>
   <sheetViews>
-    <sheetView topLeftCell="A141" zoomScale="112" zoomScaleNormal="73" workbookViewId="0">
+    <sheetView topLeftCell="A138" zoomScale="112" zoomScaleNormal="73" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -12239,25 +12250,13 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{889C9B21-92BF-4D6C-BD65-AE8DE54623A5}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F7F059E-3482-9948-A0EE-3B780BE80211}">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
@@ -12391,7 +12390,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C59D3D0B-BDA7-C849-9A02-F348974FBECC}">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
@@ -39307,7 +39306,7 @@
   <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="A2:K18"/>
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -41175,37 +41174,37 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4F93C6E-21BF-4220-AF0D-6D307F3158B8}">
-  <dimension ref="A1:Z10"/>
+  <dimension ref="A1:AA10"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
-      <selection activeCell="Z1" sqref="Z1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="25.1640625" customWidth="1"/>
-    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.83203125" style="25" customWidth="1"/>
-    <col min="9" max="10" width="24.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.5" customWidth="1"/>
-    <col min="20" max="20" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="26.5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="32.5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="30" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.5" style="13"/>
+    <col min="2" max="7" width="25.1640625" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.83203125" style="25" customWidth="1"/>
+    <col min="10" max="11" width="24.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.5" customWidth="1"/>
+    <col min="21" max="21" width="29.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="26.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="32.5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="30" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.5" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>109</v>
       </c>
@@ -41222,70 +41221,73 @@
         <v>137</v>
       </c>
       <c r="F1" s="48" t="s">
+        <v>361</v>
+      </c>
+      <c r="G1" s="48" t="s">
         <v>138</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="I1" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="48" t="s">
+      <c r="J1" s="48" t="s">
         <v>139</v>
       </c>
-      <c r="J1" s="48" t="s">
+      <c r="K1" s="48" t="s">
         <v>140</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="Y1" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="Z1" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="Z1" s="49" t="s">
+      <c r="AA1" s="49" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>130</v>
       </c>
@@ -41301,71 +41303,74 @@
       <c r="E2">
         <v>2374188</v>
       </c>
-      <c r="F2">
+      <c r="F2" t="s">
+        <v>363</v>
+      </c>
+      <c r="G2">
         <v>0.4</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>124324091</v>
       </c>
-      <c r="H2" s="25">
+      <c r="I2" s="25">
         <v>293842989501</v>
       </c>
-      <c r="I2" s="14">
+      <c r="J2" s="14">
         <v>45108</v>
       </c>
-      <c r="J2" s="14">
+      <c r="K2" s="14">
         <v>45473</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>101</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>124324511</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="N2" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>81</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>119</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>120</v>
       </c>
-      <c r="R2" t="s">
-        <v>91</v>
-      </c>
-      <c r="S2" s="4">
+      <c r="S2" t="s">
+        <v>91</v>
+      </c>
+      <c r="T2" s="4">
         <v>45292</v>
       </c>
-      <c r="T2" s="4">
+      <c r="U2" s="4">
         <v>45306</v>
       </c>
-      <c r="U2" s="4">
+      <c r="V2" s="4">
         <v>45672</v>
       </c>
-      <c r="V2" s="4">
+      <c r="W2" s="4">
         <v>45306</v>
       </c>
-      <c r="W2" s="4">
+      <c r="X2" s="4">
         <v>45672</v>
       </c>
-      <c r="X2" s="2">
+      <c r="Y2" s="2">
         <v>1200</v>
       </c>
-      <c r="Y2">
+      <c r="Z2">
         <v>600</v>
       </c>
-      <c r="Z2" s="13">
+      <c r="AA2" s="13">
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>130</v>
       </c>
@@ -41381,71 +41386,74 @@
       <c r="E3">
         <v>6987458</v>
       </c>
-      <c r="F3">
+      <c r="F3" t="s">
+        <v>363</v>
+      </c>
+      <c r="G3">
         <v>0.3</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>124324091</v>
       </c>
-      <c r="H3" s="25">
+      <c r="I3" s="25">
         <v>293842989501</v>
       </c>
-      <c r="I3" s="14">
+      <c r="J3" s="14">
         <v>45108</v>
       </c>
-      <c r="J3" s="14">
+      <c r="K3" s="14">
         <v>45473</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>101</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>124324511</v>
       </c>
-      <c r="M3" s="7" t="s">
+      <c r="N3" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="O3" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>81</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>119</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>120</v>
       </c>
-      <c r="R3" t="s">
-        <v>91</v>
-      </c>
-      <c r="S3" s="4">
+      <c r="S3" t="s">
+        <v>91</v>
+      </c>
+      <c r="T3" s="4">
         <v>45292</v>
       </c>
-      <c r="T3" s="4">
+      <c r="U3" s="4">
         <v>45306</v>
       </c>
-      <c r="U3" s="4">
+      <c r="V3" s="4">
         <v>45672</v>
       </c>
-      <c r="V3" s="4">
+      <c r="W3" s="4">
         <v>45306</v>
       </c>
-      <c r="W3" s="4">
+      <c r="X3" s="4">
         <v>45672</v>
       </c>
-      <c r="X3" s="2">
+      <c r="Y3" s="2">
         <v>1200</v>
       </c>
-      <c r="Y3">
+      <c r="Z3">
         <v>600</v>
       </c>
-      <c r="Z3" s="13">
+      <c r="AA3" s="13">
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>130</v>
       </c>
@@ -41461,71 +41469,74 @@
       <c r="E4">
         <v>3693358</v>
       </c>
-      <c r="F4">
+      <c r="F4" t="s">
+        <v>364</v>
+      </c>
+      <c r="G4">
         <v>0.3</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>124324091</v>
       </c>
-      <c r="H4" s="25">
+      <c r="I4" s="25">
         <v>293842989501</v>
       </c>
-      <c r="I4" s="14">
+      <c r="J4" s="14">
         <v>45108</v>
       </c>
-      <c r="J4" s="14">
+      <c r="K4" s="14">
         <v>45473</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>101</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>124324511</v>
       </c>
-      <c r="M4" s="7" t="s">
+      <c r="N4" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="O4" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>81</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>119</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>120</v>
       </c>
-      <c r="R4" t="s">
-        <v>91</v>
-      </c>
-      <c r="S4" s="4">
+      <c r="S4" t="s">
+        <v>91</v>
+      </c>
+      <c r="T4" s="4">
         <v>45292</v>
       </c>
-      <c r="T4" s="4">
+      <c r="U4" s="4">
         <v>45306</v>
       </c>
-      <c r="U4" s="4">
+      <c r="V4" s="4">
         <v>45672</v>
       </c>
-      <c r="V4" s="4">
+      <c r="W4" s="4">
         <v>45306</v>
       </c>
-      <c r="W4" s="4">
+      <c r="X4" s="4">
         <v>45672</v>
       </c>
-      <c r="X4" s="2">
+      <c r="Y4" s="2">
         <v>1200</v>
       </c>
-      <c r="Y4">
+      <c r="Z4">
         <v>600</v>
       </c>
-      <c r="Z4" s="13">
+      <c r="AA4" s="13">
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>129</v>
       </c>
@@ -41541,71 +41552,74 @@
       <c r="E5">
         <v>2374188</v>
       </c>
-      <c r="F5">
+      <c r="F5" t="s">
+        <v>363</v>
+      </c>
+      <c r="G5">
         <v>0.4</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>124324092</v>
       </c>
-      <c r="H5" s="25">
+      <c r="I5" s="25">
         <v>293843030701</v>
       </c>
-      <c r="I5" s="14">
+      <c r="J5" s="14">
         <v>45108</v>
       </c>
-      <c r="J5" s="14">
+      <c r="K5" s="14">
         <v>45473</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>101</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>124324512</v>
       </c>
-      <c r="M5" s="7" t="s">
+      <c r="N5" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="N5" s="3" t="s">
+      <c r="O5" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>81</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>119</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>120</v>
       </c>
-      <c r="R5" t="s">
-        <v>92</v>
-      </c>
-      <c r="S5" s="4">
+      <c r="S5" t="s">
+        <v>92</v>
+      </c>
+      <c r="T5" s="4">
         <v>45245</v>
       </c>
-      <c r="T5" s="4">
+      <c r="U5" s="4">
         <v>45306</v>
       </c>
-      <c r="U5" s="4">
+      <c r="V5" s="4">
         <v>45672</v>
       </c>
-      <c r="V5" s="4">
+      <c r="W5" s="4">
         <v>45306</v>
       </c>
-      <c r="W5" s="4">
+      <c r="X5" s="4">
         <v>45672</v>
       </c>
-      <c r="X5" s="2">
+      <c r="Y5" s="2">
         <v>1200</v>
       </c>
-      <c r="Y5">
+      <c r="Z5">
         <v>600</v>
       </c>
-      <c r="Z5" s="13">
+      <c r="AA5" s="13">
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>129</v>
       </c>
@@ -41621,71 +41635,74 @@
       <c r="E6">
         <v>6987458</v>
       </c>
-      <c r="F6">
+      <c r="F6" t="s">
+        <v>363</v>
+      </c>
+      <c r="G6">
         <v>0.3</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>124324092</v>
       </c>
-      <c r="H6" s="25">
+      <c r="I6" s="25">
         <v>293843030701</v>
       </c>
-      <c r="I6" s="14">
+      <c r="J6" s="14">
         <v>45108</v>
       </c>
-      <c r="J6" s="14">
+      <c r="K6" s="14">
         <v>45473</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>101</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>124324512</v>
       </c>
-      <c r="M6" s="7" t="s">
+      <c r="N6" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="N6" s="3" t="s">
+      <c r="O6" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>81</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>119</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>120</v>
       </c>
-      <c r="R6" t="s">
-        <v>92</v>
-      </c>
-      <c r="S6" s="4">
+      <c r="S6" t="s">
+        <v>92</v>
+      </c>
+      <c r="T6" s="4">
         <v>45245</v>
       </c>
-      <c r="T6" s="4">
+      <c r="U6" s="4">
         <v>45306</v>
       </c>
-      <c r="U6" s="4">
+      <c r="V6" s="4">
         <v>45672</v>
       </c>
-      <c r="V6" s="4">
+      <c r="W6" s="4">
         <v>45306</v>
       </c>
-      <c r="W6" s="4">
+      <c r="X6" s="4">
         <v>45672</v>
       </c>
-      <c r="X6" s="2">
+      <c r="Y6" s="2">
         <v>1200</v>
       </c>
-      <c r="Y6">
+      <c r="Z6">
         <v>600</v>
       </c>
-      <c r="Z6" s="13">
+      <c r="AA6" s="13">
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>129</v>
       </c>
@@ -41701,71 +41718,74 @@
       <c r="E7">
         <v>3693358</v>
       </c>
-      <c r="F7">
+      <c r="F7" t="s">
+        <v>364</v>
+      </c>
+      <c r="G7">
         <v>0.3</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>124324092</v>
       </c>
-      <c r="H7" s="25">
+      <c r="I7" s="25">
         <v>293843030701</v>
       </c>
-      <c r="I7" s="14">
+      <c r="J7" s="14">
         <v>45108</v>
       </c>
-      <c r="J7" s="14">
+      <c r="K7" s="14">
         <v>45473</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>101</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>124324512</v>
       </c>
-      <c r="M7" s="7" t="s">
+      <c r="N7" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="N7" s="3" t="s">
+      <c r="O7" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>81</v>
       </c>
-      <c r="P7" s="5" t="s">
+      <c r="Q7" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="R7" t="s">
         <v>120</v>
       </c>
-      <c r="R7" t="s">
-        <v>92</v>
-      </c>
-      <c r="S7" s="4">
+      <c r="S7" t="s">
+        <v>92</v>
+      </c>
+      <c r="T7" s="4">
         <v>45245</v>
       </c>
-      <c r="T7" s="4">
+      <c r="U7" s="4">
         <v>45306</v>
       </c>
-      <c r="U7" s="4">
+      <c r="V7" s="4">
         <v>45672</v>
       </c>
-      <c r="V7" s="4">
+      <c r="W7" s="4">
         <v>45306</v>
       </c>
-      <c r="W7" s="4">
+      <c r="X7" s="4">
         <v>45672</v>
       </c>
-      <c r="X7" s="2">
+      <c r="Y7" s="2">
         <v>1200</v>
       </c>
-      <c r="Y7">
+      <c r="Z7">
         <v>600</v>
       </c>
-      <c r="Z7" s="13">
+      <c r="AA7" s="13">
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>133</v>
       </c>
@@ -41781,71 +41801,74 @@
       <c r="E8">
         <v>3339928</v>
       </c>
-      <c r="F8">
+      <c r="F8" t="s">
+        <v>364</v>
+      </c>
+      <c r="G8">
         <v>1</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>634535346</v>
       </c>
-      <c r="H8" s="25">
+      <c r="I8" s="25">
         <v>293843113101</v>
       </c>
-      <c r="I8" s="14">
+      <c r="J8" s="14">
         <v>45108</v>
       </c>
-      <c r="J8" s="14">
+      <c r="K8" s="14">
         <v>45473</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>107</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <v>634535766</v>
       </c>
-      <c r="M8" s="7" t="s">
+      <c r="N8" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="N8" s="3" t="s">
+      <c r="O8" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="O8" t="s">
+      <c r="P8" t="s">
         <v>77</v>
       </c>
-      <c r="P8" t="s">
+      <c r="Q8" t="s">
         <v>119</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="R8" t="s">
         <v>120</v>
       </c>
-      <c r="R8" t="s">
-        <v>92</v>
-      </c>
-      <c r="S8" s="4">
+      <c r="S8" t="s">
+        <v>92</v>
+      </c>
+      <c r="T8" s="4">
         <v>45275</v>
       </c>
-      <c r="T8" s="4">
+      <c r="U8" s="4">
         <v>45306</v>
       </c>
-      <c r="U8" s="4">
+      <c r="V8" s="4">
         <v>45337</v>
       </c>
-      <c r="V8" s="4">
+      <c r="W8" s="4">
         <v>45306</v>
       </c>
-      <c r="W8" s="4">
+      <c r="X8" s="4">
         <v>45337</v>
       </c>
-      <c r="X8" s="2">
+      <c r="Y8" s="2">
         <v>100</v>
       </c>
-      <c r="Y8">
+      <c r="Z8">
         <v>30</v>
       </c>
-      <c r="Z8" s="13">
+      <c r="AA8" s="13">
         <v>0.3</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>124</v>
       </c>
@@ -41861,71 +41884,74 @@
       <c r="E9">
         <v>3693358</v>
       </c>
-      <c r="F9">
+      <c r="F9" t="s">
+        <v>364</v>
+      </c>
+      <c r="G9">
         <v>0.5</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>345675387</v>
       </c>
-      <c r="H9" s="25">
+      <c r="I9" s="25">
         <v>293843154301</v>
       </c>
-      <c r="I9" s="14">
+      <c r="J9" s="14">
         <v>45292</v>
       </c>
-      <c r="J9" s="14">
+      <c r="K9" s="14">
         <v>45657</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>104</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>345675807</v>
       </c>
-      <c r="M9" s="7" t="s">
+      <c r="N9" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="N9" s="3" t="s">
+      <c r="O9" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="O9" t="s">
+      <c r="P9" t="s">
         <v>77</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9" t="s">
         <v>122</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="R9" t="s">
         <v>120</v>
       </c>
-      <c r="R9" t="s">
-        <v>92</v>
-      </c>
-      <c r="S9" s="4">
+      <c r="S9" t="s">
+        <v>92</v>
+      </c>
+      <c r="T9" s="4">
         <v>45342</v>
       </c>
-      <c r="T9" s="4">
+      <c r="U9" s="4">
         <v>45306</v>
       </c>
-      <c r="U9" s="4">
+      <c r="V9" s="4">
         <v>45337</v>
       </c>
-      <c r="V9" s="4">
+      <c r="W9" s="4">
         <v>45306</v>
       </c>
-      <c r="W9" s="4">
+      <c r="X9" s="4">
         <v>45337</v>
       </c>
-      <c r="X9" s="2">
+      <c r="Y9" s="2">
         <v>100</v>
       </c>
-      <c r="Y9">
+      <c r="Z9">
         <v>60</v>
       </c>
-      <c r="Z9" s="13">
+      <c r="AA9" s="13">
         <v>0.6</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>124</v>
       </c>
@@ -41941,67 +41967,70 @@
       <c r="E10">
         <v>2374188</v>
       </c>
-      <c r="F10">
+      <c r="F10" t="s">
+        <v>363</v>
+      </c>
+      <c r="G10">
         <v>0.5</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>345675387</v>
       </c>
-      <c r="H10" s="25">
+      <c r="I10" s="25">
         <v>293843154301</v>
       </c>
-      <c r="I10" s="14">
+      <c r="J10" s="14">
         <v>45292</v>
       </c>
-      <c r="J10" s="14">
+      <c r="K10" s="14">
         <v>45657</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>104</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>345675807</v>
       </c>
-      <c r="M10" s="7" t="s">
+      <c r="N10" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="N10" s="3" t="s">
+      <c r="O10" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="O10" t="s">
+      <c r="P10" t="s">
         <v>77</v>
       </c>
-      <c r="P10" t="s">
+      <c r="Q10" t="s">
         <v>122</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="R10" t="s">
         <v>120</v>
       </c>
-      <c r="R10" t="s">
-        <v>92</v>
-      </c>
-      <c r="S10" s="4">
+      <c r="S10" t="s">
+        <v>92</v>
+      </c>
+      <c r="T10" s="4">
         <v>45342</v>
       </c>
-      <c r="T10" s="4">
+      <c r="U10" s="4">
         <v>45306</v>
       </c>
-      <c r="U10" s="4">
+      <c r="V10" s="4">
         <v>45337</v>
       </c>
-      <c r="V10" s="4">
+      <c r="W10" s="4">
         <v>45306</v>
       </c>
-      <c r="W10" s="4">
+      <c r="X10" s="4">
         <v>45337</v>
       </c>
-      <c r="X10" s="2">
+      <c r="Y10" s="2">
         <v>100</v>
       </c>
-      <c r="Y10">
+      <c r="Z10">
         <v>60</v>
       </c>
-      <c r="Z10" s="13">
+      <c r="AA10" s="13">
         <v>0.6</v>
       </c>
     </row>
@@ -42015,34 +42044,34 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED59B340-08CC-1E4C-83CE-42156F1868E1}">
-  <dimension ref="A1:W9"/>
+  <dimension ref="A1:X9"/>
   <sheetViews>
     <sheetView zoomScale="109" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="F2" sqref="F2:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="25.1640625" customWidth="1"/>
-    <col min="7" max="7" width="17.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.5" customWidth="1"/>
-    <col min="18" max="18" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="26.5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="26.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="25.1640625" customWidth="1"/>
+    <col min="8" max="8" width="17.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.5" customWidth="1"/>
+    <col min="19" max="19" width="29.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="26.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="29.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="26.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>109</v>
       </c>
@@ -42059,61 +42088,64 @@
         <v>137</v>
       </c>
       <c r="F1" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>130</v>
       </c>
@@ -42129,62 +42161,65 @@
       <c r="E2">
         <v>2374188</v>
       </c>
-      <c r="F2">
+      <c r="F2" t="s">
+        <v>363</v>
+      </c>
+      <c r="G2">
         <v>0.4</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>6720148806</v>
       </c>
-      <c r="H2" s="14">
+      <c r="I2" s="14">
         <v>45108</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="J2" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>124324091</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>101</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>124324511</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>81</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>119</v>
       </c>
-      <c r="P2" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q2" s="4">
+      <c r="Q2" t="s">
+        <v>91</v>
+      </c>
+      <c r="R2" s="4">
         <v>45292</v>
       </c>
-      <c r="R2" s="4">
+      <c r="S2" s="4">
         <v>45306</v>
       </c>
-      <c r="S2" s="4">
+      <c r="T2" s="4">
         <v>45672</v>
       </c>
-      <c r="T2" s="4">
+      <c r="U2" s="4">
         <v>45306</v>
       </c>
-      <c r="U2" s="4">
+      <c r="V2" s="4">
         <v>45672</v>
       </c>
-      <c r="V2">
+      <c r="W2">
         <v>120</v>
       </c>
-      <c r="W2">
+      <c r="X2">
         <v>0.2</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>130</v>
       </c>
@@ -42200,62 +42235,65 @@
       <c r="E3">
         <v>6987458</v>
       </c>
-      <c r="F3">
+      <c r="F3" t="s">
+        <v>363</v>
+      </c>
+      <c r="G3">
         <v>0.3</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>3517986098</v>
       </c>
-      <c r="H3" s="14">
+      <c r="I3" s="14">
         <v>45108</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="J3" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>124324091</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>101</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>124324511</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>81</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>119</v>
       </c>
-      <c r="P3" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q3" s="4">
+      <c r="Q3" t="s">
+        <v>91</v>
+      </c>
+      <c r="R3" s="4">
         <v>45292</v>
       </c>
-      <c r="R3" s="4">
+      <c r="S3" s="4">
         <v>45306</v>
       </c>
-      <c r="S3" s="4">
+      <c r="T3" s="4">
         <v>45672</v>
       </c>
-      <c r="T3" s="4">
+      <c r="U3" s="4">
         <v>45306</v>
       </c>
-      <c r="U3" s="4">
+      <c r="V3" s="4">
         <v>45672</v>
       </c>
-      <c r="V3">
+      <c r="W3">
         <v>120</v>
       </c>
-      <c r="W3">
+      <c r="X3">
         <v>0.2</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>130</v>
       </c>
@@ -42271,62 +42309,65 @@
       <c r="E4">
         <v>3693358</v>
       </c>
-      <c r="F4">
+      <c r="F4" t="s">
+        <v>364</v>
+      </c>
+      <c r="G4">
         <v>0.3</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>1944219246</v>
       </c>
-      <c r="H4" s="14">
+      <c r="I4" s="14">
         <v>45108</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="J4" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>124324091</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>101</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>124324511</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>81</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>119</v>
       </c>
-      <c r="P4" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q4" s="4">
+      <c r="Q4" t="s">
+        <v>91</v>
+      </c>
+      <c r="R4" s="4">
         <v>45292</v>
       </c>
-      <c r="R4" s="4">
+      <c r="S4" s="4">
         <v>45306</v>
       </c>
-      <c r="S4" s="4">
+      <c r="T4" s="4">
         <v>45672</v>
       </c>
-      <c r="T4" s="4">
+      <c r="U4" s="4">
         <v>45306</v>
       </c>
-      <c r="U4" s="4">
+      <c r="V4" s="4">
         <v>45672</v>
       </c>
-      <c r="V4">
+      <c r="W4">
         <v>120</v>
       </c>
-      <c r="W4">
+      <c r="X4">
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>129</v>
       </c>
@@ -42342,62 +42383,65 @@
       <c r="E5">
         <v>2374188</v>
       </c>
-      <c r="F5">
+      <c r="F5" t="s">
+        <v>363</v>
+      </c>
+      <c r="G5">
         <v>0.4</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>5249897308</v>
       </c>
-      <c r="H5" s="14">
+      <c r="I5" s="14">
         <v>45108</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="J5" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="K5" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>124324092</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>101</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>124324512</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>81</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>119</v>
       </c>
-      <c r="P5" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q5" s="4">
+      <c r="Q5" t="s">
+        <v>92</v>
+      </c>
+      <c r="R5" s="4">
         <v>45245</v>
       </c>
-      <c r="R5" s="4">
+      <c r="S5" s="4">
         <v>45306</v>
       </c>
-      <c r="S5" s="4">
+      <c r="T5" s="4">
         <v>45672</v>
       </c>
-      <c r="T5" s="4">
+      <c r="U5" s="4">
         <v>45306</v>
       </c>
-      <c r="U5" s="4">
+      <c r="V5" s="4">
         <v>45672</v>
       </c>
-      <c r="V5">
+      <c r="W5">
         <v>120</v>
       </c>
-      <c r="W5">
+      <c r="X5">
         <v>0.2</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>129</v>
       </c>
@@ -42413,62 +42457,65 @@
       <c r="E6">
         <v>6987458</v>
       </c>
-      <c r="F6">
+      <c r="F6" t="s">
+        <v>363</v>
+      </c>
+      <c r="G6">
         <v>0.3</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>4579088313</v>
       </c>
-      <c r="H6" s="14">
+      <c r="I6" s="14">
         <v>45108</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="J6" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="K6" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>124324092</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>101</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>124324512</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>81</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>119</v>
       </c>
-      <c r="P6" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q6" s="4">
+      <c r="Q6" t="s">
+        <v>92</v>
+      </c>
+      <c r="R6" s="4">
         <v>45245</v>
       </c>
-      <c r="R6" s="4">
+      <c r="S6" s="4">
         <v>45306</v>
       </c>
-      <c r="S6" s="4">
+      <c r="T6" s="4">
         <v>45672</v>
       </c>
-      <c r="T6" s="4">
+      <c r="U6" s="4">
         <v>45306</v>
       </c>
-      <c r="U6" s="4">
+      <c r="V6" s="4">
         <v>45672</v>
       </c>
-      <c r="V6">
+      <c r="W6">
         <v>120</v>
       </c>
-      <c r="W6">
+      <c r="X6">
         <v>0.2</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>129</v>
       </c>
@@ -42484,62 +42531,65 @@
       <c r="E7">
         <v>3693358</v>
       </c>
-      <c r="F7">
+      <c r="F7" t="s">
+        <v>364</v>
+      </c>
+      <c r="G7">
         <v>0.3</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>7859725531</v>
       </c>
-      <c r="H7" s="14">
+      <c r="I7" s="14">
         <v>45108</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="J7" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="K7" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>124324092</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>101</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>124324512</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>81</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>119</v>
       </c>
-      <c r="P7" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q7" s="4">
+      <c r="Q7" t="s">
+        <v>92</v>
+      </c>
+      <c r="R7" s="4">
         <v>45245</v>
       </c>
-      <c r="R7" s="4">
+      <c r="S7" s="4">
         <v>45306</v>
       </c>
-      <c r="S7" s="4">
+      <c r="T7" s="4">
         <v>45672</v>
       </c>
-      <c r="T7" s="4">
+      <c r="U7" s="4">
         <v>45306</v>
       </c>
-      <c r="U7" s="4">
+      <c r="V7" s="4">
         <v>45672</v>
       </c>
-      <c r="V7">
+      <c r="W7">
         <v>120</v>
       </c>
-      <c r="W7">
+      <c r="X7">
         <v>0.2</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>124</v>
       </c>
@@ -42555,62 +42605,65 @@
       <c r="E8">
         <v>3693358</v>
       </c>
-      <c r="F8">
+      <c r="F8" t="s">
+        <v>364</v>
+      </c>
+      <c r="G8">
         <v>0.5</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>5260869017</v>
       </c>
-      <c r="H8" s="14">
+      <c r="I8" s="14">
         <v>45292</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="J8" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="K8" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>345675387</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>104</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <v>345675807</v>
       </c>
-      <c r="N8" t="s">
+      <c r="O8" t="s">
         <v>77</v>
       </c>
-      <c r="O8" t="s">
+      <c r="P8" t="s">
         <v>122</v>
       </c>
-      <c r="P8" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q8" s="4">
+      <c r="Q8" t="s">
+        <v>92</v>
+      </c>
+      <c r="R8" s="4">
         <v>45342</v>
       </c>
-      <c r="R8" s="4">
+      <c r="S8" s="4">
         <v>45306</v>
       </c>
-      <c r="S8" s="4">
+      <c r="T8" s="4">
         <v>45337</v>
       </c>
-      <c r="T8" s="4">
+      <c r="U8" s="4">
         <v>45306</v>
       </c>
-      <c r="U8" s="4">
+      <c r="V8" s="4">
         <v>45337</v>
       </c>
-      <c r="V8">
+      <c r="W8">
         <v>6</v>
       </c>
-      <c r="W8">
+      <c r="X8">
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>124</v>
       </c>
@@ -42626,58 +42679,61 @@
       <c r="E9">
         <v>2374188</v>
       </c>
-      <c r="F9">
+      <c r="F9" t="s">
+        <v>363</v>
+      </c>
+      <c r="G9">
         <v>0.5</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>1292794322</v>
       </c>
-      <c r="H9" s="14">
+      <c r="I9" s="14">
         <v>45292</v>
       </c>
-      <c r="I9" s="7" t="s">
+      <c r="J9" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="J9" s="3" t="s">
+      <c r="K9" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>345675387</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>104</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>345675807</v>
       </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
         <v>77</v>
       </c>
-      <c r="O9" t="s">
+      <c r="P9" t="s">
         <v>122</v>
       </c>
-      <c r="P9" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q9" s="4">
+      <c r="Q9" t="s">
+        <v>92</v>
+      </c>
+      <c r="R9" s="4">
         <v>45342</v>
       </c>
-      <c r="R9" s="4">
+      <c r="S9" s="4">
         <v>45306</v>
       </c>
-      <c r="S9" s="4">
+      <c r="T9" s="4">
         <v>45337</v>
       </c>
-      <c r="T9" s="4">
+      <c r="U9" s="4">
         <v>45306</v>
       </c>
-      <c r="U9" s="4">
+      <c r="V9" s="4">
         <v>45337</v>
       </c>
-      <c r="V9">
+      <c r="W9">
         <v>6</v>
       </c>
-      <c r="W9">
+      <c r="X9">
         <v>0.1</v>
       </c>
     </row>
@@ -42690,10 +42746,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8B056C4-8D76-6947-BFDD-DD6636C4305C}">
-  <dimension ref="A1:S6"/>
+  <dimension ref="A1:T6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="G2" sqref="G2:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -42702,17 +42758,17 @@
     <col min="3" max="3" width="25.1640625" customWidth="1"/>
     <col min="4" max="4" width="16" style="14" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16" style="14" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16" style="14" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16" style="14" customWidth="1"/>
-    <col min="16" max="17" width="18.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.83203125" style="13" customWidth="1"/>
-    <col min="19" max="19" width="17.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16" style="14" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16" style="14" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16" style="14" customWidth="1"/>
+    <col min="17" max="18" width="18.83203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.83203125" style="13" customWidth="1"/>
+    <col min="20" max="20" width="17.5" style="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -42732,46 +42788,49 @@
         <v>137</v>
       </c>
       <c r="G1" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="M1" s="32" t="s">
+      <c r="N1" s="32" t="s">
         <v>115</v>
       </c>
-      <c r="N1" s="32" t="s">
+      <c r="O1" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="O1" s="15" t="s">
+      <c r="P1" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="P1" s="12" t="s">
+      <c r="Q1" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="Q1" s="12" t="s">
+      <c r="R1" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="R1" s="12" t="s">
+      <c r="S1" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="S1" s="16" t="s">
+      <c r="T1" s="16" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -42791,46 +42850,49 @@
       <c r="F2">
         <v>507351248</v>
       </c>
-      <c r="G2">
+      <c r="G2" t="s">
+        <v>363</v>
+      </c>
+      <c r="H2">
         <v>0.2</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="I2" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="J2" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="K2" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="K2" s="14">
+      <c r="L2" s="14">
         <v>45474</v>
       </c>
-      <c r="L2" s="14">
-        <f>+EDATE(K2,12)-1</f>
+      <c r="M2" s="14">
+        <f>+EDATE(L2,12)-1</f>
         <v>45838</v>
       </c>
-      <c r="M2" s="42">
+      <c r="N2" s="42">
         <v>45474</v>
       </c>
-      <c r="N2" s="42">
-        <f>+EDATE(M2,12)-1</f>
+      <c r="O2" s="42">
+        <f>+EDATE(N2,12)-1</f>
         <v>45838</v>
       </c>
-      <c r="P2" s="13">
+      <c r="Q2" s="13">
         <v>47628239</v>
       </c>
-      <c r="Q2" s="18">
+      <c r="R2" s="18">
         <v>45474</v>
       </c>
-      <c r="R2" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="S2" s="17">
+      <c r="S2" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="T2" s="17">
         <v>7000000000</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -42850,46 +42912,49 @@
       <c r="F3">
         <v>368484453</v>
       </c>
-      <c r="G3">
+      <c r="G3" t="s">
+        <v>364</v>
+      </c>
+      <c r="H3">
         <v>0.8</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="I3" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="J3" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="K3" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="K3" s="14">
+      <c r="L3" s="14">
         <v>45474</v>
       </c>
-      <c r="L3" s="14">
-        <f>+EDATE(K3,12)-1</f>
+      <c r="M3" s="14">
+        <f>+EDATE(L3,12)-1</f>
         <v>45838</v>
       </c>
-      <c r="M3" s="42">
+      <c r="N3" s="42">
         <v>45474</v>
       </c>
-      <c r="N3" s="42">
-        <f>+EDATE(M3,12)-1</f>
+      <c r="O3" s="42">
+        <f>+EDATE(N3,12)-1</f>
         <v>45838</v>
       </c>
-      <c r="P3" s="13">
+      <c r="Q3" s="13">
         <v>47628239</v>
       </c>
-      <c r="Q3" s="18">
+      <c r="R3" s="18">
         <v>45474</v>
       </c>
-      <c r="R3" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="S3" s="17">
+      <c r="S3" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="T3" s="17">
         <v>7000000000</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -42909,46 +42974,49 @@
       <c r="F4">
         <v>446526767</v>
       </c>
-      <c r="G4">
+      <c r="G4" t="s">
+        <v>363</v>
+      </c>
+      <c r="H4">
         <v>1</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="I4" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="J4" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="K4" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="K4" s="14">
+      <c r="L4" s="14">
         <v>45474</v>
       </c>
-      <c r="L4" s="14">
-        <f t="shared" ref="L4:L6" si="0">+EDATE(K4,12)-1</f>
+      <c r="M4" s="14">
+        <f t="shared" ref="M4:M6" si="0">+EDATE(L4,12)-1</f>
         <v>45838</v>
       </c>
-      <c r="M4" s="42">
+      <c r="N4" s="42">
         <v>45474</v>
       </c>
-      <c r="N4" s="42">
-        <f t="shared" ref="N4:N6" si="1">+EDATE(M4,12)-1</f>
+      <c r="O4" s="42">
+        <f t="shared" ref="O4:O6" si="1">+EDATE(N4,12)-1</f>
         <v>45838</v>
       </c>
-      <c r="P4" s="13">
+      <c r="Q4" s="13">
         <v>71800418</v>
       </c>
-      <c r="Q4" s="18">
+      <c r="R4" s="18">
         <v>45474</v>
       </c>
-      <c r="R4" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="S4" s="17">
+      <c r="S4" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="T4" s="17">
         <v>5350000000</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -42968,46 +43036,49 @@
       <c r="F5">
         <v>325775298</v>
       </c>
-      <c r="G5">
+      <c r="G5" t="s">
+        <v>363</v>
+      </c>
+      <c r="H5">
         <v>1</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="I5" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="J5" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="K5" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="K5" s="14">
+      <c r="L5" s="14">
         <v>45658</v>
       </c>
-      <c r="L5" s="14">
+      <c r="M5" s="14">
         <f t="shared" si="0"/>
         <v>46022</v>
       </c>
-      <c r="M5" s="42">
+      <c r="N5" s="42">
         <v>45658</v>
       </c>
-      <c r="N5" s="42">
+      <c r="O5" s="42">
         <f t="shared" si="1"/>
         <v>46022</v>
       </c>
-      <c r="P5" s="13">
+      <c r="Q5" s="13">
         <v>45927212</v>
       </c>
-      <c r="Q5" s="18">
+      <c r="R5" s="18">
         <v>45658</v>
       </c>
-      <c r="R5" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="S5" s="17">
+      <c r="S5" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="T5" s="17">
         <v>134000000</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -43027,45 +43098,48 @@
       <c r="F6">
         <v>360681631</v>
       </c>
-      <c r="G6">
+      <c r="G6" t="s">
+        <v>363</v>
+      </c>
+      <c r="H6">
         <v>1</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="I6" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="J6" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="K6" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="K6" s="14">
+      <c r="L6" s="14">
         <v>45658</v>
       </c>
-      <c r="L6" s="14">
+      <c r="M6" s="14">
         <f t="shared" si="0"/>
         <v>46022</v>
       </c>
-      <c r="M6" s="42">
+      <c r="N6" s="42">
         <v>45658</v>
       </c>
-      <c r="N6" s="42">
+      <c r="O6" s="42">
         <f t="shared" si="1"/>
         <v>46022</v>
       </c>
-      <c r="O6" s="14">
+      <c r="P6" s="14">
         <v>45811</v>
       </c>
-      <c r="P6" s="13">
+      <c r="Q6" s="13">
         <v>45927219</v>
       </c>
-      <c r="Q6" s="18">
+      <c r="R6" s="18">
         <v>45823</v>
       </c>
-      <c r="R6" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="S6" s="17">
+      <c r="S6" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="T6" s="17">
         <v>90000000</v>
       </c>
     </row>
@@ -43278,15 +43352,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="7ab8c0d4-f18b-4fef-b649-c77d178c2495">
@@ -43297,31 +43362,55 @@
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FE9F65F-EA31-4275-8B78-F92EA3895E8B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FE9F65F-EA31-4275-8B78-F92EA3895E8B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="7ab8c0d4-f18b-4fef-b649-c77d178c2495"/>
+    <ds:schemaRef ds:uri="65efab6e-20b9-465e-9733-f0c2ab732419"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C685BDB-1785-4A39-A308-4CA166889A49}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE50E33B-922F-4D33-8831-2DF5BA7F11F6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="65efab6e-20b9-465e-9733-f0c2ab732419"/>
+    <ds:schemaRef ds:uri="7ab8c0d4-f18b-4fef-b649-c77d178c2495"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE50E33B-922F-4D33-8831-2DF5BA7F11F6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C685BDB-1785-4A39-A308-4CA166889A49}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="7ab8c0d4-f18b-4fef-b649-c77d178c2495"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="65efab6e-20b9-465e-9733-f0c2ab732419"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
tabla traduccion componente a nomenclatura sabana
</commit_message>
<xml_diff>
--- a/prototipo_pcr/inputs/insumos.xlsx
+++ b/prototipo_pcr/inputs/insumos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://suramericana.sharepoint.com/sites/TraNIFF/Shared Documents/féniX/01 IFRS17/02 Entregables Procesos/05 Reservas/03 PCR CP/03 Tecnología/01 Prototipo/prototipo_pcr/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="195" documentId="13_ncr:1_{3EC42E67-7DA1-2342-97B9-902C865173C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0B3E641F-3141-244E-BB4A-C161E59D8C6B}"/>
+  <xr:revisionPtr revIDLastSave="213" documentId="13_ncr:1_{3EC42E67-7DA1-2342-97B9-902C865173C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB584D9E-E17B-5746-BA54-1334DCDF752C}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17420" tabRatio="959" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17420" tabRatio="959" firstSheet="3" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="param_contabilidad" sheetId="6" r:id="rId1"/>
@@ -24,20 +24,19 @@
     <sheet name="costo_rea_noprop" sheetId="8" r:id="rId9"/>
     <sheet name="seguimiento_rea_noprop" sheetId="19" r:id="rId10"/>
     <sheet name="onerosidad" sheetId="26" r:id="rId11"/>
-    <sheet name="Hoja2" sheetId="27" r:id="rId12"/>
-    <sheet name="map_bt" sheetId="20" r:id="rId13"/>
-    <sheet name="tipo_seguro" sheetId="21" r:id="rId14"/>
-    <sheet name="cuenta_cobrar_directo" sheetId="23" r:id="rId15"/>
-    <sheet name="cuenta_corriente_rea" sheetId="25" r:id="rId16"/>
+    <sheet name="map_bt" sheetId="20" r:id="rId12"/>
+    <sheet name="tipo_seguro" sheetId="21" r:id="rId13"/>
+    <sheet name="cuenta_cobrar_directo" sheetId="23" r:id="rId14"/>
+    <sheet name="cuenta_corriente_rea" sheetId="25" r:id="rId15"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">comision_rea!$A$1:$V$9</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">map_bt!$A$1:$I$261</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">map_bt!$A$1:$I$261</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">param_contabilidad!$A$1:$I$33</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">porc_descuento!$A$1:$K$17</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">produccion_directo!$A$1:$T$18</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">produccion_rea!$A$1:$Y$10</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">tipo_seguro!$A$1:$C$61</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">tipo_seguro!$A$1:$C$61</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -462,7 +461,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>La prima anual registrada corresponde a toda la vigencia de la póliza para todos los tipos de operación</t>
+          <t>Siempre son los mismos, pues la prima anual registrada corresponde a toda la vigencia de la póliza para todos los tipos de operación</t>
         </r>
       </text>
     </comment>
@@ -1641,6 +1640,9 @@
     <t>dias_vigencia</t>
   </si>
   <si>
+    <t>dias_no_devengados</t>
+  </si>
+  <si>
     <t>pct_onerosidad</t>
   </si>
   <si>
@@ -1697,20 +1699,18 @@
   <si>
     <t>valor_prima_onerosa</t>
   </si>
-  <si>
-    <t>dias_onerosidad</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="167" formatCode="_-&quot;$&quot;\ * #,##0.000_-;\-&quot;$&quot;\ * #,##0.000_-;_-&quot;$&quot;\ * &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1831,13 +1831,6 @@
     <font>
       <sz val="11"/>
       <color theme="0" tint="-0.499984740745262"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1981,7 +1974,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Millares [0]" xfId="2" builtinId="6"/>
@@ -4891,8 +4884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20B783E5-A0C2-5D46-A94A-481A8E8B68D6}">
   <dimension ref="A1:V5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="165" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="165" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4911,7 +4904,7 @@
     <col min="12" max="12" width="20.83203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="19" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="17.5" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="13.6640625" bestFit="1" customWidth="1"/>
@@ -4943,7 +4936,7 @@
         <v>368</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>369</v>
@@ -4964,30 +4957,30 @@
         <v>374</v>
       </c>
       <c r="O1" s="5" t="s">
+        <v>375</v>
+      </c>
+      <c r="P1" s="5" t="s">
         <v>394</v>
       </c>
-      <c r="P1" s="5" t="s">
-        <v>393</v>
-      </c>
       <c r="Q1" s="5" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="R1" s="5" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="S1" s="5" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="T1" s="5" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="U1" s="5" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B2" s="14">
         <v>45747</v>
@@ -5005,7 +4998,7 @@
         <v>80</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="H2">
         <v>1200</v>
@@ -5024,7 +5017,7 @@
         <v>46022</v>
       </c>
       <c r="M2" s="14" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="N2">
         <f>+L2-K2+1</f>
@@ -5052,22 +5045,22 @@
         <v>68.046904109589036</v>
       </c>
       <c r="U2" t="s">
-        <v>383</v>
-      </c>
-      <c r="V2" s="17">
-        <f t="shared" ref="V2:V5" si="0">+T2*(L2-DATE(2025,7,31))/(L2-C2+1)</f>
-        <v>37.72165336509827</v>
+        <v>384</v>
+      </c>
+      <c r="V2" s="56">
+        <f>+T2*(L2-DATE(2025,6,30))/(L2-C2+1)</f>
+        <v>45.364602739726024</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="B3" s="14">
         <v>45777</v>
       </c>
       <c r="C3" s="14">
-        <v>45777</v>
+        <v>45762</v>
       </c>
       <c r="D3">
         <v>123456</v>
@@ -5079,7 +5072,7 @@
         <v>80</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="H3">
         <v>200</v>
@@ -5098,19 +5091,19 @@
         <v>46022</v>
       </c>
       <c r="M3" s="14" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="N3">
         <f>+L3-K3+1</f>
         <v>365</v>
       </c>
       <c r="O3">
-        <f t="shared" ref="O3:O5" si="1">+L3-C3</f>
-        <v>245</v>
+        <f t="shared" ref="O3:O5" si="0">+L3-C3</f>
+        <v>260</v>
       </c>
       <c r="P3">
         <f>+O3*H3/N3</f>
-        <v>134.24657534246575</v>
+        <v>142.46575342465752</v>
       </c>
       <c r="Q3" s="55">
         <v>0.08</v>
@@ -5123,25 +5116,25 @@
       </c>
       <c r="T3">
         <f>+P3*Q3*(1-R3)*(1-S3)</f>
-        <v>10.103934246575342</v>
+        <v>10.722542465753424</v>
       </c>
       <c r="U3" t="s">
-        <v>386</v>
-      </c>
-      <c r="V3" s="17">
-        <f t="shared" si="0"/>
-        <v>6.2841542265285666</v>
+        <v>387</v>
+      </c>
+      <c r="V3" s="56">
+        <f>+T3*(L3-DATE(2025,6,30))/(L3-C3+1)</f>
+        <v>7.5591870256652491</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B4" s="14">
         <v>45808</v>
       </c>
       <c r="C4" s="14">
-        <v>45808</v>
+        <v>45795</v>
       </c>
       <c r="D4">
         <v>123456</v>
@@ -5153,7 +5146,7 @@
         <v>80</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="H4">
         <v>1400</v>
@@ -5172,19 +5165,19 @@
         <v>46022</v>
       </c>
       <c r="M4" s="14" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="N4">
         <f>+L4-K4+1</f>
         <v>365</v>
       </c>
       <c r="O4">
-        <f t="shared" si="1"/>
-        <v>214</v>
+        <f t="shared" si="0"/>
+        <v>227</v>
       </c>
       <c r="P4">
         <f>+O4*H4/N4</f>
-        <v>820.82191780821915</v>
+        <v>870.68493150684935</v>
       </c>
       <c r="Q4" s="55">
         <v>-0.01</v>
@@ -5197,25 +5190,25 @@
       </c>
       <c r="T4">
         <f>+P4*Q4*(1-R4)*(1-S4)</f>
-        <v>-7.7222926027397261</v>
+        <v>-8.1914038356164376</v>
       </c>
       <c r="U4" t="s">
-        <v>389</v>
-      </c>
-      <c r="V4" s="17">
-        <f t="shared" si="0"/>
-        <v>-5.4953989219496657</v>
+        <v>390</v>
+      </c>
+      <c r="V4" s="56">
+        <f>+T4*(L4-DATE(2025,6,30))/(L4-C4+1)</f>
+        <v>-6.6106066041816867</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B5" s="14">
         <v>45838</v>
       </c>
       <c r="C5" s="14">
-        <v>45838</v>
+        <v>45815</v>
       </c>
       <c r="D5">
         <v>123456</v>
@@ -5227,7 +5220,7 @@
         <v>80</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="H5">
         <v>1400</v>
@@ -5253,12 +5246,12 @@
         <v>365</v>
       </c>
       <c r="O5">
-        <f t="shared" si="1"/>
-        <v>184</v>
+        <f t="shared" si="0"/>
+        <v>207</v>
       </c>
       <c r="P5">
         <f>+O5*H5/N5</f>
-        <v>705.7534246575342</v>
+        <v>793.97260273972597</v>
       </c>
       <c r="Q5" s="55">
         <v>-7.0000000000000007E-2</v>
@@ -5271,14 +5264,14 @@
       </c>
       <c r="T5">
         <f>+P5*Q5*(1-R5)*(1-S5)</f>
-        <v>-46.478097534246579</v>
+        <v>-52.287859726027392</v>
       </c>
       <c r="U5" t="s">
-        <v>391</v>
-      </c>
-      <c r="V5" s="17">
-        <f>+T5*(L5-DATE(2025,7,31))/(L5-C5+1)</f>
-        <v>-38.438642825620143</v>
+        <v>392</v>
+      </c>
+      <c r="V5" s="56">
+        <f>+T5*(L5-DATE(2025,6,30))/(L5-C5+1)</f>
+        <v>-46.254645142255001</v>
       </c>
     </row>
   </sheetData>
@@ -5288,241 +5281,6 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21AA4FD7-1B77-0D41-9350-7677CF35A11D}">
-  <dimension ref="A1:M13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B1">
-        <v>1</v>
-      </c>
-      <c r="C1">
-        <f>+B1+1</f>
-        <v>2</v>
-      </c>
-      <c r="D1">
-        <f>+C1+1</f>
-        <v>3</v>
-      </c>
-      <c r="E1">
-        <f>+D1+1</f>
-        <v>4</v>
-      </c>
-      <c r="F1">
-        <f>+E1+1</f>
-        <v>5</v>
-      </c>
-      <c r="G1">
-        <f>+F1+1</f>
-        <v>6</v>
-      </c>
-      <c r="H1">
-        <f>+G1+1</f>
-        <v>7</v>
-      </c>
-      <c r="I1">
-        <f>+H1+1</f>
-        <v>8</v>
-      </c>
-      <c r="J1">
-        <f>+I1+1</f>
-        <v>9</v>
-      </c>
-      <c r="K1">
-        <f>+J1+1</f>
-        <v>10</v>
-      </c>
-      <c r="L1">
-        <f>+K1+1</f>
-        <v>11</v>
-      </c>
-      <c r="M1">
-        <f>+L1+1</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <f>+onerosidad!T2</f>
-        <v>68.046904109589036</v>
-      </c>
-      <c r="D3">
-        <f>-A3</f>
-        <v>-68.046904109589036</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <f>+onerosidad!T3</f>
-        <v>10.103934246575342</v>
-      </c>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56">
-        <f>-$D$3/9</f>
-        <v>7.560767123287671</v>
-      </c>
-      <c r="F4" s="56">
-        <f t="shared" ref="F4:M4" si="0">-$D$3/9</f>
-        <v>7.560767123287671</v>
-      </c>
-      <c r="G4" s="56">
-        <f t="shared" si="0"/>
-        <v>7.560767123287671</v>
-      </c>
-      <c r="H4" s="56">
-        <f t="shared" si="0"/>
-        <v>7.560767123287671</v>
-      </c>
-      <c r="I4" s="56">
-        <f t="shared" si="0"/>
-        <v>7.560767123287671</v>
-      </c>
-      <c r="J4" s="56">
-        <f t="shared" si="0"/>
-        <v>7.560767123287671</v>
-      </c>
-      <c r="K4" s="56">
-        <f t="shared" si="0"/>
-        <v>7.560767123287671</v>
-      </c>
-      <c r="L4" s="56">
-        <f t="shared" si="0"/>
-        <v>7.560767123287671</v>
-      </c>
-      <c r="M4" s="56">
-        <f t="shared" si="0"/>
-        <v>7.560767123287671</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <f>+onerosidad!T4</f>
-        <v>-7.7222926027397261</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <f>+onerosidad!T5</f>
-        <v>-46.478097534246579</v>
-      </c>
-      <c r="E6">
-        <f>-A4</f>
-        <v>-10.103934246575342</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="F7">
-        <f>-$E$6/8</f>
-        <v>1.2629917808219178</v>
-      </c>
-      <c r="G7">
-        <f>-$E$6/8</f>
-        <v>1.2629917808219178</v>
-      </c>
-      <c r="H7">
-        <f>-$E$6/8</f>
-        <v>1.2629917808219178</v>
-      </c>
-      <c r="I7">
-        <f>-$E$6/8</f>
-        <v>1.2629917808219178</v>
-      </c>
-      <c r="J7">
-        <f>-$E$6/8</f>
-        <v>1.2629917808219178</v>
-      </c>
-      <c r="K7">
-        <f>-$E$6/8</f>
-        <v>1.2629917808219178</v>
-      </c>
-      <c r="L7">
-        <f>-$E$6/8</f>
-        <v>1.2629917808219178</v>
-      </c>
-      <c r="M7">
-        <f>-$E$6/8</f>
-        <v>1.2629917808219178</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="F9">
-        <f>-A5</f>
-        <v>7.7222926027397261</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="G10">
-        <f>-$F$9/7</f>
-        <v>-1.1031846575342465</v>
-      </c>
-      <c r="H10">
-        <f t="shared" ref="H10:M10" si="1">-$F$9/7</f>
-        <v>-1.1031846575342465</v>
-      </c>
-      <c r="I10">
-        <f t="shared" si="1"/>
-        <v>-1.1031846575342465</v>
-      </c>
-      <c r="J10">
-        <f t="shared" si="1"/>
-        <v>-1.1031846575342465</v>
-      </c>
-      <c r="K10">
-        <f t="shared" si="1"/>
-        <v>-1.1031846575342465</v>
-      </c>
-      <c r="L10">
-        <f t="shared" si="1"/>
-        <v>-1.1031846575342465</v>
-      </c>
-      <c r="M10">
-        <f t="shared" si="1"/>
-        <v>-1.1031846575342465</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="G12">
-        <f>-A6</f>
-        <v>46.478097534246579</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="H13">
-        <f>-$G$12/6</f>
-        <v>-7.7463495890410963</v>
-      </c>
-      <c r="I13">
-        <f>-$G$12/6</f>
-        <v>-7.7463495890410963</v>
-      </c>
-      <c r="J13">
-        <f>-$G$12/6</f>
-        <v>-7.7463495890410963</v>
-      </c>
-      <c r="K13">
-        <f>-$G$12/6</f>
-        <v>-7.7463495890410963</v>
-      </c>
-      <c r="L13">
-        <f>-$G$12/6</f>
-        <v>-7.7463495890410963</v>
-      </c>
-      <c r="M13">
-        <f>-$G$12/6</f>
-        <v>-7.7463495890410963</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A12977D-9D3C-784D-BA64-82A8AADC1B2E}">
   <sheetPr>
     <tabColor theme="4"/>
@@ -12341,7 +12099,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04FB4049-F651-384C-8DCF-CEAFB17703EB}">
   <sheetPr>
     <tabColor theme="4"/>
@@ -13035,7 +12793,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F7F059E-3482-9948-A0EE-3B780BE80211}">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
@@ -13176,7 +12934,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C59D3D0B-BDA7-C849-9A02-F348974FBECC}">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
@@ -40739,7 +40497,7 @@
   <dimension ref="A1:T19"/>
   <sheetViews>
     <sheetView zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -44202,7 +43960,7 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0927BB69-CCA6-4A0B-98A7-FAB196BCC808}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29BC6BAE-B540-4FA6-B5DD-C754AEE24698}"/>
 </file>
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
se eliminan duplicados riesgo credito
</commit_message>
<xml_diff>
--- a/prototipo_pcr/inputs/insumos.xlsx
+++ b/prototipo_pcr/inputs/insumos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://suramericana.sharepoint.com/sites/TraNIFF/Shared Documents/féniX/01 IFRS17/02 Entregables Procesos/05 Reservas/03 PCR CP/03 Tecnología/01 Prototipo/prototipo_pcr/inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://suramericana.sharepoint.com/sites/TraNIFF/Shared Documents/féniX/01 IFRS17/02 Entregables Procesos/05 Reservas/03 PCR CP/03 Tecnología/01 Prototipo/prototipo_pcr/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="275" documentId="13_ncr:1_{3EC42E67-7DA1-2342-97B9-902C865173C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{70724DF7-1213-8B49-8F97-E19E3EC4F780}"/>
+  <xr:revisionPtr revIDLastSave="273" documentId="13_ncr:1_{3EC42E67-7DA1-2342-97B9-902C865173C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BBF821F4-647A-4B4E-A4BF-123A4D2134D7}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" tabRatio="959" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">produccion_rea!$A$1:$Z$10</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">tipo_seguro!$A$1:$C$61</definedName>
   </definedNames>
-  <calcPr calcId="191028" iterate="1"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1727,7 +1727,7 @@
     <numFmt numFmtId="42" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
-    <numFmt numFmtId="167" formatCode="_-&quot;$&quot;\ * #,##0.000_-;\-&quot;$&quot;\ * #,##0.000_-;_-&quot;$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-&quot;$&quot;\ * #,##0.000_-;\-&quot;$&quot;\ * #,##0.000_-;_-&quot;$&quot;\ * &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -1924,7 +1924,7 @@
     <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1988,13 +1988,12 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Millares [0]" xfId="2" builtinId="6"/>
@@ -2331,7 +2330,7 @@
     <col min="5" max="6" width="15.5" customWidth="1"/>
     <col min="7" max="7" width="15.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.5" customWidth="1"/>
-    <col min="9" max="9" width="106.5" style="55" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="106.5" style="54" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -2359,7 +2358,7 @@
       <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="54" t="s">
+      <c r="I1" s="53" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2388,7 +2387,7 @@
       <c r="H2">
         <v>1</v>
       </c>
-      <c r="I2" s="55" t="s">
+      <c r="I2" s="54" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2417,7 +2416,7 @@
       <c r="H3">
         <v>1</v>
       </c>
-      <c r="I3" s="55" t="s">
+      <c r="I3" s="54" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2446,7 +2445,7 @@
       <c r="H4">
         <v>1</v>
       </c>
-      <c r="I4" s="55" t="s">
+      <c r="I4" s="54" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2475,7 +2474,7 @@
       <c r="H5">
         <v>1</v>
       </c>
-      <c r="I5" s="55" t="s">
+      <c r="I5" s="54" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2504,7 +2503,7 @@
       <c r="H6">
         <v>0</v>
       </c>
-      <c r="I6" s="55" t="s">
+      <c r="I6" s="54" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2533,7 +2532,7 @@
       <c r="H7">
         <v>0</v>
       </c>
-      <c r="I7" s="55" t="s">
+      <c r="I7" s="54" t="s">
         <v>29</v>
       </c>
     </row>
@@ -2562,7 +2561,7 @@
       <c r="H8">
         <v>1</v>
       </c>
-      <c r="I8" s="55" t="s">
+      <c r="I8" s="54" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2591,7 +2590,7 @@
       <c r="H9">
         <v>1</v>
       </c>
-      <c r="I9" s="55" t="s">
+      <c r="I9" s="54" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2620,7 +2619,7 @@
       <c r="H10">
         <v>1</v>
       </c>
-      <c r="I10" s="55" t="s">
+      <c r="I10" s="54" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2649,7 +2648,7 @@
       <c r="H11">
         <v>1</v>
       </c>
-      <c r="I11" s="55" t="s">
+      <c r="I11" s="54" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2678,7 +2677,7 @@
       <c r="H12">
         <v>1</v>
       </c>
-      <c r="I12" s="55" t="s">
+      <c r="I12" s="54" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2707,7 +2706,7 @@
       <c r="H13">
         <v>1</v>
       </c>
-      <c r="I13" s="55" t="s">
+      <c r="I13" s="54" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2736,7 +2735,7 @@
       <c r="H14">
         <v>1</v>
       </c>
-      <c r="I14" s="55" t="s">
+      <c r="I14" s="54" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2765,7 +2764,7 @@
       <c r="H15">
         <v>1</v>
       </c>
-      <c r="I15" s="55" t="s">
+      <c r="I15" s="54" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2794,7 +2793,7 @@
       <c r="H16">
         <v>1</v>
       </c>
-      <c r="I16" s="55" t="s">
+      <c r="I16" s="54" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2823,7 +2822,7 @@
       <c r="H17">
         <v>1</v>
       </c>
-      <c r="I17" s="55" t="s">
+      <c r="I17" s="54" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2852,7 +2851,7 @@
       <c r="H18">
         <v>1</v>
       </c>
-      <c r="I18" s="55" t="s">
+      <c r="I18" s="54" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2881,7 +2880,7 @@
       <c r="H19">
         <v>1</v>
       </c>
-      <c r="I19" s="55" t="s">
+      <c r="I19" s="54" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2910,7 +2909,7 @@
       <c r="H20">
         <v>1</v>
       </c>
-      <c r="I20" s="55" t="s">
+      <c r="I20" s="54" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2939,7 +2938,7 @@
       <c r="H21">
         <v>1</v>
       </c>
-      <c r="I21" s="55" t="s">
+      <c r="I21" s="54" t="s">
         <v>42</v>
       </c>
     </row>
@@ -2968,7 +2967,7 @@
       <c r="H22">
         <v>1</v>
       </c>
-      <c r="I22" s="55" t="s">
+      <c r="I22" s="54" t="s">
         <v>42</v>
       </c>
     </row>
@@ -2997,7 +2996,7 @@
       <c r="H23">
         <v>1</v>
       </c>
-      <c r="I23" s="55" t="s">
+      <c r="I23" s="54" t="s">
         <v>45</v>
       </c>
     </row>
@@ -3026,7 +3025,7 @@
       <c r="H24">
         <v>1</v>
       </c>
-      <c r="I24" s="55" t="s">
+      <c r="I24" s="54" t="s">
         <v>47</v>
       </c>
     </row>
@@ -3055,7 +3054,7 @@
       <c r="H25">
         <v>1</v>
       </c>
-      <c r="I25" s="55" t="s">
+      <c r="I25" s="54" t="s">
         <v>49</v>
       </c>
     </row>
@@ -3084,7 +3083,7 @@
       <c r="H26">
         <v>1</v>
       </c>
-      <c r="I26" s="55" t="s">
+      <c r="I26" s="54" t="s">
         <v>51</v>
       </c>
     </row>
@@ -3113,7 +3112,7 @@
       <c r="H27">
         <v>0</v>
       </c>
-      <c r="I27" s="55" t="s">
+      <c r="I27" s="54" t="s">
         <v>53</v>
       </c>
     </row>
@@ -3142,7 +3141,7 @@
       <c r="H28">
         <v>0</v>
       </c>
-      <c r="I28" s="55" t="s">
+      <c r="I28" s="54" t="s">
         <v>55</v>
       </c>
     </row>
@@ -3171,7 +3170,7 @@
       <c r="H29">
         <v>1</v>
       </c>
-      <c r="I29" s="55" t="s">
+      <c r="I29" s="54" t="s">
         <v>58</v>
       </c>
     </row>
@@ -3200,7 +3199,7 @@
       <c r="H30">
         <v>1</v>
       </c>
-      <c r="I30" s="55" t="s">
+      <c r="I30" s="54" t="s">
         <v>45</v>
       </c>
     </row>
@@ -3229,7 +3228,7 @@
       <c r="H31">
         <v>1</v>
       </c>
-      <c r="I31" s="55" t="s">
+      <c r="I31" s="54" t="s">
         <v>58</v>
       </c>
     </row>
@@ -3258,7 +3257,7 @@
       <c r="H32">
         <v>1</v>
       </c>
-      <c r="I32" s="55" t="s">
+      <c r="I32" s="54" t="s">
         <v>45</v>
       </c>
     </row>
@@ -3287,7 +3286,7 @@
       <c r="H33">
         <v>1</v>
       </c>
-      <c r="I33" s="55" t="s">
+      <c r="I33" s="54" t="s">
         <v>58</v>
       </c>
     </row>
@@ -3316,7 +3315,7 @@
       <c r="H34">
         <v>1</v>
       </c>
-      <c r="I34" s="55" t="s">
+      <c r="I34" s="54" t="s">
         <v>42</v>
       </c>
     </row>
@@ -3345,7 +3344,7 @@
       <c r="H35">
         <v>1</v>
       </c>
-      <c r="I35" s="55" t="s">
+      <c r="I35" s="54" t="s">
         <v>42</v>
       </c>
     </row>
@@ -3374,7 +3373,7 @@
       <c r="H36">
         <v>1</v>
       </c>
-      <c r="I36" s="55" t="s">
+      <c r="I36" s="54" t="s">
         <v>45</v>
       </c>
     </row>
@@ -3403,7 +3402,7 @@
       <c r="H37">
         <v>1</v>
       </c>
-      <c r="I37" s="55" t="s">
+      <c r="I37" s="54" t="s">
         <v>47</v>
       </c>
     </row>
@@ -3432,7 +3431,7 @@
       <c r="H38">
         <v>1</v>
       </c>
-      <c r="I38" s="55" t="s">
+      <c r="I38" s="54" t="s">
         <v>49</v>
       </c>
     </row>
@@ -3461,7 +3460,7 @@
       <c r="H39">
         <v>1</v>
       </c>
-      <c r="I39" s="55" t="s">
+      <c r="I39" s="54" t="s">
         <v>51</v>
       </c>
     </row>
@@ -3490,7 +3489,7 @@
       <c r="H40">
         <v>0</v>
       </c>
-      <c r="I40" s="55" t="s">
+      <c r="I40" s="54" t="s">
         <v>53</v>
       </c>
     </row>
@@ -3519,7 +3518,7 @@
       <c r="H41">
         <v>0</v>
       </c>
-      <c r="I41" s="55" t="s">
+      <c r="I41" s="54" t="s">
         <v>55</v>
       </c>
     </row>
@@ -3548,7 +3547,7 @@
       <c r="H42">
         <v>1</v>
       </c>
-      <c r="I42" s="55" t="s">
+      <c r="I42" s="54" t="s">
         <v>58</v>
       </c>
     </row>
@@ -3577,7 +3576,7 @@
       <c r="H43">
         <v>1</v>
       </c>
-      <c r="I43" s="55" t="s">
+      <c r="I43" s="54" t="s">
         <v>45</v>
       </c>
     </row>
@@ -3606,7 +3605,7 @@
       <c r="H44">
         <v>1</v>
       </c>
-      <c r="I44" s="55" t="s">
+      <c r="I44" s="54" t="s">
         <v>58</v>
       </c>
     </row>
@@ -3635,7 +3634,7 @@
       <c r="H45">
         <v>1</v>
       </c>
-      <c r="I45" s="55" t="s">
+      <c r="I45" s="54" t="s">
         <v>45</v>
       </c>
     </row>
@@ -3664,7 +3663,7 @@
       <c r="H46">
         <v>1</v>
       </c>
-      <c r="I46" s="55" t="s">
+      <c r="I46" s="54" t="s">
         <v>58</v>
       </c>
     </row>
@@ -3693,7 +3692,7 @@
       <c r="H47">
         <v>1</v>
       </c>
-      <c r="I47" s="55" t="s">
+      <c r="I47" s="54" t="s">
         <v>42</v>
       </c>
     </row>
@@ -3722,7 +3721,7 @@
       <c r="H48">
         <v>1</v>
       </c>
-      <c r="I48" s="55" t="s">
+      <c r="I48" s="54" t="s">
         <v>42</v>
       </c>
     </row>
@@ -3751,7 +3750,7 @@
       <c r="H49">
         <v>1</v>
       </c>
-      <c r="I49" s="55" t="s">
+      <c r="I49" s="54" t="s">
         <v>45</v>
       </c>
     </row>
@@ -3780,7 +3779,7 @@
       <c r="H50">
         <v>1</v>
       </c>
-      <c r="I50" s="55" t="s">
+      <c r="I50" s="54" t="s">
         <v>47</v>
       </c>
     </row>
@@ -3809,7 +3808,7 @@
       <c r="H51">
         <v>1</v>
       </c>
-      <c r="I51" s="55" t="s">
+      <c r="I51" s="54" t="s">
         <v>49</v>
       </c>
     </row>
@@ -3838,7 +3837,7 @@
       <c r="H52">
         <v>1</v>
       </c>
-      <c r="I52" s="55" t="s">
+      <c r="I52" s="54" t="s">
         <v>51</v>
       </c>
     </row>
@@ -3867,7 +3866,7 @@
       <c r="H53">
         <v>0</v>
       </c>
-      <c r="I53" s="55" t="s">
+      <c r="I53" s="54" t="s">
         <v>53</v>
       </c>
     </row>
@@ -3896,7 +3895,7 @@
       <c r="H54">
         <v>0</v>
       </c>
-      <c r="I54" s="55" t="s">
+      <c r="I54" s="54" t="s">
         <v>55</v>
       </c>
     </row>
@@ -3925,7 +3924,7 @@
       <c r="H55">
         <v>1</v>
       </c>
-      <c r="I55" s="55" t="s">
+      <c r="I55" s="54" t="s">
         <v>58</v>
       </c>
     </row>
@@ -3954,7 +3953,7 @@
       <c r="H56">
         <v>1</v>
       </c>
-      <c r="I56" s="55" t="s">
+      <c r="I56" s="54" t="s">
         <v>45</v>
       </c>
     </row>
@@ -3983,7 +3982,7 @@
       <c r="H57">
         <v>1</v>
       </c>
-      <c r="I57" s="55" t="s">
+      <c r="I57" s="54" t="s">
         <v>58</v>
       </c>
     </row>
@@ -4012,7 +4011,7 @@
       <c r="H58">
         <v>1</v>
       </c>
-      <c r="I58" s="55" t="s">
+      <c r="I58" s="54" t="s">
         <v>45</v>
       </c>
     </row>
@@ -4041,7 +4040,7 @@
       <c r="H59">
         <v>1</v>
       </c>
-      <c r="I59" s="55" t="s">
+      <c r="I59" s="54" t="s">
         <v>58</v>
       </c>
     </row>
@@ -5058,13 +5057,13 @@
         <f>+O2*H2/N2</f>
         <v>904.10958904109589</v>
       </c>
-      <c r="Q2" s="56">
+      <c r="Q2" s="55">
         <v>0.08</v>
       </c>
-      <c r="R2" s="56">
+      <c r="R2" s="55">
         <v>0.04</v>
       </c>
-      <c r="S2" s="56">
+      <c r="S2" s="55">
         <v>0.02</v>
       </c>
       <c r="T2">
@@ -5082,7 +5081,7 @@
         <f>+L2-DATE(2025,7,31)</f>
         <v>153</v>
       </c>
-      <c r="Y2" s="57">
+      <c r="Y2" s="56">
         <f>+T2*X2/W2</f>
         <v>37.72165336509827</v>
       </c>
@@ -5140,13 +5139,13 @@
         <f>+O3*H3/N3</f>
         <v>142.46575342465752</v>
       </c>
-      <c r="Q3" s="56">
+      <c r="Q3" s="55">
         <v>0.08</v>
       </c>
-      <c r="R3" s="56">
+      <c r="R3" s="55">
         <v>0.04</v>
       </c>
-      <c r="S3" s="56">
+      <c r="S3" s="55">
         <v>0.02</v>
       </c>
       <c r="T3">
@@ -5164,7 +5163,7 @@
         <f>+L3-DATE(2025,7,31)</f>
         <v>153</v>
       </c>
-      <c r="Y3" s="57">
+      <c r="Y3" s="56">
         <f>+T3*X3/W3</f>
         <v>6.2856283419933865</v>
       </c>
@@ -5222,13 +5221,13 @@
         <f>+O4*H4/N4</f>
         <v>870.68493150684935</v>
       </c>
-      <c r="Q4" s="56">
+      <c r="Q4" s="55">
         <v>-0.01</v>
       </c>
-      <c r="R4" s="56">
+      <c r="R4" s="55">
         <v>0.04</v>
       </c>
-      <c r="S4" s="56">
+      <c r="S4" s="55">
         <v>0.02</v>
       </c>
       <c r="T4">
@@ -5246,7 +5245,7 @@
         <f>+L4-DATE(2025,7,31)</f>
         <v>153</v>
       </c>
-      <c r="Y4" s="57">
+      <c r="Y4" s="56">
         <f>+T4*X4/W4</f>
         <v>-5.4968631002162933</v>
       </c>
@@ -5304,13 +5303,13 @@
         <f>+O5*H5/N5</f>
         <v>793.97260273972597</v>
       </c>
-      <c r="Q5" s="56">
+      <c r="Q5" s="55">
         <v>-7.0000000000000007E-2</v>
       </c>
-      <c r="R5" s="56">
+      <c r="R5" s="55">
         <v>0.04</v>
       </c>
-      <c r="S5" s="56">
+      <c r="S5" s="55">
         <v>0.02</v>
       </c>
       <c r="T5">
@@ -5328,7 +5327,7 @@
         <f>+L5-DATE(2025,7,31)</f>
         <v>153</v>
       </c>
-      <c r="Y5" s="57">
+      <c r="Y5" s="56">
         <f>+T5*X5/W5</f>
         <v>-38.461742971548993</v>
       </c>
@@ -5383,13 +5382,13 @@
         <f>+O7*H7/N7</f>
         <v>805.47945205479448</v>
       </c>
-      <c r="Q7" s="56">
+      <c r="Q7" s="55">
         <v>-0.08</v>
       </c>
-      <c r="R7" s="56">
+      <c r="R7" s="55">
         <v>0.04</v>
       </c>
-      <c r="S7" s="56">
+      <c r="S7" s="55">
         <v>0.02</v>
       </c>
       <c r="T7">
@@ -5407,7 +5406,7 @@
         <f>+L7-DATE(2025,7,31)</f>
         <v>153</v>
       </c>
-      <c r="Y7" s="57">
+      <c r="Y7" s="56">
         <f>+T7*X7/W7</f>
         <v>-37.704925359171398</v>
       </c>
@@ -41854,7 +41853,7 @@
   <dimension ref="A1:AB21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="I2" sqref="I2:I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -41882,47 +41881,47 @@
     <col min="28" max="28" width="11.5" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="51" t="s">
+    <row r="1" spans="1:28" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
         <v>109</v>
       </c>
       <c r="B1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="C1" s="5" t="s">
         <v>136</v>
       </c>
       <c r="D1" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="51" t="s">
+      <c r="E1" s="5" t="s">
         <v>137</v>
       </c>
       <c r="F1" s="49" t="s">
         <v>361</v>
       </c>
-      <c r="G1" s="51" t="s">
+      <c r="G1" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="H1" s="51" t="s">
+      <c r="H1" s="5" t="s">
         <v>93</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="J1" s="52" t="s">
+      <c r="J1" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="51" t="s">
+      <c r="K1" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="L1" s="51" t="s">
+      <c r="L1" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="M1" s="51" t="s">
+      <c r="M1" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="N1" s="51" t="s">
+      <c r="N1" s="5" t="s">
         <v>96</v>
       </c>
       <c r="O1" s="49" t="s">
@@ -41931,40 +41930,40 @@
       <c r="P1" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="Q1" s="51" t="s">
+      <c r="Q1" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="R1" s="51" t="s">
+      <c r="R1" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="S1" s="51" t="s">
+      <c r="S1" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="T1" s="51" t="s">
+      <c r="T1" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="U1" s="51" t="s">
+      <c r="U1" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="V1" s="51" t="s">
+      <c r="V1" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="W1" s="51" t="s">
+      <c r="W1" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="X1" s="51" t="s">
+      <c r="X1" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="Y1" s="51" t="s">
+      <c r="Y1" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="Z1" s="51" t="s">
+      <c r="Z1" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="AA1" s="51" t="s">
+      <c r="AA1" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="AB1" s="53" t="s">
+      <c r="AB1" s="52" t="s">
         <v>142</v>
       </c>
     </row>
@@ -41993,7 +41992,8 @@
       <c r="H2">
         <v>124324091</v>
       </c>
-      <c r="I2" s="14">
+      <c r="I2">
+        <f>+VLOOKUP(H2,produccion_directo!$D$2:$E$19,2,FALSE)</f>
         <v>45292</v>
       </c>
       <c r="J2" s="24">
@@ -42079,7 +42079,8 @@
       <c r="H3">
         <v>124324091</v>
       </c>
-      <c r="I3" s="14">
+      <c r="I3">
+        <f>+VLOOKUP(H3,produccion_directo!$D$2:$E$19,2,FALSE)</f>
         <v>45292</v>
       </c>
       <c r="J3" s="24">
@@ -42165,7 +42166,8 @@
       <c r="H4">
         <v>124324091</v>
       </c>
-      <c r="I4" s="14">
+      <c r="I4">
+        <f>+VLOOKUP(H4,produccion_directo!$D$2:$E$19,2,FALSE)</f>
         <v>45292</v>
       </c>
       <c r="J4" s="24">
@@ -42251,7 +42253,8 @@
       <c r="H5">
         <v>124324092</v>
       </c>
-      <c r="I5" s="14">
+      <c r="I5">
+        <f>+VLOOKUP(H5,produccion_directo!$D$2:$E$19,2,FALSE)</f>
         <v>45245</v>
       </c>
       <c r="J5" s="24">
@@ -42337,7 +42340,8 @@
       <c r="H6">
         <v>124324092</v>
       </c>
-      <c r="I6" s="14">
+      <c r="I6">
+        <f>+VLOOKUP(H6,produccion_directo!$D$2:$E$19,2,FALSE)</f>
         <v>45245</v>
       </c>
       <c r="J6" s="24">
@@ -42423,7 +42427,8 @@
       <c r="H7">
         <v>124324092</v>
       </c>
-      <c r="I7" s="14">
+      <c r="I7">
+        <f>+VLOOKUP(H7,produccion_directo!$D$2:$E$19,2,FALSE)</f>
         <v>45245</v>
       </c>
       <c r="J7" s="24">
@@ -42509,7 +42514,8 @@
       <c r="H8">
         <v>634535346</v>
       </c>
-      <c r="I8" s="14">
+      <c r="I8">
+        <f>+VLOOKUP(H8,produccion_directo!$D$2:$E$19,2,FALSE)</f>
         <v>45275</v>
       </c>
       <c r="J8" s="24">
@@ -42595,7 +42601,8 @@
       <c r="H9">
         <v>345675387</v>
       </c>
-      <c r="I9" s="14">
+      <c r="I9">
+        <f>+VLOOKUP(H9,produccion_directo!$D$2:$E$19,2,FALSE)</f>
         <v>45342</v>
       </c>
       <c r="J9" s="24">
@@ -42681,7 +42688,8 @@
       <c r="H10">
         <v>345675387</v>
       </c>
-      <c r="I10" s="14">
+      <c r="I10">
+        <f>+VLOOKUP(H10,produccion_directo!$D$2:$E$19,2,FALSE)</f>
         <v>45342</v>
       </c>
       <c r="J10" s="24">
@@ -42757,7 +42765,7 @@
     </row>
     <row r="21" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F21" t="str">
-        <f t="shared" ref="F13:F26" si="0">+LOWER(F11)</f>
+        <f t="shared" ref="F21" si="0">+LOWER(F11)</f>
         <v/>
       </c>
     </row>
@@ -43887,19 +43895,8 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7ab8c0d4-f18b-4fef-b649-c77d178c2495">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="65efab6e-20b9-465e-9733-f0c2ab732419" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003456B0730C78B347BD7589BC061D6E7A" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="eb47ff602caa7ec4c93498109dbc0598">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7ab8c0d4-f18b-4fef-b649-c77d178c2495" xmlns:ns3="65efab6e-20b9-465e-9733-f0c2ab732419" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="15d39866744b831c8a58edb1b96951e3" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101003456B0730C78B347BD7589BC061D6E7A" ma:contentTypeVersion="12" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="63fa1c64418ad5e2c432e8a28af753ff">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7ab8c0d4-f18b-4fef-b649-c77d178c2495" xmlns:ns3="65efab6e-20b9-465e-9733-f0c2ab732419" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0084d3678d80c20d937c1596fa80271a" ns2:_="" ns3:_="">
     <xsd:import namespace="7ab8c0d4-f18b-4fef-b649-c77d178c2495"/>
     <xsd:import namespace="65efab6e-20b9-465e-9733-f0c2ab732419"/>
     <xsd:element name="properties">
@@ -43949,7 +43946,7 @@
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="13" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="68ae7bf6-5ac9-4edb-a7e0-886d92fb71e5" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="13" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Etiquetas de imagen" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="68ae7bf6-5ac9-4edb-a7e0-886d92fb71e5" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
@@ -44008,8 +44005,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Tipo de contenido"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Título"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -44098,6 +44095,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7ab8c0d4-f18b-4fef-b649-c77d178c2495">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="65efab6e-20b9-465e-9733-f0c2ab732419" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C685BDB-1785-4A39-A308-4CA166889A49}">
   <ds:schemaRefs>
@@ -44107,24 +44115,24 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE50E33B-922F-4D33-8831-2DF5BA7F11F6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="7ab8c0d4-f18b-4fef-b649-c77d178c2495"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="65efab6e-20b9-465e-9733-f0c2ab732419"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{810C8FED-C705-4335-91D9-7FBBCD676D0F}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{842D5E37-BA4B-4B32-A043-AB9B5363C194}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE50E33B-922F-4D33-8831-2DF5BA7F11F6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="65efab6e-20b9-465e-9733-f0c2ab732419"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="7ab8c0d4-f18b-4fef-b649-c77d178c2495"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
Agregar hoja de insumo de onerosidad y detalle en param_contabilidad
</commit_message>
<xml_diff>
--- a/prototipo_pcr/inputs/insumos.xlsx
+++ b/prototipo_pcr/inputs/insumos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://suramericana.sharepoint.com/sites/TraNIFF/Shared Documents/féniX/01 IFRS17/02 Entregables Procesos/05 Reservas/03 PCR CP/03 Tecnología/01 Prototipo/prototipo_pcr/inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://suramericana.sharepoint.com/sites/TraNIFF/Shared Documents/féniX/01 IFRS17/02 Entregables Procesos/05 Reservas/03 PCR CP/03 Tecnología/01 Prototipo/prototipo_pcr/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="277" documentId="13_ncr:1_{3EC42E67-7DA1-2342-97B9-902C865173C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C51D2A4-F8F5-C144-9DBE-1028A83E1F94}"/>
+  <xr:revisionPtr revIDLastSave="310" documentId="13_ncr:1_{3EC42E67-7DA1-2342-97B9-902C865173C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37E48C4E-A301-7348-9256-F86EF1ED55E9}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" tabRatio="959" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" tabRatio="959" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="param_contabilidad" sheetId="6" r:id="rId1"/>
@@ -32,7 +32,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">comision_rea!$A$1:$V$9</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">map_bt!$A$1:$I$261</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">param_contabilidad!$A$1:$I$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">param_contabilidad!$A$1:$I$35</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">porc_descuento!$A$1:$K$17</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">produccion_directo!$A$1:$T$18</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">produccion_rea!$A$1:$Z$10</definedName>
@@ -107,7 +107,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F22" authorId="0" shapeId="0" xr:uid="{CADF5D80-B324-BD4D-83EF-7103C7C4BCDC}">
+    <comment ref="F24" authorId="0" shapeId="0" xr:uid="{CADF5D80-B324-BD4D-83EF-7103C7C4BCDC}">
       <text>
         <r>
           <rPr>
@@ -120,7 +120,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F35" authorId="0" shapeId="0" xr:uid="{60B7F3D0-2F4A-0645-8858-314766FA3CB7}">
+    <comment ref="F37" authorId="0" shapeId="0" xr:uid="{60B7F3D0-2F4A-0645-8858-314766FA3CB7}">
       <text>
         <r>
           <rPr>
@@ -133,7 +133,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F48" authorId="0" shapeId="0" xr:uid="{F47F6BE0-1988-7A49-8D44-80895B191E26}">
+    <comment ref="F50" authorId="0" shapeId="0" xr:uid="{F47F6BE0-1988-7A49-8D44-80895B191E26}">
       <text>
         <r>
           <rPr>
@@ -445,7 +445,7 @@
     <author>Sebatian Tobon Echavarría</author>
   </authors>
   <commentList>
-    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{64744ABB-A17D-A545-BFCC-CC32FD80DAF0}">
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{E04BEEEF-5039-174B-BB2C-DDBC8BC35098}">
       <text>
         <r>
           <rPr>
@@ -475,6 +475,39 @@
             <family val="2"/>
           </rPr>
           <t>Siempre son los mismos, pues la prima anual registrada corresponde a toda la vigencia de la póliza para todos los tipos de operación</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{F19DA337-D789-FD42-AABD-13D069A00F53}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sebatian Tobon Echavarría:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tiene que tener el +1, porque son los días de vigencia con los que se va a devengar la onerosidad</t>
         </r>
       </text>
     </comment>
@@ -526,7 +559,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7311" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7327" uniqueCount="396">
   <si>
     <t>tipo_insumo</t>
   </si>
@@ -1614,9 +1647,6 @@
     <t>tipo_reasegurador</t>
   </si>
   <si>
-    <t>tipo_reaesegurador</t>
-  </si>
-  <si>
     <t>mantenido</t>
   </si>
   <si>
@@ -1713,21 +1743,20 @@
     <t>valor_prima_vigencia</t>
   </si>
   <si>
-    <t>dias_vig</t>
+    <t>onerosidad</t>
   </si>
   <si>
-    <t>dias_no_dev</t>
+    <t>componente de onerosidad del seguro directo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="42" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
-    <numFmt numFmtId="165" formatCode="_-&quot;$&quot;\ * #,##0.000_-;\-&quot;$&quot;\ * #,##0.000_-;_-&quot;$&quot;\ * &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -1924,7 +1953,7 @@
     <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1993,7 +2022,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Millares [0]" xfId="2" builtinId="6"/>
@@ -2315,10 +2343,10 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:I59"/>
+  <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:B20"/>
+    <sheetView topLeftCell="B1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2915,16 +2943,16 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>38</v>
+        <v>394</v>
       </c>
       <c r="B21" t="s">
-        <v>39</v>
+        <v>394</v>
       </c>
       <c r="C21" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="D21" t="s">
-        <v>363</v>
+        <v>11</v>
       </c>
       <c r="E21" t="s">
         <v>30</v>
@@ -2933,62 +2961,62 @@
         <v>31</v>
       </c>
       <c r="G21">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H21">
         <v>1</v>
       </c>
       <c r="I21" s="54" t="s">
-        <v>42</v>
+        <v>395</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>38</v>
+        <v>394</v>
       </c>
       <c r="B22" t="s">
-        <v>39</v>
+        <v>394</v>
       </c>
       <c r="C22" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="D22" t="s">
-        <v>363</v>
+        <v>11</v>
       </c>
       <c r="E22" t="s">
         <v>32</v>
       </c>
-      <c r="F22" s="30" t="s">
-        <v>13</v>
+      <c r="F22" t="s">
+        <v>31</v>
       </c>
       <c r="G22">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H22">
         <v>1</v>
       </c>
       <c r="I22" s="54" t="s">
-        <v>42</v>
+        <v>395</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B23" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="C23" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D23" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E23" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="F23" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="G23">
         <v>1</v>
@@ -2997,26 +3025,26 @@
         <v>1</v>
       </c>
       <c r="I23" s="54" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B24" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="C24" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D24" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E24" t="s">
-        <v>12</v>
-      </c>
-      <c r="F24" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24" s="30" t="s">
         <v>13</v>
       </c>
       <c r="G24">
@@ -3026,21 +3054,21 @@
         <v>1</v>
       </c>
       <c r="I24" s="54" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B25" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C25" t="s">
         <v>44</v>
       </c>
       <c r="D25" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E25" t="s">
         <v>12</v>
@@ -3055,21 +3083,21 @@
         <v>1</v>
       </c>
       <c r="I25" s="54" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B26" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C26" t="s">
         <v>44</v>
       </c>
       <c r="D26" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E26" t="s">
         <v>12</v>
@@ -3078,27 +3106,27 @@
         <v>13</v>
       </c>
       <c r="G26">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H26">
         <v>1</v>
       </c>
       <c r="I26" s="54" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C27" t="s">
         <v>44</v>
       </c>
       <c r="D27" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E27" t="s">
         <v>12</v>
@@ -3110,24 +3138,24 @@
         <v>1</v>
       </c>
       <c r="H27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I27" s="54" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B28" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C28" t="s">
         <v>44</v>
       </c>
       <c r="D28" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E28" t="s">
         <v>12</v>
@@ -3136,27 +3164,27 @@
         <v>13</v>
       </c>
       <c r="G28">
+        <v>-1</v>
+      </c>
+      <c r="H28">
         <v>1</v>
       </c>
-      <c r="H28">
-        <v>0</v>
-      </c>
       <c r="I28" s="54" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B29" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="C29" t="s">
         <v>44</v>
       </c>
       <c r="D29" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E29" t="s">
         <v>12</v>
@@ -3165,42 +3193,42 @@
         <v>13</v>
       </c>
       <c r="G29">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I29" s="54" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="B30" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="C30" t="s">
         <v>44</v>
       </c>
       <c r="D30" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E30" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="F30" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="G30">
         <v>1</v>
       </c>
       <c r="H30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I30" s="54" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
@@ -3214,13 +3242,13 @@
         <v>44</v>
       </c>
       <c r="D31" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E31" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="F31" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="G31">
         <v>-1</v>
@@ -3243,10 +3271,10 @@
         <v>44</v>
       </c>
       <c r="D32" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E32" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F32" t="s">
         <v>31</v>
@@ -3272,10 +3300,10 @@
         <v>44</v>
       </c>
       <c r="D33" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E33" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F33" t="s">
         <v>31</v>
@@ -3292,51 +3320,51 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B34" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="C34" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D34" t="s">
-        <v>59</v>
+        <v>362</v>
       </c>
       <c r="E34" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F34" t="s">
         <v>31</v>
       </c>
       <c r="G34">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H34">
         <v>1</v>
       </c>
       <c r="I34" s="54" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="B35" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="C35" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D35" t="s">
-        <v>59</v>
+        <v>362</v>
       </c>
       <c r="E35" t="s">
         <v>32</v>
       </c>
-      <c r="F35" s="30" t="s">
-        <v>13</v>
+      <c r="F35" t="s">
+        <v>31</v>
       </c>
       <c r="G35">
         <v>-1</v>
@@ -3345,27 +3373,27 @@
         <v>1</v>
       </c>
       <c r="I35" s="54" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B36" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="C36" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D36" t="s">
         <v>59</v>
       </c>
       <c r="E36" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="F36" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="G36">
         <v>-1</v>
@@ -3374,26 +3402,26 @@
         <v>1</v>
       </c>
       <c r="I36" s="54" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B37" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="C37" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D37" t="s">
         <v>59</v>
       </c>
       <c r="E37" t="s">
-        <v>12</v>
-      </c>
-      <c r="F37" t="s">
+        <v>32</v>
+      </c>
+      <c r="F37" s="30" t="s">
         <v>13</v>
       </c>
       <c r="G37">
@@ -3403,15 +3431,15 @@
         <v>1</v>
       </c>
       <c r="I37" s="54" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B38" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C38" t="s">
         <v>44</v>
@@ -3432,15 +3460,15 @@
         <v>1</v>
       </c>
       <c r="I38" s="54" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B39" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C39" t="s">
         <v>44</v>
@@ -3455,21 +3483,21 @@
         <v>13</v>
       </c>
       <c r="G39">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H39">
         <v>1</v>
       </c>
       <c r="I39" s="54" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B40" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C40" t="s">
         <v>44</v>
@@ -3487,18 +3515,18 @@
         <v>-1</v>
       </c>
       <c r="H40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I40" s="54" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B41" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C41" t="s">
         <v>44</v>
@@ -3513,21 +3541,21 @@
         <v>13</v>
       </c>
       <c r="G41">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I41" s="54" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B42" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="C42" t="s">
         <v>44</v>
@@ -3542,21 +3570,21 @@
         <v>13</v>
       </c>
       <c r="G42">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I42" s="54" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="B43" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="C43" t="s">
         <v>44</v>
@@ -3565,19 +3593,19 @@
         <v>59</v>
       </c>
       <c r="E43" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="F43" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="G43">
         <v>-1</v>
       </c>
       <c r="H43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I43" s="54" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
@@ -3594,10 +3622,10 @@
         <v>59</v>
       </c>
       <c r="E44" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="F44" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="G44">
         <v>1</v>
@@ -3623,7 +3651,7 @@
         <v>59</v>
       </c>
       <c r="E45" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F45" t="s">
         <v>31</v>
@@ -3652,7 +3680,7 @@
         <v>59</v>
       </c>
       <c r="E46" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F46" t="s">
         <v>31</v>
@@ -3669,51 +3697,51 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B47" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="C47" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D47" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E47" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F47" t="s">
         <v>31</v>
       </c>
       <c r="G47">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H47">
         <v>1</v>
       </c>
       <c r="I47" s="54" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="B48" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="C48" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D48" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E48" t="s">
         <v>32</v>
       </c>
-      <c r="F48" s="30" t="s">
-        <v>13</v>
+      <c r="F48" t="s">
+        <v>31</v>
       </c>
       <c r="G48">
         <v>1</v>
@@ -3722,27 +3750,27 @@
         <v>1</v>
       </c>
       <c r="I48" s="54" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B49" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="C49" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D49" t="s">
         <v>60</v>
       </c>
       <c r="E49" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="F49" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="G49">
         <v>1</v>
@@ -3751,26 +3779,26 @@
         <v>1</v>
       </c>
       <c r="I49" s="54" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B50" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="C50" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D50" t="s">
         <v>60</v>
       </c>
       <c r="E50" t="s">
-        <v>12</v>
-      </c>
-      <c r="F50" t="s">
+        <v>32</v>
+      </c>
+      <c r="F50" s="30" t="s">
         <v>13</v>
       </c>
       <c r="G50">
@@ -3780,15 +3808,15 @@
         <v>1</v>
       </c>
       <c r="I50" s="54" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B51" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C51" t="s">
         <v>44</v>
@@ -3809,15 +3837,15 @@
         <v>1</v>
       </c>
       <c r="I51" s="54" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B52" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C52" t="s">
         <v>44</v>
@@ -3832,21 +3860,21 @@
         <v>13</v>
       </c>
       <c r="G52">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H52">
         <v>1</v>
       </c>
       <c r="I52" s="54" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B53" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C53" t="s">
         <v>44</v>
@@ -3864,18 +3892,18 @@
         <v>1</v>
       </c>
       <c r="H53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I53" s="54" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B54" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C54" t="s">
         <v>44</v>
@@ -3890,21 +3918,21 @@
         <v>13</v>
       </c>
       <c r="G54">
+        <v>-1</v>
+      </c>
+      <c r="H54">
         <v>1</v>
       </c>
-      <c r="H54">
-        <v>0</v>
-      </c>
       <c r="I54" s="54" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B55" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="C55" t="s">
         <v>44</v>
@@ -3919,21 +3947,21 @@
         <v>13</v>
       </c>
       <c r="G55">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I55" s="54" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="C56" t="s">
         <v>44</v>
@@ -3942,19 +3970,19 @@
         <v>60</v>
       </c>
       <c r="E56" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="F56" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="G56">
         <v>1</v>
       </c>
       <c r="H56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I56" s="54" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
@@ -3971,10 +3999,10 @@
         <v>60</v>
       </c>
       <c r="E57" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="F57" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="G57">
         <v>-1</v>
@@ -4000,7 +4028,7 @@
         <v>60</v>
       </c>
       <c r="E58" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F58" t="s">
         <v>31</v>
@@ -4029,7 +4057,7 @@
         <v>60</v>
       </c>
       <c r="E59" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F59" t="s">
         <v>31</v>
@@ -4041,6 +4069,64 @@
         <v>1</v>
       </c>
       <c r="I59" s="54" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>43</v>
+      </c>
+      <c r="B60" t="s">
+        <v>10</v>
+      </c>
+      <c r="C60" t="s">
+        <v>44</v>
+      </c>
+      <c r="D60" t="s">
+        <v>60</v>
+      </c>
+      <c r="E60" t="s">
+        <v>32</v>
+      </c>
+      <c r="F60" t="s">
+        <v>31</v>
+      </c>
+      <c r="G60">
+        <v>1</v>
+      </c>
+      <c r="H60">
+        <v>1</v>
+      </c>
+      <c r="I60" s="54" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>56</v>
+      </c>
+      <c r="B61" t="s">
+        <v>57</v>
+      </c>
+      <c r="C61" t="s">
+        <v>44</v>
+      </c>
+      <c r="D61" t="s">
+        <v>60</v>
+      </c>
+      <c r="E61" t="s">
+        <v>32</v>
+      </c>
+      <c r="F61" t="s">
+        <v>31</v>
+      </c>
+      <c r="G61">
+        <v>-1</v>
+      </c>
+      <c r="H61">
+        <v>1</v>
+      </c>
+      <c r="I61" s="54" t="s">
         <v>58</v>
       </c>
     </row>
@@ -4901,514 +4987,410 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20B783E5-A0C2-5D46-A94A-481A8E8B68D6}">
-  <dimension ref="A1:Y7"/>
+  <dimension ref="A1:W5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="39.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="58.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="58.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>366</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>345</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="F1" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>367</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>284</v>
-      </c>
-      <c r="G1" s="5" t="s">
+      <c r="J1" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="K1" s="5" t="s">
         <v>368</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="L1" s="5" t="s">
+        <v>369</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>372</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>373</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>374</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>375</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>377</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>379</v>
+      </c>
+      <c r="W1" s="5" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>381</v>
+      </c>
+      <c r="B2" s="14" t="s">
         <v>394</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>369</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>370</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>371</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>372</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>373</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>374</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>375</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>376</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>377</v>
-      </c>
-      <c r="R1" s="5" t="s">
-        <v>378</v>
-      </c>
-      <c r="S1" s="5" t="s">
-        <v>379</v>
-      </c>
-      <c r="T1" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="U1" s="5" t="s">
-        <v>381</v>
-      </c>
-      <c r="W1" s="5" t="s">
-        <v>395</v>
-      </c>
-      <c r="X1" s="5" t="s">
-        <v>396</v>
-      </c>
-      <c r="Y1" s="5" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="C2" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="14">
+        <v>45747</v>
+      </c>
+      <c r="E2" s="14">
+        <v>45747</v>
+      </c>
+      <c r="F2">
+        <v>123456</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I2" s="7" t="s">
         <v>382</v>
       </c>
-      <c r="B2" s="14">
-        <v>45747</v>
-      </c>
-      <c r="C2" s="14">
-        <v>45747</v>
-      </c>
-      <c r="D2">
-        <v>123456</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>383</v>
-      </c>
-      <c r="H2">
+      <c r="J2">
         <v>1200</v>
-      </c>
-      <c r="I2" s="14">
-        <v>45658</v>
-      </c>
-      <c r="J2">
-        <f>+YEAR(I2)</f>
-        <v>2025</v>
       </c>
       <c r="K2" s="14">
         <v>45658</v>
       </c>
-      <c r="L2" s="14">
+      <c r="L2">
+        <f>+YEAR(K2)</f>
+        <v>2025</v>
+      </c>
+      <c r="M2" s="14">
+        <v>45658</v>
+      </c>
+      <c r="N2" s="14">
         <v>46022</v>
       </c>
-      <c r="M2" s="14" t="s">
+      <c r="O2" s="14" t="s">
+        <v>383</v>
+      </c>
+      <c r="P2">
+        <f>+N2-M2+1</f>
+        <v>365</v>
+      </c>
+      <c r="Q2">
+        <f>+N2-E2+1</f>
+        <v>276</v>
+      </c>
+      <c r="R2">
+        <f>+Q2*J2/P2</f>
+        <v>907.39726027397262</v>
+      </c>
+      <c r="S2" s="55">
+        <v>0.08</v>
+      </c>
+      <c r="T2" s="55">
+        <v>0.04</v>
+      </c>
+      <c r="U2" s="55">
+        <v>0.02</v>
+      </c>
+      <c r="V2">
+        <f>+R2*S2*(1-T2)*(1-U2)</f>
+        <v>68.294347397260267</v>
+      </c>
+      <c r="W2" t="s">
         <v>384</v>
       </c>
-      <c r="N2">
-        <f>+L2-K2+1</f>
-        <v>365</v>
-      </c>
-      <c r="O2">
-        <f>+L2-C2</f>
-        <v>275</v>
-      </c>
-      <c r="P2">
-        <f>+O2*H2/N2</f>
-        <v>904.10958904109589</v>
-      </c>
-      <c r="Q2" s="55">
-        <v>0.08</v>
-      </c>
-      <c r="R2" s="55">
-        <v>0.04</v>
-      </c>
-      <c r="S2" s="55">
-        <v>0.02</v>
-      </c>
-      <c r="T2">
-        <f>+P2*Q2*(1-R2)*(1-S2)</f>
-        <v>68.046904109589036</v>
-      </c>
-      <c r="U2" t="s">
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>385</v>
       </c>
-      <c r="W2">
-        <f>+L2-C2+1</f>
-        <v>276</v>
-      </c>
-      <c r="X2">
-        <f>+L2-DATE(2025,7,31)</f>
-        <v>153</v>
-      </c>
-      <c r="Y2" s="56">
-        <f>+T2*X2/W2</f>
-        <v>37.72165336509827</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>386</v>
-      </c>
-      <c r="B3" s="14">
+      <c r="B3" s="14" t="s">
+        <v>394</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="14">
         <v>45777</v>
       </c>
-      <c r="C3" s="14">
+      <c r="E3" s="14">
         <v>45762</v>
       </c>
-      <c r="D3">
+      <c r="F3">
         <v>123456</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="G3" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="H3" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="G3" s="7" t="s">
-        <v>383</v>
-      </c>
-      <c r="H3">
+      <c r="I3" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="J3">
         <v>200</v>
-      </c>
-      <c r="I3" s="14">
-        <v>45658</v>
-      </c>
-      <c r="J3">
-        <f>+YEAR(I3)</f>
-        <v>2025</v>
       </c>
       <c r="K3" s="14">
         <v>45658</v>
       </c>
-      <c r="L3" s="14">
+      <c r="L3">
+        <f>+YEAR(K3)</f>
+        <v>2025</v>
+      </c>
+      <c r="M3" s="14">
+        <v>45658</v>
+      </c>
+      <c r="N3" s="14">
         <v>46022</v>
       </c>
-      <c r="M3" s="14" t="s">
+      <c r="O3" s="14" t="s">
+        <v>386</v>
+      </c>
+      <c r="P3">
+        <f>+N3-M3+1</f>
+        <v>365</v>
+      </c>
+      <c r="Q3">
+        <f>+N3-E3+1</f>
+        <v>261</v>
+      </c>
+      <c r="R3">
+        <f>+Q3*J3/P3</f>
+        <v>143.01369863013699</v>
+      </c>
+      <c r="S3" s="55">
+        <v>0.08</v>
+      </c>
+      <c r="T3" s="55">
+        <v>0.04</v>
+      </c>
+      <c r="U3" s="55">
+        <v>0.02</v>
+      </c>
+      <c r="V3">
+        <f>+R3*S3*(1-T3)*(1-U3)</f>
+        <v>10.76378301369863</v>
+      </c>
+      <c r="W3" t="s">
         <v>387</v>
       </c>
-      <c r="N3">
-        <f>+L3-K3+1</f>
-        <v>365</v>
-      </c>
-      <c r="O3">
-        <f>+L3-C3</f>
-        <v>260</v>
-      </c>
-      <c r="P3">
-        <f>+O3*H3/N3</f>
-        <v>142.46575342465752</v>
-      </c>
-      <c r="Q3" s="55">
-        <v>0.08</v>
-      </c>
-      <c r="R3" s="55">
-        <v>0.04</v>
-      </c>
-      <c r="S3" s="55">
-        <v>0.02</v>
-      </c>
-      <c r="T3">
-        <f>+P3*Q3*(1-R3)*(1-S3)</f>
-        <v>10.722542465753424</v>
-      </c>
-      <c r="U3" t="s">
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>388</v>
       </c>
-      <c r="W3">
-        <f>+L3-C3+1</f>
-        <v>261</v>
-      </c>
-      <c r="X3">
-        <f>+L3-DATE(2025,7,31)</f>
-        <v>153</v>
-      </c>
-      <c r="Y3" s="56">
-        <f>+T3*X3/W3</f>
-        <v>6.2856283419933865</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>389</v>
-      </c>
-      <c r="B4" s="14">
+      <c r="B4" s="14" t="s">
+        <v>394</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="14">
         <v>45808</v>
       </c>
-      <c r="C4" s="14">
+      <c r="E4" s="14">
         <v>45795</v>
       </c>
-      <c r="D4">
+      <c r="F4">
         <v>123456</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="G4" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="H4" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="G4" s="7" t="s">
-        <v>383</v>
-      </c>
-      <c r="H4">
+      <c r="I4" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="J4">
         <v>1400</v>
-      </c>
-      <c r="I4" s="14">
-        <v>45658</v>
-      </c>
-      <c r="J4">
-        <f>+YEAR(I4)</f>
-        <v>2025</v>
       </c>
       <c r="K4" s="14">
         <v>45658</v>
       </c>
-      <c r="L4" s="14">
+      <c r="L4">
+        <f>+YEAR(K4)</f>
+        <v>2025</v>
+      </c>
+      <c r="M4" s="14">
+        <v>45658</v>
+      </c>
+      <c r="N4" s="14">
         <v>46022</v>
       </c>
-      <c r="M4" s="14" t="s">
+      <c r="O4" s="14" t="s">
+        <v>389</v>
+      </c>
+      <c r="P4">
+        <f>+N4-M4+1</f>
+        <v>365</v>
+      </c>
+      <c r="Q4">
+        <f>+N4-E4+1</f>
+        <v>228</v>
+      </c>
+      <c r="R4">
+        <f>+Q4*J4/P4</f>
+        <v>874.52054794520552</v>
+      </c>
+      <c r="S4" s="55">
+        <v>-0.01</v>
+      </c>
+      <c r="T4" s="55">
+        <v>0.04</v>
+      </c>
+      <c r="U4" s="55">
+        <v>0.02</v>
+      </c>
+      <c r="V4">
+        <f>+R4*S4*(1-T4)*(1-U4)</f>
+        <v>-8.2274893150684925</v>
+      </c>
+      <c r="W4" t="s">
         <v>390</v>
       </c>
-      <c r="N4">
-        <f>+L4-K4+1</f>
-        <v>365</v>
-      </c>
-      <c r="O4">
-        <f>+L4-C4</f>
-        <v>227</v>
-      </c>
-      <c r="P4">
-        <f>+O4*H4/N4</f>
-        <v>870.68493150684935</v>
-      </c>
-      <c r="Q4" s="55">
-        <v>-0.01</v>
-      </c>
-      <c r="R4" s="55">
-        <v>0.04</v>
-      </c>
-      <c r="S4" s="55">
-        <v>0.02</v>
-      </c>
-      <c r="T4">
-        <f>+P4*Q4*(1-R4)*(1-S4)</f>
-        <v>-8.1914038356164376</v>
-      </c>
-      <c r="U4" t="s">
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>391</v>
       </c>
-      <c r="W4">
-        <f>+L4-C4+1</f>
-        <v>228</v>
-      </c>
-      <c r="X4">
-        <f>+L4-DATE(2025,7,31)</f>
-        <v>153</v>
-      </c>
-      <c r="Y4" s="56">
-        <f>+T4*X4/W4</f>
-        <v>-5.4968631002162933</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>392</v>
-      </c>
-      <c r="B5" s="14">
+      <c r="B5" s="14" t="s">
+        <v>394</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="14">
         <v>45838</v>
       </c>
-      <c r="C5" s="14">
+      <c r="E5" s="14">
         <v>45815</v>
       </c>
-      <c r="D5">
+      <c r="F5">
         <v>123456</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="G5" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="H5" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="G5" s="7" t="s">
-        <v>383</v>
-      </c>
-      <c r="H5">
+      <c r="I5" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="J5">
         <v>1400</v>
-      </c>
-      <c r="I5" s="14">
-        <v>45658</v>
-      </c>
-      <c r="J5">
-        <f>+YEAR(I5)</f>
-        <v>2025</v>
       </c>
       <c r="K5" s="14">
         <v>45658</v>
       </c>
-      <c r="L5" s="14">
+      <c r="L5">
+        <f>+YEAR(K5)</f>
+        <v>2025</v>
+      </c>
+      <c r="M5" s="14">
+        <v>45658</v>
+      </c>
+      <c r="N5" s="14">
         <v>46022</v>
       </c>
-      <c r="M5" s="14" t="s">
+      <c r="O5" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="N5">
-        <f>+L5-K5+1</f>
+      <c r="P5">
+        <f>+N5-M5+1</f>
         <v>365</v>
       </c>
-      <c r="O5">
-        <f>+L5-C5</f>
-        <v>207</v>
-      </c>
-      <c r="P5">
-        <f>+O5*H5/N5</f>
-        <v>793.97260273972597</v>
-      </c>
-      <c r="Q5" s="55">
+      <c r="Q5">
+        <f>+N5-E5+1</f>
+        <v>208</v>
+      </c>
+      <c r="R5">
+        <f>+Q5*J5/P5</f>
+        <v>797.80821917808214</v>
+      </c>
+      <c r="S5" s="55">
         <v>-7.0000000000000007E-2</v>
       </c>
-      <c r="R5" s="55">
+      <c r="T5" s="55">
         <v>0.04</v>
       </c>
-      <c r="S5" s="55">
+      <c r="U5" s="55">
         <v>0.02</v>
       </c>
-      <c r="T5">
-        <f>+P5*Q5*(1-R5)*(1-S5)</f>
-        <v>-52.287859726027392</v>
-      </c>
-      <c r="U5" t="s">
-        <v>393</v>
-      </c>
-      <c r="W5">
-        <f>+L5-C5+1</f>
-        <v>208</v>
-      </c>
-      <c r="X5">
-        <f>+L5-DATE(2025,7,31)</f>
-        <v>153</v>
-      </c>
-      <c r="Y5" s="56">
-        <f>+T5*X5/W5</f>
-        <v>-38.461742971548993</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B7" s="14">
-        <v>45777</v>
-      </c>
-      <c r="C7" s="14">
-        <v>45777</v>
-      </c>
-      <c r="D7">
-        <v>123456</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>383</v>
-      </c>
-      <c r="H7">
-        <v>1200</v>
-      </c>
-      <c r="I7" s="14">
-        <v>45658</v>
-      </c>
-      <c r="J7">
-        <f>+YEAR(I7)</f>
-        <v>2025</v>
-      </c>
-      <c r="K7" s="14">
-        <v>45658</v>
-      </c>
-      <c r="L7" s="14">
-        <v>46022</v>
-      </c>
-      <c r="M7" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="N7">
-        <f>+L7-K7+1</f>
-        <v>365</v>
-      </c>
-      <c r="O7">
-        <f>+L7-C7</f>
-        <v>245</v>
-      </c>
-      <c r="P7">
-        <f>+O7*H7/N7</f>
-        <v>805.47945205479448</v>
-      </c>
-      <c r="Q7" s="55">
-        <v>-0.08</v>
-      </c>
-      <c r="R7" s="55">
-        <v>0.04</v>
-      </c>
-      <c r="S7" s="55">
-        <v>0.02</v>
-      </c>
-      <c r="T7">
-        <f>+P7*Q7*(1-R7)*(1-S7)</f>
-        <v>-60.623605479452053</v>
-      </c>
-      <c r="U7" t="s">
-        <v>393</v>
-      </c>
-      <c r="W7">
-        <f>+L7-C7+1</f>
-        <v>246</v>
-      </c>
-      <c r="X7">
-        <f>+L7-DATE(2025,7,31)</f>
-        <v>153</v>
-      </c>
-      <c r="Y7" s="56">
-        <f>+T7*X7/W7</f>
-        <v>-37.704925359171398</v>
+      <c r="V5">
+        <f>+R5*S5*(1-T5)*(1-U5)</f>
+        <v>-52.540458082191783</v>
+      </c>
+      <c r="W5" t="s">
+        <v>392</v>
       </c>
     </row>
   </sheetData>
@@ -41852,7 +41834,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4F93C6E-21BF-4220-AF0D-6D307F3158B8}">
   <dimension ref="A1:AB21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
+    <sheetView zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
@@ -41978,13 +41960,13 @@
         <v>1111</v>
       </c>
       <c r="D2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E2">
         <v>2374188</v>
       </c>
       <c r="F2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="G2">
         <v>0.4</v>
@@ -42065,13 +42047,13 @@
         <v>1111</v>
       </c>
       <c r="D3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E3">
         <v>6987458</v>
       </c>
       <c r="F3" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="G3">
         <v>0.3</v>
@@ -42152,13 +42134,13 @@
         <v>1111</v>
       </c>
       <c r="D4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E4">
         <v>3693358</v>
       </c>
       <c r="F4" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="G4">
         <v>0.3</v>
@@ -42239,13 +42221,13 @@
         <v>1111</v>
       </c>
       <c r="D5" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E5">
         <v>2374188</v>
       </c>
       <c r="F5" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="G5">
         <v>0.4</v>
@@ -42326,13 +42308,13 @@
         <v>1111</v>
       </c>
       <c r="D6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E6">
         <v>6987458</v>
       </c>
       <c r="F6" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="G6">
         <v>0.3</v>
@@ -42413,13 +42395,13 @@
         <v>1111</v>
       </c>
       <c r="D7" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E7">
         <v>3693358</v>
       </c>
       <c r="F7" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="G7">
         <v>0.3</v>
@@ -42500,13 +42482,13 @@
         <v>1113</v>
       </c>
       <c r="D8" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E8">
         <v>3339928</v>
       </c>
       <c r="F8" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -42587,13 +42569,13 @@
         <v>1245</v>
       </c>
       <c r="D9" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E9">
         <v>3693358</v>
       </c>
       <c r="F9" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="G9">
         <v>0.5</v>
@@ -42674,13 +42656,13 @@
         <v>1245</v>
       </c>
       <c r="D10" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E10">
         <v>2374188</v>
       </c>
       <c r="F10" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="G10">
         <v>0.5</v>
@@ -42823,7 +42805,7 @@
         <v>137</v>
       </c>
       <c r="F1" s="49" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>138</v>
@@ -42891,13 +42873,13 @@
         <v>1111</v>
       </c>
       <c r="D2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E2">
         <v>2374188</v>
       </c>
       <c r="F2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="G2">
         <v>0.4</v>
@@ -42965,13 +42947,13 @@
         <v>1111</v>
       </c>
       <c r="D3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E3">
         <v>6987458</v>
       </c>
       <c r="F3" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="G3">
         <v>0.3</v>
@@ -43039,13 +43021,13 @@
         <v>1111</v>
       </c>
       <c r="D4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E4">
         <v>3693358</v>
       </c>
       <c r="F4" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="G4">
         <v>0.3</v>
@@ -43113,13 +43095,13 @@
         <v>1111</v>
       </c>
       <c r="D5" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E5">
         <v>2374188</v>
       </c>
       <c r="F5" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="G5">
         <v>0.4</v>
@@ -43187,13 +43169,13 @@
         <v>1111</v>
       </c>
       <c r="D6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E6">
         <v>6987458</v>
       </c>
       <c r="F6" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="G6">
         <v>0.3</v>
@@ -43261,13 +43243,13 @@
         <v>1111</v>
       </c>
       <c r="D7" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E7">
         <v>3693358</v>
       </c>
       <c r="F7" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="G7">
         <v>0.3</v>
@@ -43335,13 +43317,13 @@
         <v>1245</v>
       </c>
       <c r="D8" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E8">
         <v>3693358</v>
       </c>
       <c r="F8" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="G8">
         <v>0.5</v>
@@ -43409,13 +43391,13 @@
         <v>1245</v>
       </c>
       <c r="D9" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E9">
         <v>2374188</v>
       </c>
       <c r="F9" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="G9">
         <v>0.5</v>
@@ -43573,7 +43555,7 @@
         <v>292161</v>
       </c>
       <c r="C2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D2" s="14">
         <f>+EDATE(E2,12)-1</f>
@@ -43586,7 +43568,7 @@
         <v>507351248</v>
       </c>
       <c r="G2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="H2">
         <v>0.2</v>
@@ -43635,7 +43617,7 @@
         <v>292161</v>
       </c>
       <c r="C3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D3" s="14">
         <f>+EDATE(E3,12)-1</f>
@@ -43648,7 +43630,7 @@
         <v>368484453</v>
       </c>
       <c r="G3" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="H3">
         <v>0.8</v>
@@ -43697,7 +43679,7 @@
         <v>373318</v>
       </c>
       <c r="C4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D4" s="14">
         <f>+EDATE(E4,12)-1</f>
@@ -43710,7 +43692,7 @@
         <v>446526767</v>
       </c>
       <c r="G4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -43759,7 +43741,7 @@
         <v>867346</v>
       </c>
       <c r="C5" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D5" s="14">
         <f>+EDATE(E5,12)-1</f>
@@ -43772,7 +43754,7 @@
         <v>325775298</v>
       </c>
       <c r="G5" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -43821,7 +43803,7 @@
         <v>867346</v>
       </c>
       <c r="C6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D6" s="14">
         <f>+EDATE(E6,12)-1</f>
@@ -43834,7 +43816,7 @@
         <v>360681631</v>
       </c>
       <c r="G6" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -43886,19 +43868,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7ab8c0d4-f18b-4fef-b649-c77d178c2495">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="65efab6e-20b9-465e-9733-f0c2ab732419" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101003456B0730C78B347BD7589BC061D6E7A" ma:contentTypeVersion="12" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="63fa1c64418ad5e2c432e8a28af753ff">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7ab8c0d4-f18b-4fef-b649-c77d178c2495" xmlns:ns3="65efab6e-20b9-465e-9733-f0c2ab732419" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0084d3678d80c20d937c1596fa80271a" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003456B0730C78B347BD7589BC061D6E7A" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="eb47ff602caa7ec4c93498109dbc0598">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7ab8c0d4-f18b-4fef-b649-c77d178c2495" xmlns:ns3="65efab6e-20b9-465e-9733-f0c2ab732419" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="15d39866744b831c8a58edb1b96951e3" ns2:_="" ns3:_="">
     <xsd:import namespace="7ab8c0d4-f18b-4fef-b649-c77d178c2495"/>
     <xsd:import namespace="65efab6e-20b9-465e-9733-f0c2ab732419"/>
     <xsd:element name="properties">
@@ -43948,7 +43928,7 @@
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="13" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Etiquetas de imagen" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="68ae7bf6-5ac9-4edb-a7e0-886d92fb71e5" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="13" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="68ae7bf6-5ac9-4edb-a7e0-886d92fb71e5" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
@@ -44007,8 +43987,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Tipo de contenido"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Título"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -44098,54 +44078,41 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7ab8c0d4-f18b-4fef-b649-c77d178c2495">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="65efab6e-20b9-465e-9733-f0c2ab732419" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE50E33B-922F-4D33-8831-2DF5BA7F11F6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C685BDB-1785-4A39-A308-4CA166889A49}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="7ab8c0d4-f18b-4fef-b649-c77d178c2495"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="65efab6e-20b9-465e-9733-f0c2ab732419"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{810C8FED-C705-4335-91D9-7FBBCD676D0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="7ab8c0d4-f18b-4fef-b649-c77d178c2495"/>
-    <ds:schemaRef ds:uri="65efab6e-20b9-465e-9733-f0c2ab732419"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F3C7F6A-0FC9-41A9-B239-02CC4793674F}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C685BDB-1785-4A39-A308-4CA166889A49}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE50E33B-922F-4D33-8831-2DF5BA7F11F6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7ab8c0d4-f18b-4fef-b649-c77d178c2495"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="65efab6e-20b9-465e-9733-f0c2ab732419"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Agregar insumo de recuperacion de onerosidad PP
</commit_message>
<xml_diff>
--- a/prototipo_pcr/inputs/insumos.xlsx
+++ b/prototipo_pcr/inputs/insumos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10720"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10824"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://suramericana.sharepoint.com/sites/TraNIFF/Shared Documents/féniX/01 IFRS17/02 Entregables Procesos/05 Reservas/03 PCR CP/03 Tecnología/01 Prototipo/prototipo_pcr/inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebatoec/Library/CloudStorage/OneDrive-SharedLibraries-SegurosSuramericana,S.A/Proyecto féniX - féniX/01 IFRS17/02 Entregables Procesos/05 Reservas/03 PCR CP/03 Tecnología/01 Prototipo/prototipo_pcr/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="404" documentId="13_ncr:1_{3EC42E67-7DA1-2342-97B9-902C865173C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0F1092D7-4EEC-944C-A6F4-7C97CA90E6A7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4908367B-1DF6-8B42-97B3-D3B46F8EE6F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17420" tabRatio="959" firstSheet="4" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17420" tabRatio="959" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="param_contabilidad" sheetId="6" r:id="rId1"/>
@@ -24,19 +24,20 @@
     <sheet name="costo_rea_noprop" sheetId="8" r:id="rId9"/>
     <sheet name="seguimiento_rea_noprop" sheetId="19" r:id="rId10"/>
     <sheet name="onerosidad" sheetId="26" r:id="rId11"/>
-    <sheet name="map_bt" sheetId="20" r:id="rId12"/>
-    <sheet name="tipo_seguro" sheetId="21" r:id="rId13"/>
-    <sheet name="cuenta_cobrar_directo" sheetId="23" r:id="rId14"/>
-    <sheet name="cuenta_corriente_rea" sheetId="25" r:id="rId15"/>
+    <sheet name="recup_onerosidad" sheetId="27" r:id="rId12"/>
+    <sheet name="map_bt" sheetId="20" r:id="rId13"/>
+    <sheet name="tipo_seguro" sheetId="21" r:id="rId14"/>
+    <sheet name="cuenta_cobrar_directo" sheetId="23" r:id="rId15"/>
+    <sheet name="cuenta_corriente_rea" sheetId="25" r:id="rId16"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">comision_rea!$A$1:$V$9</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">map_bt!$A$1:$I$261</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">param_contabilidad!$A$1:$I$36</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">map_bt!$A$1:$I$261</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">param_contabilidad!$A$1:$I$39</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">porc_descuento!$A$1:$K$17</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">produccion_directo!$A$1:$T$18</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">produccion_rea!$A$1:$Z$10</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">tipo_seguro!$A$1:$C$61</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">tipo_seguro!$A$1:$C$61</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -107,7 +108,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F25" authorId="0" shapeId="0" xr:uid="{CADF5D80-B324-BD4D-83EF-7103C7C4BCDC}">
+    <comment ref="F27" authorId="0" shapeId="0" xr:uid="{E2EB6F16-7DC2-B547-9D29-6287117B6B6D}">
       <text>
         <r>
           <rPr>
@@ -120,7 +121,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F38" authorId="0" shapeId="0" xr:uid="{60B7F3D0-2F4A-0645-8858-314766FA3CB7}">
+    <comment ref="F28" authorId="0" shapeId="0" xr:uid="{CADF5D80-B324-BD4D-83EF-7103C7C4BCDC}">
       <text>
         <r>
           <rPr>
@@ -133,7 +134,46 @@
         </r>
       </text>
     </comment>
-    <comment ref="F51" authorId="0" shapeId="0" xr:uid="{F47F6BE0-1988-7A49-8D44-80895B191E26}">
+    <comment ref="F43" authorId="0" shapeId="0" xr:uid="{7D06FA4A-5748-C349-AE6A-6BF22180618F}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>aquí cobertura no tiene tanto sentido</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F44" authorId="0" shapeId="0" xr:uid="{60B7F3D0-2F4A-0645-8858-314766FA3CB7}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>aquí cobertura no tiene tanto sentido</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F59" authorId="0" shapeId="0" xr:uid="{03FC245B-BB84-D04E-951E-37009D11D476}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>aquí cobertura no tiene tanto sentido</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F60" authorId="0" shapeId="0" xr:uid="{F47F6BE0-1988-7A49-8D44-80895B191E26}">
       <text>
         <r>
           <rPr>
@@ -153,6 +193,49 @@
 <file path=xl/comments10.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>Priscilla Andrea Palacios Ruiz</author>
+  </authors>
+  <commentList>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{F45A81B6-76FA-6A45-BF63-3EFA4DDE4845}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Priscilla Andrea Palacios Ruiz:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>saldo constitucion / saldo liberacion / movimiento constitucion / movimiento liberacion / fluctuacion / deterioro</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments11.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
     <author>tc={B4F53F10-94F2-0D4A-8418-EA623B88C944}</author>
   </authors>
   <commentList>
@@ -168,7 +251,7 @@
 </comments>
 </file>
 
-<file path=xl/comments11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments12.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Priscilla Andrea Palacios Ruiz</author>
@@ -386,7 +469,7 @@
     <author>Priscilla Andrea Palacios Ruiz</author>
   </authors>
   <commentList>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{1770F033-91D7-0047-BD15-7694292C6393}">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{1770F033-91D7-0047-BD15-7694292C6393}">
       <text>
         <r>
           <rPr>
@@ -399,7 +482,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{C8C07976-3C72-1D44-9A79-A6697E245BBC}">
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{C8C07976-3C72-1D44-9A79-A6697E245BBC}">
       <text>
         <r>
           <rPr>
@@ -568,18 +651,8 @@
     <author>Priscilla Andrea Palacios Ruiz</author>
   </authors>
   <commentList>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{F45A81B6-76FA-6A45-BF63-3EFA4DDE4845}">
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{4528A10A-A994-8442-A047-E7A1AE24EFF8}">
       <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Priscilla Andrea Palacios Ruiz:</t>
-        </r>
         <r>
           <rPr>
             <sz val="10"/>
@@ -587,17 +660,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>saldo constitucion / saldo liberacion / movimiento constitucion / movimiento liberacion / fluctuacion / deterioro</t>
+          <t>Está completa total contrato, se abre por reasegurador con la columna porcentaje participacion reasegurador. Si ya viene abierta no es necesaria esta operación</t>
         </r>
       </text>
     </comment>
@@ -606,7 +669,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7340" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7446" uniqueCount="396">
   <si>
     <t>tipo_insumo</t>
   </si>
@@ -1759,6 +1822,42 @@
   <si>
     <t>fecha_calculo_onerosidad</t>
   </si>
+  <si>
+    <t>tipo_reaseguro</t>
+  </si>
+  <si>
+    <t>no_proporcional</t>
+  </si>
+  <si>
+    <t>participacion_reasegurador</t>
+  </si>
+  <si>
+    <t>valor_recuperacion</t>
+  </si>
+  <si>
+    <t>fecha_inicio_vigencia_contrato</t>
+  </si>
+  <si>
+    <t>fecha_fin_vigencia_contrato</t>
+  </si>
+  <si>
+    <t>fecha_calculo</t>
+  </si>
+  <si>
+    <t>recuperacion_reasegurador_multiple</t>
+  </si>
+  <si>
+    <t>recuperacion_reasegurador_unico</t>
+  </si>
+  <si>
+    <t>recup_onerosidad_pp</t>
+  </si>
+  <si>
+    <t>recuperación del componente de onerosidad por reaseguro</t>
+  </si>
+  <si>
+    <t>recup_onerosidad_np</t>
+  </si>
 </sst>
 </file>
 
@@ -1964,7 +2063,7 @@
     <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2033,6 +2132,8 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Millares [0]" xfId="2" builtinId="6"/>
@@ -2354,10 +2455,10 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:I62"/>
+  <dimension ref="A1:I71"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="A14" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3041,22 +3142,22 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>40</v>
+        <v>393</v>
       </c>
       <c r="B24" t="s">
-        <v>41</v>
+        <v>393</v>
       </c>
       <c r="C24" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D24" t="s">
         <v>43</v>
       </c>
       <c r="E24" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="F24" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="G24">
         <v>1</v>
@@ -3065,27 +3166,27 @@
         <v>1</v>
       </c>
       <c r="I24" s="54" t="s">
-        <v>44</v>
+        <v>394</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>40</v>
+        <v>393</v>
       </c>
       <c r="B25" t="s">
-        <v>41</v>
+        <v>393</v>
       </c>
       <c r="C25" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D25" t="s">
         <v>43</v>
       </c>
       <c r="E25" t="s">
-        <v>32</v>
-      </c>
-      <c r="F25" s="30" t="s">
-        <v>13</v>
+        <v>30</v>
+      </c>
+      <c r="F25" t="s">
+        <v>31</v>
       </c>
       <c r="G25">
         <v>1</v>
@@ -3094,15 +3195,15 @@
         <v>1</v>
       </c>
       <c r="I25" s="54" t="s">
-        <v>44</v>
+        <v>394</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>45</v>
+        <v>393</v>
       </c>
       <c r="B26" t="s">
-        <v>10</v>
+        <v>393</v>
       </c>
       <c r="C26" t="s">
         <v>46</v>
@@ -3111,10 +3212,10 @@
         <v>43</v>
       </c>
       <c r="E26" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="F26" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="G26">
         <v>1</v>
@@ -3123,26 +3224,26 @@
         <v>1</v>
       </c>
       <c r="I26" s="54" t="s">
-        <v>47</v>
+        <v>394</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B27" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="C27" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D27" t="s">
         <v>43</v>
       </c>
       <c r="E27" t="s">
-        <v>12</v>
-      </c>
-      <c r="F27" t="s">
+        <v>30</v>
+      </c>
+      <c r="F27" s="30" t="s">
         <v>13</v>
       </c>
       <c r="G27">
@@ -3152,26 +3253,26 @@
         <v>1</v>
       </c>
       <c r="I27" s="54" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B28" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="C28" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D28" t="s">
         <v>43</v>
       </c>
       <c r="E28" t="s">
-        <v>12</v>
-      </c>
-      <c r="F28" t="s">
+        <v>32</v>
+      </c>
+      <c r="F28" s="30" t="s">
         <v>13</v>
       </c>
       <c r="G28">
@@ -3181,15 +3282,15 @@
         <v>1</v>
       </c>
       <c r="I28" s="54" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B29" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="C29" t="s">
         <v>46</v>
@@ -3204,21 +3305,21 @@
         <v>13</v>
       </c>
       <c r="G29">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H29">
         <v>1</v>
       </c>
       <c r="I29" s="54" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B30" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="C30" t="s">
         <v>46</v>
@@ -3236,18 +3337,18 @@
         <v>1</v>
       </c>
       <c r="H30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I30" s="54" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B31" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="C31" t="s">
         <v>46</v>
@@ -3265,18 +3366,18 @@
         <v>1</v>
       </c>
       <c r="H31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I31" s="54" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B32" t="s">
-        <v>59</v>
+        <v>22</v>
       </c>
       <c r="C32" t="s">
         <v>46</v>
@@ -3297,15 +3398,15 @@
         <v>1</v>
       </c>
       <c r="I32" s="54" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="B33" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C33" t="s">
         <v>46</v>
@@ -3314,27 +3415,27 @@
         <v>43</v>
       </c>
       <c r="E33" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="F33" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="G33">
         <v>1</v>
       </c>
       <c r="H33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I33" s="54" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B34" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="C34" t="s">
         <v>46</v>
@@ -3343,27 +3444,27 @@
         <v>43</v>
       </c>
       <c r="E34" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="F34" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="G34">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I34" s="54" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="B35" t="s">
-        <v>10</v>
+        <v>59</v>
       </c>
       <c r="C35" t="s">
         <v>46</v>
@@ -3372,27 +3473,27 @@
         <v>43</v>
       </c>
       <c r="E35" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="F35" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="G35">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H35">
         <v>1</v>
       </c>
       <c r="I35" s="54" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="B36" t="s">
-        <v>59</v>
+        <v>10</v>
       </c>
       <c r="C36" t="s">
         <v>46</v>
@@ -3401,33 +3502,33 @@
         <v>43</v>
       </c>
       <c r="E36" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F36" t="s">
         <v>31</v>
       </c>
       <c r="G36">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H36">
         <v>1</v>
       </c>
       <c r="I36" s="54" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="B37" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="C37" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D37" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="E37" t="s">
         <v>30</v>
@@ -3442,56 +3543,56 @@
         <v>1</v>
       </c>
       <c r="I37" s="54" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B38" t="s">
-        <v>41</v>
+        <v>10</v>
       </c>
       <c r="C38" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D38" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="E38" t="s">
         <v>32</v>
       </c>
-      <c r="F38" s="30" t="s">
-        <v>13</v>
+      <c r="F38" t="s">
+        <v>31</v>
       </c>
       <c r="G38">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H38">
         <v>1</v>
       </c>
       <c r="I38" s="54" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="B39" t="s">
-        <v>10</v>
+        <v>59</v>
       </c>
       <c r="C39" t="s">
         <v>46</v>
       </c>
       <c r="D39" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="E39" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="F39" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="G39">
         <v>-1</v>
@@ -3500,15 +3601,15 @@
         <v>1</v>
       </c>
       <c r="I39" s="54" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>48</v>
+        <v>393</v>
       </c>
       <c r="B40" t="s">
-        <v>16</v>
+        <v>393</v>
       </c>
       <c r="C40" t="s">
         <v>46</v>
@@ -3523,21 +3624,21 @@
         <v>13</v>
       </c>
       <c r="G40">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H40">
         <v>1</v>
       </c>
       <c r="I40" s="54" t="s">
-        <v>49</v>
+        <v>394</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>50</v>
+        <v>393</v>
       </c>
       <c r="B41" t="s">
-        <v>19</v>
+        <v>393</v>
       </c>
       <c r="C41" t="s">
         <v>46</v>
@@ -3546,27 +3647,27 @@
         <v>61</v>
       </c>
       <c r="E41" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="F41" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="G41">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H41">
         <v>1</v>
       </c>
       <c r="I41" s="54" t="s">
-        <v>51</v>
+        <v>394</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>52</v>
+        <v>393</v>
       </c>
       <c r="B42" t="s">
-        <v>22</v>
+        <v>393</v>
       </c>
       <c r="C42" t="s">
         <v>46</v>
@@ -3575,10 +3676,10 @@
         <v>61</v>
       </c>
       <c r="E42" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="F42" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="G42">
         <v>1</v>
@@ -3587,73 +3688,73 @@
         <v>1</v>
       </c>
       <c r="I42" s="54" t="s">
-        <v>53</v>
+        <v>394</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="B43" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="C43" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D43" t="s">
         <v>61</v>
       </c>
       <c r="E43" t="s">
-        <v>12</v>
-      </c>
-      <c r="F43" t="s">
+        <v>30</v>
+      </c>
+      <c r="F43" s="30" t="s">
         <v>13</v>
       </c>
       <c r="G43">
         <v>-1</v>
       </c>
       <c r="H43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I43" s="54" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="B44" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C44" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D44" t="s">
         <v>61</v>
       </c>
       <c r="E44" t="s">
-        <v>12</v>
-      </c>
-      <c r="F44" t="s">
+        <v>32</v>
+      </c>
+      <c r="F44" s="30" t="s">
         <v>13</v>
       </c>
       <c r="G44">
         <v>-1</v>
       </c>
       <c r="H44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I44" s="54" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="B45" t="s">
-        <v>59</v>
+        <v>10</v>
       </c>
       <c r="C45" t="s">
         <v>46</v>
@@ -3668,21 +3769,21 @@
         <v>13</v>
       </c>
       <c r="G45">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H45">
         <v>1</v>
       </c>
       <c r="I45" s="54" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B46" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C46" t="s">
         <v>46</v>
@@ -3691,10 +3792,10 @@
         <v>61</v>
       </c>
       <c r="E46" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="F46" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="G46">
         <v>-1</v>
@@ -3703,15 +3804,15 @@
         <v>1</v>
       </c>
       <c r="I46" s="54" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B47" t="s">
-        <v>59</v>
+        <v>19</v>
       </c>
       <c r="C47" t="s">
         <v>46</v>
@@ -3720,27 +3821,27 @@
         <v>61</v>
       </c>
       <c r="E47" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="F47" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="G47">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H47">
         <v>1</v>
       </c>
       <c r="I47" s="54" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B48" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="C48" t="s">
         <v>46</v>
@@ -3749,27 +3850,27 @@
         <v>61</v>
       </c>
       <c r="E48" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="F48" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="G48">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H48">
         <v>1</v>
       </c>
       <c r="I48" s="54" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B49" t="s">
-        <v>59</v>
+        <v>25</v>
       </c>
       <c r="C49" t="s">
         <v>46</v>
@@ -3778,67 +3879,67 @@
         <v>61</v>
       </c>
       <c r="E49" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="F49" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="G49">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I49" s="54" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="B50" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C50" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E50" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="F50" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="G50">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I50" s="54" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="B51" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="C51" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D51" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E51" t="s">
-        <v>32</v>
-      </c>
-      <c r="F51" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="F51" t="s">
         <v>13</v>
       </c>
       <c r="G51">
@@ -3848,7 +3949,7 @@
         <v>1</v>
       </c>
       <c r="I51" s="54" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
@@ -3862,16 +3963,16 @@
         <v>46</v>
       </c>
       <c r="D52" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E52" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="F52" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="G52">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H52">
         <v>1</v>
@@ -3882,22 +3983,22 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="B53" t="s">
-        <v>16</v>
+        <v>59</v>
       </c>
       <c r="C53" t="s">
         <v>46</v>
       </c>
       <c r="D53" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E53" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="F53" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="G53">
         <v>1</v>
@@ -3906,73 +4007,73 @@
         <v>1</v>
       </c>
       <c r="I53" s="54" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B54" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C54" t="s">
         <v>46</v>
       </c>
       <c r="D54" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E54" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="F54" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="G54">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H54">
         <v>1</v>
       </c>
       <c r="I54" s="54" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B55" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="C55" t="s">
         <v>46</v>
       </c>
       <c r="D55" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E55" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="F55" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="G55">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H55">
         <v>1</v>
       </c>
       <c r="I55" s="54" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>54</v>
+        <v>393</v>
       </c>
       <c r="B56" t="s">
-        <v>25</v>
+        <v>393</v>
       </c>
       <c r="C56" t="s">
         <v>46</v>
@@ -3990,18 +4091,18 @@
         <v>1</v>
       </c>
       <c r="H56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I56" s="54" t="s">
-        <v>55</v>
+        <v>394</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>56</v>
+        <v>393</v>
       </c>
       <c r="B57" t="s">
-        <v>28</v>
+        <v>393</v>
       </c>
       <c r="C57" t="s">
         <v>46</v>
@@ -4010,27 +4111,27 @@
         <v>62</v>
       </c>
       <c r="E57" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="F57" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="G57">
         <v>1</v>
       </c>
       <c r="H57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I57" s="54" t="s">
-        <v>57</v>
+        <v>394</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>58</v>
+        <v>393</v>
       </c>
       <c r="B58" t="s">
-        <v>59</v>
+        <v>393</v>
       </c>
       <c r="C58" t="s">
         <v>46</v>
@@ -4039,30 +4140,30 @@
         <v>62</v>
       </c>
       <c r="E58" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="F58" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="G58">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H58">
         <v>1</v>
       </c>
       <c r="I58" s="54" t="s">
-        <v>60</v>
+        <v>394</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B59" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="C59" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D59" t="s">
         <v>62</v>
@@ -4070,8 +4171,8 @@
       <c r="E59" t="s">
         <v>30</v>
       </c>
-      <c r="F59" t="s">
-        <v>31</v>
+      <c r="F59" s="30" t="s">
+        <v>13</v>
       </c>
       <c r="G59">
         <v>1</v>
@@ -4080,36 +4181,36 @@
         <v>1</v>
       </c>
       <c r="I59" s="54" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="B60" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="C60" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D60" t="s">
         <v>62</v>
       </c>
       <c r="E60" t="s">
-        <v>30</v>
-      </c>
-      <c r="F60" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="F60" s="30" t="s">
+        <v>13</v>
       </c>
       <c r="G60">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H60">
         <v>1</v>
       </c>
       <c r="I60" s="54" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
@@ -4126,10 +4227,10 @@
         <v>62</v>
       </c>
       <c r="E61" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="F61" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="G61">
         <v>1</v>
@@ -4143,10 +4244,10 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="B62" t="s">
-        <v>59</v>
+        <v>16</v>
       </c>
       <c r="C62" t="s">
         <v>46</v>
@@ -4155,18 +4256,279 @@
         <v>62</v>
       </c>
       <c r="E62" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="F62" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="G62">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H62">
         <v>1</v>
       </c>
       <c r="I62" s="54" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>50</v>
+      </c>
+      <c r="B63" t="s">
+        <v>19</v>
+      </c>
+      <c r="C63" t="s">
+        <v>46</v>
+      </c>
+      <c r="D63" t="s">
+        <v>62</v>
+      </c>
+      <c r="E63" t="s">
+        <v>12</v>
+      </c>
+      <c r="F63" t="s">
+        <v>13</v>
+      </c>
+      <c r="G63">
+        <v>1</v>
+      </c>
+      <c r="H63">
+        <v>1</v>
+      </c>
+      <c r="I63" s="54" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>52</v>
+      </c>
+      <c r="B64" t="s">
+        <v>22</v>
+      </c>
+      <c r="C64" t="s">
+        <v>46</v>
+      </c>
+      <c r="D64" t="s">
+        <v>62</v>
+      </c>
+      <c r="E64" t="s">
+        <v>12</v>
+      </c>
+      <c r="F64" t="s">
+        <v>13</v>
+      </c>
+      <c r="G64">
+        <v>-1</v>
+      </c>
+      <c r="H64">
+        <v>1</v>
+      </c>
+      <c r="I64" s="54" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>54</v>
+      </c>
+      <c r="B65" t="s">
+        <v>25</v>
+      </c>
+      <c r="C65" t="s">
+        <v>46</v>
+      </c>
+      <c r="D65" t="s">
+        <v>62</v>
+      </c>
+      <c r="E65" t="s">
+        <v>12</v>
+      </c>
+      <c r="F65" t="s">
+        <v>13</v>
+      </c>
+      <c r="G65">
+        <v>1</v>
+      </c>
+      <c r="H65">
+        <v>0</v>
+      </c>
+      <c r="I65" s="54" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>56</v>
+      </c>
+      <c r="B66" t="s">
+        <v>28</v>
+      </c>
+      <c r="C66" t="s">
+        <v>46</v>
+      </c>
+      <c r="D66" t="s">
+        <v>62</v>
+      </c>
+      <c r="E66" t="s">
+        <v>12</v>
+      </c>
+      <c r="F66" t="s">
+        <v>13</v>
+      </c>
+      <c r="G66">
+        <v>1</v>
+      </c>
+      <c r="H66">
+        <v>0</v>
+      </c>
+      <c r="I66" s="54" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>58</v>
+      </c>
+      <c r="B67" t="s">
+        <v>59</v>
+      </c>
+      <c r="C67" t="s">
+        <v>46</v>
+      </c>
+      <c r="D67" t="s">
+        <v>62</v>
+      </c>
+      <c r="E67" t="s">
+        <v>12</v>
+      </c>
+      <c r="F67" t="s">
+        <v>13</v>
+      </c>
+      <c r="G67">
+        <v>-1</v>
+      </c>
+      <c r="H67">
+        <v>1</v>
+      </c>
+      <c r="I67" s="54" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>45</v>
+      </c>
+      <c r="B68" t="s">
+        <v>10</v>
+      </c>
+      <c r="C68" t="s">
+        <v>46</v>
+      </c>
+      <c r="D68" t="s">
+        <v>62</v>
+      </c>
+      <c r="E68" t="s">
+        <v>30</v>
+      </c>
+      <c r="F68" t="s">
+        <v>31</v>
+      </c>
+      <c r="G68">
+        <v>1</v>
+      </c>
+      <c r="H68">
+        <v>1</v>
+      </c>
+      <c r="I68" s="54" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>58</v>
+      </c>
+      <c r="B69" t="s">
+        <v>59</v>
+      </c>
+      <c r="C69" t="s">
+        <v>46</v>
+      </c>
+      <c r="D69" t="s">
+        <v>62</v>
+      </c>
+      <c r="E69" t="s">
+        <v>30</v>
+      </c>
+      <c r="F69" t="s">
+        <v>31</v>
+      </c>
+      <c r="G69">
+        <v>-1</v>
+      </c>
+      <c r="H69">
+        <v>1</v>
+      </c>
+      <c r="I69" s="54" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>45</v>
+      </c>
+      <c r="B70" t="s">
+        <v>10</v>
+      </c>
+      <c r="C70" t="s">
+        <v>46</v>
+      </c>
+      <c r="D70" t="s">
+        <v>62</v>
+      </c>
+      <c r="E70" t="s">
+        <v>32</v>
+      </c>
+      <c r="F70" t="s">
+        <v>31</v>
+      </c>
+      <c r="G70">
+        <v>1</v>
+      </c>
+      <c r="H70">
+        <v>1</v>
+      </c>
+      <c r="I70" s="54" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>58</v>
+      </c>
+      <c r="B71" t="s">
+        <v>59</v>
+      </c>
+      <c r="C71" t="s">
+        <v>46</v>
+      </c>
+      <c r="D71" t="s">
+        <v>62</v>
+      </c>
+      <c r="E71" t="s">
+        <v>32</v>
+      </c>
+      <c r="F71" t="s">
+        <v>31</v>
+      </c>
+      <c r="G71">
+        <v>-1</v>
+      </c>
+      <c r="H71">
+        <v>1</v>
+      </c>
+      <c r="I71" s="54" t="s">
         <v>60</v>
       </c>
     </row>
@@ -5027,8 +5389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20B783E5-A0C2-5D46-A94A-481A8E8B68D6}">
   <dimension ref="A1:Y5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="D1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5037,7 +5399,7 @@
     <col min="2" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.1640625" bestFit="1" customWidth="1"/>
@@ -5149,8 +5511,8 @@
       <c r="E2" s="14">
         <v>45382</v>
       </c>
-      <c r="F2">
-        <v>123456</v>
+      <c r="F2" s="2">
+        <v>124324091</v>
       </c>
       <c r="G2" s="2">
         <v>-1</v>
@@ -5159,10 +5521,10 @@
         <v>-1</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>82</v>
       </c>
       <c r="K2" t="s">
         <v>81</v>
@@ -5230,8 +5592,8 @@
       <c r="E3" s="14">
         <v>45397</v>
       </c>
-      <c r="F3">
-        <v>123456</v>
+      <c r="F3" s="2">
+        <v>124324091</v>
       </c>
       <c r="G3" s="2">
         <v>-1</v>
@@ -5240,10 +5602,10 @@
         <v>-1</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>82</v>
       </c>
       <c r="K3" t="s">
         <v>81</v>
@@ -5311,8 +5673,8 @@
       <c r="E4" s="14">
         <v>45430</v>
       </c>
-      <c r="F4">
-        <v>123456</v>
+      <c r="F4" s="2">
+        <v>124324091</v>
       </c>
       <c r="G4" s="2">
         <v>-1</v>
@@ -5321,10 +5683,10 @@
         <v>-1</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>82</v>
       </c>
       <c r="K4" t="s">
         <v>81</v>
@@ -5392,8 +5754,8 @@
       <c r="E5" s="14">
         <v>45450</v>
       </c>
-      <c r="F5">
-        <v>123456</v>
+      <c r="F5" s="2">
+        <v>124324091</v>
       </c>
       <c r="G5" s="2">
         <v>-1</v>
@@ -5402,10 +5764,10 @@
         <v>-1</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>82</v>
       </c>
       <c r="K5" t="s">
         <v>81</v>
@@ -5455,6 +5817,244 @@
       <c r="Y5">
         <f t="shared" si="0"/>
         <v>-52.396904918032781</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{749D5A92-E07C-E345-9059-987184A894F0}">
+  <dimension ref="A1:P4"/>
+  <sheetViews>
+    <sheetView topLeftCell="G1" zoomScale="188" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>390</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>388</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>389</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>386</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>391</v>
+      </c>
+      <c r="B2" t="s">
+        <v>395</v>
+      </c>
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="56">
+        <v>45657</v>
+      </c>
+      <c r="E2" s="57" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="G2" s="56" t="s">
+        <v>67</v>
+      </c>
+      <c r="H2" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="I2" t="s">
+        <v>385</v>
+      </c>
+      <c r="J2">
+        <v>96355</v>
+      </c>
+      <c r="K2" s="14">
+        <v>45474</v>
+      </c>
+      <c r="L2" s="14">
+        <f>+EOMONTH(K2,11)</f>
+        <v>45838</v>
+      </c>
+      <c r="M2">
+        <v>90435839</v>
+      </c>
+      <c r="N2" t="s">
+        <v>146</v>
+      </c>
+      <c r="O2" s="55">
+        <v>0.4</v>
+      </c>
+      <c r="P2" s="17">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>391</v>
+      </c>
+      <c r="B3" t="s">
+        <v>395</v>
+      </c>
+      <c r="C3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="56">
+        <v>45657</v>
+      </c>
+      <c r="E3" s="57" t="s">
+        <v>71</v>
+      </c>
+      <c r="F3" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="G3" s="56" t="s">
+        <v>67</v>
+      </c>
+      <c r="H3" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="I3" t="s">
+        <v>385</v>
+      </c>
+      <c r="J3">
+        <v>96355</v>
+      </c>
+      <c r="K3" s="14">
+        <v>45474</v>
+      </c>
+      <c r="L3" s="14">
+        <f>+EOMONTH(K3,11)</f>
+        <v>45838</v>
+      </c>
+      <c r="M3">
+        <v>80193523</v>
+      </c>
+      <c r="N3" t="s">
+        <v>146</v>
+      </c>
+      <c r="O3" s="55">
+        <v>0.6</v>
+      </c>
+      <c r="P3" s="17">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>392</v>
+      </c>
+      <c r="B4" t="s">
+        <v>395</v>
+      </c>
+      <c r="C4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="56">
+        <v>45657</v>
+      </c>
+      <c r="E4" s="57" t="s">
+        <v>71</v>
+      </c>
+      <c r="F4" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="G4" s="56" t="s">
+        <v>67</v>
+      </c>
+      <c r="H4" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="I4" t="s">
+        <v>385</v>
+      </c>
+      <c r="J4">
+        <v>93261</v>
+      </c>
+      <c r="K4" s="14">
+        <v>45474</v>
+      </c>
+      <c r="L4" s="14">
+        <f>+EOMONTH(K4,11)</f>
+        <v>45838</v>
+      </c>
+      <c r="M4">
+        <v>15143145</v>
+      </c>
+      <c r="N4" t="s">
+        <v>147</v>
+      </c>
+      <c r="O4" s="55">
+        <v>1</v>
+      </c>
+      <c r="P4" s="17">
+        <v>500000000</v>
       </c>
     </row>
   </sheetData>
@@ -5463,7 +6063,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A12977D-9D3C-784D-BA64-82A8AADC1B2E}">
   <sheetPr>
     <tabColor theme="4"/>
@@ -12282,7 +12882,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04FB4049-F651-384C-8DCF-CEAFB17703EB}">
   <sheetPr>
     <tabColor theme="4"/>
@@ -12976,7 +13576,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F7F059E-3482-9948-A0EE-3B780BE80211}">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
@@ -13117,7 +13717,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C59D3D0B-BDA7-C849-9A02-F348974FBECC}">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
@@ -13454,7 +14054,7 @@
   <dimension ref="A1:I209"/>
   <sheetViews>
     <sheetView topLeftCell="A107" zoomScale="150" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="G112" sqref="G112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -40679,8 +41279,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3AB633E-9AEE-C044-8F09-ED4F88978E4B}">
   <dimension ref="A1:T19"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -41898,8 +42498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4F93C6E-21BF-4220-AF0D-6D307F3158B8}">
   <dimension ref="A1:AB21"/>
   <sheetViews>
-    <sheetView zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView topLeftCell="F1" zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2:P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -41924,6 +42524,7 @@
     <col min="24" max="24" width="32.5" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="30" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="16.5" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="11.5" style="13"/>
   </cols>
   <sheetData>
@@ -43529,22 +44130,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8B056C4-8D76-6947-BFDD-DD6636C4305C}">
   <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:J1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16" style="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16" style="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="18.83203125" style="13" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="16" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="16" style="14" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16" style="14" customWidth="1"/>
-    <col min="17" max="18" width="18.83203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16" style="14" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16" style="14" customWidth="1"/>
     <col min="19" max="19" width="18.83203125" style="13" customWidth="1"/>
     <col min="20" max="20" width="17.5" style="17" bestFit="1" customWidth="1"/>
   </cols>
@@ -43553,56 +44154,56 @@
       <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="49" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="49" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="C1" s="49" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="5" t="s">
+      <c r="G1" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="H1" s="49" t="s">
+        <v>140</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="G1" s="49" t="s">
-        <v>140</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="I1" s="49" t="s">
-        <v>63</v>
-      </c>
-      <c r="J1" s="49" t="s">
-        <v>64</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="N1" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="N1" s="31" t="s">
+      <c r="P1" s="31" t="s">
         <v>117</v>
       </c>
-      <c r="O1" s="31" t="s">
+      <c r="Q1" s="31" t="s">
         <v>118</v>
       </c>
-      <c r="P1" s="15" t="s">
+      <c r="R1" s="15" t="s">
         <v>152</v>
-      </c>
-      <c r="Q1" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="R1" s="12" t="s">
-        <v>114</v>
       </c>
       <c r="S1" s="12" t="s">
         <v>113</v>
@@ -43615,56 +44216,56 @@
       <c r="A2" t="s">
         <v>40</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="F2">
         <v>292161</v>
       </c>
-      <c r="C2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2" s="14">
-        <f>+EDATE(E2,12)-1</f>
+      <c r="G2">
+        <v>507351248</v>
+      </c>
+      <c r="H2" t="s">
+        <v>146</v>
+      </c>
+      <c r="I2">
+        <v>0.2</v>
+      </c>
+      <c r="J2" s="14">
+        <v>45474</v>
+      </c>
+      <c r="K2" s="14">
+        <f>+EOMONTH(J2,11)</f>
         <v>45838</v>
       </c>
-      <c r="E2" s="14">
+      <c r="L2" s="13">
+        <v>47628239</v>
+      </c>
+      <c r="M2" s="18">
         <v>45474</v>
       </c>
-      <c r="F2">
-        <v>507351248</v>
-      </c>
-      <c r="G2" t="s">
-        <v>146</v>
-      </c>
-      <c r="H2">
-        <v>0.2</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="L2" s="14">
+      <c r="N2" s="14">
         <v>45474</v>
       </c>
-      <c r="M2" s="14">
-        <f>+EDATE(L2,12)-1</f>
-        <v>45838</v>
-      </c>
-      <c r="N2" s="41">
-        <v>45474</v>
-      </c>
-      <c r="O2" s="41">
+      <c r="O2" s="14">
         <f>+EDATE(N2,12)-1</f>
         <v>45838</v>
       </c>
-      <c r="Q2" s="13">
-        <v>47628239</v>
-      </c>
-      <c r="R2" s="18">
+      <c r="P2" s="41">
         <v>45474</v>
+      </c>
+      <c r="Q2" s="41">
+        <f>+EDATE(P2,12)-1</f>
+        <v>45838</v>
       </c>
       <c r="S2" s="13" t="s">
         <v>94</v>
@@ -43677,56 +44278,56 @@
       <c r="A3" t="s">
         <v>40</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="F3">
         <v>292161</v>
       </c>
-      <c r="C3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D3" s="14">
-        <f>+EDATE(E3,12)-1</f>
+      <c r="G3">
+        <v>368484453</v>
+      </c>
+      <c r="H3" t="s">
+        <v>147</v>
+      </c>
+      <c r="I3">
+        <v>0.8</v>
+      </c>
+      <c r="J3" s="14">
+        <v>45474</v>
+      </c>
+      <c r="K3" s="14">
+        <f>+EOMONTH(J3,11)</f>
         <v>45838</v>
       </c>
-      <c r="E3" s="14">
+      <c r="L3" s="13">
+        <v>47628239</v>
+      </c>
+      <c r="M3" s="18">
         <v>45474</v>
       </c>
-      <c r="F3">
-        <v>368484453</v>
-      </c>
-      <c r="G3" t="s">
-        <v>147</v>
-      </c>
-      <c r="H3">
-        <v>0.8</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="L3" s="14">
+      <c r="N3" s="14">
         <v>45474</v>
       </c>
-      <c r="M3" s="14">
-        <f>+EDATE(L3,12)-1</f>
-        <v>45838</v>
-      </c>
-      <c r="N3" s="41">
-        <v>45474</v>
-      </c>
-      <c r="O3" s="41">
+      <c r="O3" s="14">
         <f>+EDATE(N3,12)-1</f>
         <v>45838</v>
       </c>
-      <c r="Q3" s="13">
-        <v>47628239</v>
-      </c>
-      <c r="R3" s="18">
+      <c r="P3" s="41">
         <v>45474</v>
+      </c>
+      <c r="Q3" s="41">
+        <f>+EDATE(P3,12)-1</f>
+        <v>45838</v>
       </c>
       <c r="S3" s="13" t="s">
         <v>94</v>
@@ -43739,56 +44340,56 @@
       <c r="A4" t="s">
         <v>40</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="F4">
         <v>373318</v>
       </c>
-      <c r="C4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D4" s="14">
-        <f>+EDATE(E4,12)-1</f>
+      <c r="G4">
+        <v>446526767</v>
+      </c>
+      <c r="H4" t="s">
+        <v>146</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4" s="14">
+        <v>45474</v>
+      </c>
+      <c r="K4" s="14">
+        <f>+EOMONTH(J4,11)</f>
         <v>45838</v>
       </c>
-      <c r="E4" s="14">
+      <c r="L4" s="13">
+        <v>71800418</v>
+      </c>
+      <c r="M4" s="18">
         <v>45474</v>
       </c>
-      <c r="F4">
-        <v>446526767</v>
-      </c>
-      <c r="G4" t="s">
-        <v>146</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="L4" s="14">
+      <c r="N4" s="14">
         <v>45474</v>
       </c>
-      <c r="M4" s="14">
-        <f t="shared" ref="M4:M6" si="0">+EDATE(L4,12)-1</f>
+      <c r="O4" s="14">
+        <f t="shared" ref="O4:O6" si="0">+EDATE(N4,12)-1</f>
         <v>45838</v>
       </c>
-      <c r="N4" s="41">
+      <c r="P4" s="41">
         <v>45474</v>
       </c>
-      <c r="O4" s="41">
-        <f t="shared" ref="O4:O6" si="1">+EDATE(N4,12)-1</f>
+      <c r="Q4" s="41">
+        <f t="shared" ref="Q4:Q6" si="1">+EDATE(P4,12)-1</f>
         <v>45838</v>
-      </c>
-      <c r="Q4" s="13">
-        <v>71800418</v>
-      </c>
-      <c r="R4" s="18">
-        <v>45474</v>
       </c>
       <c r="S4" s="13" t="s">
         <v>94</v>
@@ -43801,56 +44402,56 @@
       <c r="A5" t="s">
         <v>40</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="F5">
         <v>867346</v>
       </c>
-      <c r="C5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D5" s="14">
-        <f>+EDATE(E5,12)-1</f>
+      <c r="G5">
+        <v>325775298</v>
+      </c>
+      <c r="H5" t="s">
+        <v>146</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5" s="14">
+        <v>45658</v>
+      </c>
+      <c r="K5" s="14">
+        <f>+EOMONTH(J5,11)</f>
         <v>46022</v>
       </c>
-      <c r="E5" s="14">
+      <c r="L5" s="13">
+        <v>45927212</v>
+      </c>
+      <c r="M5" s="18">
         <v>45658</v>
       </c>
-      <c r="F5">
-        <v>325775298</v>
-      </c>
-      <c r="G5" t="s">
-        <v>146</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="L5" s="14">
+      <c r="N5" s="14">
         <v>45658</v>
       </c>
-      <c r="M5" s="14">
+      <c r="O5" s="14">
         <f t="shared" si="0"/>
         <v>46022</v>
       </c>
-      <c r="N5" s="41">
+      <c r="P5" s="41">
         <v>45658</v>
       </c>
-      <c r="O5" s="41">
+      <c r="Q5" s="41">
         <f t="shared" si="1"/>
         <v>46022</v>
-      </c>
-      <c r="Q5" s="13">
-        <v>45927212</v>
-      </c>
-      <c r="R5" s="18">
-        <v>45658</v>
       </c>
       <c r="S5" s="13" t="s">
         <v>94</v>
@@ -43863,59 +44464,59 @@
       <c r="A6" t="s">
         <v>40</v>
       </c>
-      <c r="B6">
+      <c r="B6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="F6">
         <v>867346</v>
       </c>
-      <c r="C6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6" s="14">
-        <f>+EDATE(E6,12)-1</f>
+      <c r="G6">
+        <v>325775298</v>
+      </c>
+      <c r="H6" t="s">
+        <v>146</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6" s="14">
+        <v>45658</v>
+      </c>
+      <c r="K6" s="14">
+        <f>+EOMONTH(J6,11)</f>
         <v>46022</v>
       </c>
-      <c r="E6" s="14">
+      <c r="L6" s="13">
+        <v>45927219</v>
+      </c>
+      <c r="M6" s="18">
+        <v>45823</v>
+      </c>
+      <c r="N6" s="14">
         <v>45658</v>
       </c>
-      <c r="F6">
-        <v>360681631</v>
-      </c>
-      <c r="G6" t="s">
-        <v>146</v>
-      </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="L6" s="14">
-        <v>45658</v>
-      </c>
-      <c r="M6" s="14">
+      <c r="O6" s="14">
         <f t="shared" si="0"/>
         <v>46022</v>
       </c>
-      <c r="N6" s="41">
+      <c r="P6" s="41">
         <v>45658</v>
       </c>
-      <c r="O6" s="41">
+      <c r="Q6" s="41">
         <f t="shared" si="1"/>
         <v>46022</v>
       </c>
-      <c r="P6" s="14">
+      <c r="R6" s="14">
         <v>45811</v>
-      </c>
-      <c r="Q6" s="13">
-        <v>45927219</v>
-      </c>
-      <c r="R6" s="18">
-        <v>45823</v>
       </c>
       <c r="S6" s="13" t="s">
         <v>94</v>
@@ -43932,6 +44533,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7ab8c0d4-f18b-4fef-b649-c77d178c2495">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="65efab6e-20b9-465e-9733-f0c2ab732419" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101003456B0730C78B347BD7589BC061D6E7A" ma:contentTypeVersion="12" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="63fa1c64418ad5e2c432e8a28af753ff">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7ab8c0d4-f18b-4fef-b649-c77d178c2495" xmlns:ns3="65efab6e-20b9-465e-9733-f0c2ab732419" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0084d3678d80c20d937c1596fa80271a" ns2:_="" ns3:_="">
     <xsd:import namespace="7ab8c0d4-f18b-4fef-b649-c77d178c2495"/>
@@ -44132,7 +44744,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -44141,18 +44753,24 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7ab8c0d4-f18b-4fef-b649-c77d178c2495">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="65efab6e-20b9-465e-9733-f0c2ab732419" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE50E33B-922F-4D33-8831-2DF5BA7F11F6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="7ab8c0d4-f18b-4fef-b649-c77d178c2495"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="65efab6e-20b9-465e-9733-f0c2ab732419"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{215DDC88-1A19-494F-B8DF-0B0259427CE0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -44171,27 +44789,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C685BDB-1785-4A39-A308-4CA166889A49}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE50E33B-922F-4D33-8831-2DF5BA7F11F6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="7ab8c0d4-f18b-4fef-b649-c77d178c2495"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="65efab6e-20b9-465e-9733-f0c2ab732419"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Cambiar anio_liberacion a no_aplica para constituciones
</commit_message>
<xml_diff>
--- a/prototipo_pcr/inputs/insumos.xlsx
+++ b/prototipo_pcr/inputs/insumos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebatoec/Library/CloudStorage/OneDrive-SharedLibraries-SegurosSuramericana,S.A/Proyecto féniX - féniX/01 IFRS17/02 Entregables Procesos/05 Reservas/03 PCR CP/03 Tecnología/01 Prototipo/prototipo_pcr/inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://suramericana.sharepoint.com/sites/TraNIFF/Shared Documents/féniX/01 IFRS17/02 Entregables Procesos/05 Reservas/03 PCR CP/03 Tecnología/01 Prototipo/prototipo_pcr/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD28944F-9393-4D4A-B4A3-509D2DD14883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{2C5D209E-47BE-3B4E-8690-75A33B496FD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{614DE68D-695B-6D46-9143-7DF64612FECB}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17420" tabRatio="959" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17420" tabRatio="959" firstSheet="7" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="param_contabilidad" sheetId="6" r:id="rId1"/>
@@ -39,7 +39,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">produccion_rea!$A$1:$Z$10</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">tipo_seguro!$A$1:$C$61</definedName>
   </definedNames>
-  <calcPr calcId="191028" iterate="1"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2565,8 +2565,8 @@
   </sheetPr>
   <dimension ref="A1:J80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3322,7 +3322,7 @@
         <v>383</v>
       </c>
       <c r="B24" t="s">
-        <v>383</v>
+        <v>35</v>
       </c>
       <c r="C24" t="s">
         <v>392</v>
@@ -3354,7 +3354,7 @@
         <v>383</v>
       </c>
       <c r="B25" t="s">
-        <v>383</v>
+        <v>35</v>
       </c>
       <c r="C25" t="s">
         <v>392</v>
@@ -3386,7 +3386,7 @@
         <v>383</v>
       </c>
       <c r="B26" t="s">
-        <v>383</v>
+        <v>35</v>
       </c>
       <c r="C26" t="s">
         <v>392</v>
@@ -3418,7 +3418,7 @@
         <v>384</v>
       </c>
       <c r="B27" t="s">
-        <v>384</v>
+        <v>35</v>
       </c>
       <c r="C27" t="s">
         <v>392</v>
@@ -3450,7 +3450,7 @@
         <v>384</v>
       </c>
       <c r="B28" t="s">
-        <v>384</v>
+        <v>35</v>
       </c>
       <c r="C28" t="s">
         <v>392</v>
@@ -3482,7 +3482,7 @@
         <v>384</v>
       </c>
       <c r="B29" t="s">
-        <v>384</v>
+        <v>35</v>
       </c>
       <c r="C29" t="s">
         <v>392</v>
@@ -3930,7 +3930,7 @@
         <v>383</v>
       </c>
       <c r="B43" t="s">
-        <v>383</v>
+        <v>35</v>
       </c>
       <c r="C43" t="s">
         <v>392</v>
@@ -3962,7 +3962,7 @@
         <v>383</v>
       </c>
       <c r="B44" t="s">
-        <v>383</v>
+        <v>35</v>
       </c>
       <c r="C44" t="s">
         <v>392</v>
@@ -3994,7 +3994,7 @@
         <v>383</v>
       </c>
       <c r="B45" t="s">
-        <v>383</v>
+        <v>35</v>
       </c>
       <c r="C45" t="s">
         <v>392</v>
@@ -4026,7 +4026,7 @@
         <v>384</v>
       </c>
       <c r="B46" t="s">
-        <v>384</v>
+        <v>35</v>
       </c>
       <c r="C46" t="s">
         <v>392</v>
@@ -4058,7 +4058,7 @@
         <v>384</v>
       </c>
       <c r="B47" t="s">
-        <v>384</v>
+        <v>35</v>
       </c>
       <c r="C47" t="s">
         <v>392</v>
@@ -4090,7 +4090,7 @@
         <v>384</v>
       </c>
       <c r="B48" t="s">
-        <v>384</v>
+        <v>35</v>
       </c>
       <c r="C48" t="s">
         <v>392</v>
@@ -4538,7 +4538,7 @@
         <v>383</v>
       </c>
       <c r="B62" t="s">
-        <v>383</v>
+        <v>35</v>
       </c>
       <c r="C62" t="s">
         <v>392</v>
@@ -4570,7 +4570,7 @@
         <v>383</v>
       </c>
       <c r="B63" t="s">
-        <v>383</v>
+        <v>35</v>
       </c>
       <c r="C63" t="s">
         <v>392</v>
@@ -4602,7 +4602,7 @@
         <v>383</v>
       </c>
       <c r="B64" t="s">
-        <v>383</v>
+        <v>35</v>
       </c>
       <c r="C64" t="s">
         <v>392</v>
@@ -4634,7 +4634,7 @@
         <v>384</v>
       </c>
       <c r="B65" t="s">
-        <v>384</v>
+        <v>35</v>
       </c>
       <c r="C65" t="s">
         <v>392</v>
@@ -4666,7 +4666,7 @@
         <v>384</v>
       </c>
       <c r="B66" t="s">
-        <v>384</v>
+        <v>35</v>
       </c>
       <c r="C66" t="s">
         <v>392</v>
@@ -4698,7 +4698,7 @@
         <v>384</v>
       </c>
       <c r="B67" t="s">
-        <v>384</v>
+        <v>35</v>
       </c>
       <c r="C67" t="s">
         <v>392</v>
@@ -14321,8 +14321,8 @@
   </sheetPr>
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14333,8 +14333,8 @@
     <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.1640625" customWidth="1"/>
     <col min="10" max="10" width="8.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.1640625" bestFit="1" customWidth="1"/>
@@ -45380,16 +45380,16 @@
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE50E33B-922F-4D33-8831-2DF5BA7F11F6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="7ab8c0d4-f18b-4fef-b649-c77d178c2495"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="65efab6e-20b9-465e-9733-f0c2ab732419"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="7ab8c0d4-f18b-4fef-b649-c77d178c2495"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Corregir devengo recuperacion onerosidad NP
</commit_message>
<xml_diff>
--- a/prototipo_pcr/inputs/insumos.xlsx
+++ b/prototipo_pcr/inputs/insumos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://suramericana.sharepoint.com/sites/TraNIFF/Shared Documents/féniX/01 IFRS17/02 Entregables Procesos/05 Reservas/03 PCR CP/03 Tecnología/01 Prototipo/prototipo_pcr/inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebatoec/Library/CloudStorage/OneDrive-SharedLibraries-SegurosSuramericana,S.A/Proyecto féniX - féniX/01 IFRS17/02 Entregables Procesos/05 Reservas/03 PCR CP/03 Tecnología/01 Prototipo/prototipo_pcr/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{2C5D209E-47BE-3B4E-8690-75A33B496FD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{614DE68D-695B-6D46-9143-7DF64612FECB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00586EC5-CB98-5846-803B-E7F2D3147B8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17420" tabRatio="959" firstSheet="7" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17420" tabRatio="959" firstSheet="7" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="param_contabilidad" sheetId="6" r:id="rId1"/>
@@ -768,7 +768,7 @@
     <author>Priscilla Andrea Palacios Ruiz</author>
   </authors>
   <commentList>
-    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{4528A10A-A994-8442-A047-E7A1AE24EFF8}">
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{4528A10A-A994-8442-A047-E7A1AE24EFF8}">
       <text>
         <r>
           <rPr>
@@ -786,7 +786,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7579" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7583" uniqueCount="393">
   <si>
     <t>tipo_insumo</t>
   </si>
@@ -6438,10 +6438,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{749D5A92-E07C-E345-9059-987184A894F0}">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScale="188" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="188" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6460,10 +6460,11 @@
     <col min="12" max="12" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="27.1640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>108</v>
       </c>
@@ -6507,10 +6508,13 @@
         <v>138</v>
       </c>
       <c r="O1" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="P1" s="5" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>381</v>
       </c>
@@ -6554,11 +6558,14 @@
       <c r="N2" s="55">
         <v>0.4</v>
       </c>
-      <c r="O2" s="17">
+      <c r="O2" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="P2" s="17">
         <v>1000000000</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>381</v>
       </c>
@@ -6602,11 +6609,14 @@
       <c r="N3" s="55">
         <v>0.6</v>
       </c>
-      <c r="O3" s="17">
+      <c r="O3" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="P3" s="17">
         <v>1000000000</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>382</v>
       </c>
@@ -6650,7 +6660,10 @@
       <c r="N4" s="55">
         <v>1</v>
       </c>
-      <c r="O4" s="17">
+      <c r="O4" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="P4" s="17">
         <v>500000000</v>
       </c>
     </row>
@@ -14321,7 +14334,7 @@
   </sheetPr>
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
@@ -45130,12 +45143,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7ab8c0d4-f18b-4fef-b649-c77d178c2495">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="65efab6e-20b9-465e-9733-f0c2ab732419" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -45340,20 +45355,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7ab8c0d4-f18b-4fef-b649-c77d178c2495">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="65efab6e-20b9-465e-9733-f0c2ab732419" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C685BDB-1785-4A39-A308-4CA166889A49}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE50E33B-922F-4D33-8831-2DF5BA7F11F6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="65efab6e-20b9-465e-9733-f0c2ab732419"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="7ab8c0d4-f18b-4fef-b649-c77d178c2495"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -45378,18 +45400,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE50E33B-922F-4D33-8831-2DF5BA7F11F6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C685BDB-1785-4A39-A308-4CA166889A49}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="65efab6e-20b9-465e-9733-f0c2ab732419"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="7ab8c0d4-f18b-4fef-b649-c77d178c2495"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Agregar nueva BT de PPR para terremoto
</commit_message>
<xml_diff>
--- a/prototipo_pcr/inputs/insumos.xlsx
+++ b/prototipo_pcr/inputs/insumos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebatoec/Library/CloudStorage/OneDrive-SharedLibraries-SegurosSuramericana,S.A/Proyecto féniX - féniX/01 IFRS17/02 Entregables Procesos/05 Reservas/03 PCR CP/03 Tecnología/01 Prototipo/prototipo_pcr/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00586EC5-CB98-5846-803B-E7F2D3147B8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C58AFE32-A100-4844-97D2-829CB81F64C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17420" tabRatio="959" firstSheet="7" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17420" tabRatio="959" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="param_contabilidad" sheetId="6" r:id="rId1"/>
@@ -2565,8 +2565,8 @@
   </sheetPr>
   <dimension ref="A1:J80"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3005,7 +3005,7 @@
         <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>392</v>
       </c>
       <c r="D14" t="s">
         <v>11</v>
@@ -3037,7 +3037,7 @@
         <v>32</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>392</v>
       </c>
       <c r="D15" t="s">
         <v>11</v>
@@ -3069,7 +3069,7 @@
         <v>30</v>
       </c>
       <c r="C16" t="s">
-        <v>30</v>
+        <v>392</v>
       </c>
       <c r="D16" t="s">
         <v>11</v>
@@ -3101,7 +3101,7 @@
         <v>32</v>
       </c>
       <c r="C17" t="s">
-        <v>32</v>
+        <v>392</v>
       </c>
       <c r="D17" t="s">
         <v>11</v>
@@ -6440,7 +6440,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{749D5A92-E07C-E345-9059-987184A894F0}">
   <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="188" workbookViewId="0">
+    <sheetView topLeftCell="K1" zoomScale="188" workbookViewId="0">
       <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
@@ -45143,14 +45143,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7ab8c0d4-f18b-4fef-b649-c77d178c2495">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="65efab6e-20b9-465e-9733-f0c2ab732419" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -45355,27 +45353,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7ab8c0d4-f18b-4fef-b649-c77d178c2495">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="65efab6e-20b9-465e-9733-f0c2ab732419" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE50E33B-922F-4D33-8831-2DF5BA7F11F6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C685BDB-1785-4A39-A308-4CA166889A49}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="65efab6e-20b9-465e-9733-f0c2ab732419"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="7ab8c0d4-f18b-4fef-b649-c77d178c2495"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -45400,9 +45391,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C685BDB-1785-4A39-A308-4CA166889A49}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE50E33B-922F-4D33-8831-2DF5BA7F11F6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="65efab6e-20b9-465e-9733-f0c2ab732419"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="7ab8c0d4-f18b-4fef-b649-c77d178c2495"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Agregar casuistica de PCR que se contabiliza como RMAT en NIIF4
</commit_message>
<xml_diff>
--- a/prototipo_pcr/inputs/insumos.xlsx
+++ b/prototipo_pcr/inputs/insumos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebatoec/Library/CloudStorage/OneDrive-SharedLibraries-SegurosSuramericana,S.A/Proyecto féniX - féniX/01 IFRS17/02 Entregables Procesos/05 Reservas/03 PCR CP/03 Tecnología/01 Prototipo/prototipo_pcr/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C58AFE32-A100-4844-97D2-829CB81F64C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A61D9D-B307-6C4C-BABE-E4CCFD27DBFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17420" tabRatio="959" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">comision_rea!$A$1:$V$9</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">map_bt!$A$1:$I$261</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">param_contabilidad!$A$1:$J$80</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">param_contabilidad!$A$1:$J$83</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">porc_descuento!$A$1:$K$17</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">produccion_directo!$A$1:$T$18</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">produccion_rea!$A$1:$Z$10</definedName>
@@ -63,6 +63,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Priscilla Andrea Palacios Ruiz</author>
+    <author>Sebatian Tobon Echavarría</author>
   </authors>
   <commentList>
     <comment ref="E1" authorId="0" shapeId="0" xr:uid="{E0C48D36-D894-244B-B7C4-97A8DFD467D1}">
@@ -108,7 +109,106 @@
         </r>
       </text>
     </comment>
-    <comment ref="G27" authorId="0" shapeId="0" xr:uid="{E59A34B5-D270-2F42-B52A-76C0C15E87D1}">
+    <comment ref="A21" authorId="1" shapeId="0" xr:uid="{00118428-2633-E248-924C-CAEC15BB77E2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sebatian Tobon Echavarría:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>No tiene componentes de descuento comercial porque no se rige por la norma de la PCR en NIIF4</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A22" authorId="1" shapeId="0" xr:uid="{0BCCDF6A-AF2F-BF43-ACC4-B11CDF3BF7E7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sebatian Tobon Echavarría:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>No tiene componentes de descuento comercial porque no se rige por la norma de la PCR en NIIF4</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A23" authorId="1" shapeId="0" xr:uid="{9F84EA09-0C86-6E40-8241-5BA37E843C3A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sebatian Tobon Echavarría:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>No tiene componentes de descuento comercial porque no se rige por la norma de la PCR en NIIF4</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G30" authorId="0" shapeId="0" xr:uid="{E59A34B5-D270-2F42-B52A-76C0C15E87D1}">
       <text>
         <r>
           <rPr>
@@ -121,7 +221,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G28" authorId="0" shapeId="0" xr:uid="{60704782-0207-754E-8C3D-579B8D19FB81}">
+    <comment ref="G31" authorId="0" shapeId="0" xr:uid="{60704782-0207-754E-8C3D-579B8D19FB81}">
       <text>
         <r>
           <rPr>
@@ -134,7 +234,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G29" authorId="0" shapeId="0" xr:uid="{79E1C198-5A7C-3E4A-B967-D774BDD95BB9}">
+    <comment ref="G32" authorId="0" shapeId="0" xr:uid="{79E1C198-5A7C-3E4A-B967-D774BDD95BB9}">
       <text>
         <r>
           <rPr>
@@ -147,7 +247,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G30" authorId="0" shapeId="0" xr:uid="{E2EB6F16-7DC2-B547-9D29-6287117B6B6D}">
+    <comment ref="G33" authorId="0" shapeId="0" xr:uid="{E2EB6F16-7DC2-B547-9D29-6287117B6B6D}">
       <text>
         <r>
           <rPr>
@@ -160,7 +260,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G31" authorId="0" shapeId="0" xr:uid="{CADF5D80-B324-BD4D-83EF-7103C7C4BCDC}">
+    <comment ref="G34" authorId="0" shapeId="0" xr:uid="{CADF5D80-B324-BD4D-83EF-7103C7C4BCDC}">
       <text>
         <r>
           <rPr>
@@ -173,8 +273,18 @@
         </r>
       </text>
     </comment>
-    <comment ref="G46" authorId="0" shapeId="0" xr:uid="{2F8A8F21-AF4A-114C-A2D9-75E8451135A5}">
+    <comment ref="A46" authorId="1" shapeId="0" xr:uid="{A584AB8F-D4EA-F440-A6C6-268A2F359AEC}">
       <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sebatian Tobon Echavarría:</t>
+        </r>
         <r>
           <rPr>
             <sz val="10"/>
@@ -182,12 +292,9 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>aquí cobertura no tiene tanto sentido</t>
+          <t xml:space="preserve">
+</t>
         </r>
-      </text>
-    </comment>
-    <comment ref="G47" authorId="0" shapeId="0" xr:uid="{AA1C8E44-739E-684B-937A-F6E67147AA09}">
-      <text>
         <r>
           <rPr>
             <sz val="10"/>
@@ -195,12 +302,22 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>aquí cobertura no tiene tanto sentido</t>
+          <t>No tiene componentes de descuento comercial porque no se rige por la norma de la PCR en NIIF4</t>
         </r>
       </text>
     </comment>
-    <comment ref="G48" authorId="0" shapeId="0" xr:uid="{1C501671-D027-4748-85A0-62782DC8D7C1}">
+    <comment ref="A47" authorId="1" shapeId="0" xr:uid="{E8392D49-751D-5148-AF1A-838F2A8CBC22}">
       <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sebatian Tobon Echavarría:</t>
+        </r>
         <r>
           <rPr>
             <sz val="10"/>
@@ -208,7 +325,50 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>aquí cobertura no tiene tanto sentido</t>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>No tiene componentes de descuento comercial porque no se rige por la norma de la PCR en NIIF4</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A48" authorId="1" shapeId="0" xr:uid="{FAB79EAC-9640-B243-A698-E5D5A4CE0B1D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sebatian Tobon Echavarría:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>No tiene componentes de descuento comercial porque no se rige por la norma de la PCR en NIIF4</t>
         </r>
       </text>
     </comment>
@@ -300,6 +460,105 @@
             <family val="2"/>
           </rPr>
           <t>aquí cobertura no tiene tanto sentido</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A81" authorId="1" shapeId="0" xr:uid="{CE13C260-1EB1-214D-B033-67177BE55852}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sebatian Tobon Echavarría:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>No tiene componentes de descuento comercial porque no se rige por la norma de la PCR en NIIF4</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A82" authorId="1" shapeId="0" xr:uid="{6A0CBB84-2976-6E44-91CD-A5D7D3F3E33E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sebatian Tobon Echavarría:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>No tiene componentes de descuento comercial porque no se rige por la norma de la PCR en NIIF4</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A83" authorId="1" shapeId="0" xr:uid="{D99704EE-3529-2545-979F-75AB1B52743F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sebatian Tobon Echavarría:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>No tiene componentes de descuento comercial porque no se rige por la norma de la PCR en NIIF4</t>
         </r>
       </text>
     </comment>
@@ -786,7 +1045,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7583" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7628" uniqueCount="400">
   <si>
     <t>tipo_insumo</t>
   </si>
@@ -1966,6 +2225,27 @@
   <si>
     <t>reserva</t>
   </si>
+  <si>
+    <t>matematica</t>
+  </si>
+  <si>
+    <t>matematica_niif4_directo</t>
+  </si>
+  <si>
+    <t>matematica_niif4_reaseguro</t>
+  </si>
+  <si>
+    <t>componente de prima del 092 y 095 que se calcula como PCR pero se contabiliza como RMAT</t>
+  </si>
+  <si>
+    <t>componente de gasto de expedición diferente de comisiones del 092 y 095 que se calcula como PCR pero se contabiliza como RMAT</t>
+  </si>
+  <si>
+    <t>componente de gasto de expedición por comisiones del 092 y 095 que se calcula como PCR pero se contabiliza como RMAT</t>
+  </si>
+  <si>
+    <t>SCP</t>
+  </si>
 </sst>
 </file>
 
@@ -2171,7 +2451,7 @@
     <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2242,6 +2522,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Millares [0]" xfId="2" builtinId="6"/>
@@ -2250,7 +2531,17 @@
     <cellStyle name="Normal 2" xfId="4" xr:uid="{E9C85521-AE54-9B43-8377-75044D8DBD3C}"/>
     <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2563,15 +2854,15 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:J80"/>
+  <dimension ref="A1:K83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="26.5" customWidth="1"/>
     <col min="4" max="4" width="22.1640625" customWidth="1"/>
     <col min="5" max="5" width="21" customWidth="1"/>
@@ -2581,7 +2872,7 @@
     <col min="10" max="10" width="106.5" style="54" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2613,7 +2904,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -2645,7 +2936,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -2674,10 +2965,10 @@
         <v>1</v>
       </c>
       <c r="J3" s="54" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -2706,10 +2997,11 @@
         <v>1</v>
       </c>
       <c r="J4" s="54" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+      <c r="K4" s="54"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -2741,7 +3033,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -2773,7 +3065,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -2805,7 +3097,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -2837,7 +3129,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -2869,7 +3161,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -2901,7 +3193,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -2933,7 +3225,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -2965,7 +3257,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -2997,7 +3289,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -3029,7 +3321,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -3061,7 +3353,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -3093,7 +3385,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -3125,7 +3417,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -3157,7 +3449,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -3189,7 +3481,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -3221,15 +3513,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>35</v>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="30" t="s">
+        <v>394</v>
       </c>
       <c r="B21" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="C21" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="D21" t="s">
         <v>11</v>
@@ -3250,18 +3542,18 @@
         <v>1</v>
       </c>
       <c r="J21" s="54" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>35</v>
+        <v>396</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="30" t="s">
+        <v>394</v>
       </c>
       <c r="B22" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="C22" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="D22" t="s">
         <v>11</v>
@@ -3270,30 +3562,31 @@
         <v>11</v>
       </c>
       <c r="F22" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="G22" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="H22">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="I22">
         <v>1</v>
       </c>
       <c r="J22" s="54" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>35</v>
+        <v>398</v>
+      </c>
+      <c r="K22" s="54"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="30" t="s">
+        <v>394</v>
       </c>
       <c r="B23" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="C23" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="D23" t="s">
         <v>11</v>
@@ -3302,24 +3595,24 @@
         <v>11</v>
       </c>
       <c r="F23" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="G23" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="H23">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="I23">
         <v>1</v>
       </c>
       <c r="J23" s="54" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>383</v>
+        <v>35</v>
       </c>
       <c r="B24" t="s">
         <v>35</v>
@@ -3328,10 +3621,10 @@
         <v>392</v>
       </c>
       <c r="D24" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="E24" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="F24" t="s">
         <v>12</v>
@@ -3340,18 +3633,18 @@
         <v>13</v>
       </c>
       <c r="H24">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="I24">
         <v>1</v>
       </c>
       <c r="J24" s="54" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>383</v>
+        <v>35</v>
       </c>
       <c r="B25" t="s">
         <v>35</v>
@@ -3360,10 +3653,10 @@
         <v>392</v>
       </c>
       <c r="D25" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="E25" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="F25" t="s">
         <v>27</v>
@@ -3372,18 +3665,18 @@
         <v>28</v>
       </c>
       <c r="H25">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="I25">
         <v>1</v>
       </c>
       <c r="J25" s="54" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>383</v>
+        <v>35</v>
       </c>
       <c r="B26" t="s">
         <v>35</v>
@@ -3392,10 +3685,10 @@
         <v>392</v>
       </c>
       <c r="D26" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="E26" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="F26" t="s">
         <v>29</v>
@@ -3404,18 +3697,18 @@
         <v>28</v>
       </c>
       <c r="H26">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="I26">
         <v>1</v>
       </c>
       <c r="J26" s="54" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B27" t="s">
         <v>35</v>
@@ -3424,7 +3717,7 @@
         <v>392</v>
       </c>
       <c r="D27" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E27" t="s">
         <v>40</v>
@@ -3432,7 +3725,7 @@
       <c r="F27" t="s">
         <v>12</v>
       </c>
-      <c r="G27" s="30" t="s">
+      <c r="G27" t="s">
         <v>13</v>
       </c>
       <c r="H27">
@@ -3442,12 +3735,12 @@
         <v>1</v>
       </c>
       <c r="J27" s="54" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B28" t="s">
         <v>35</v>
@@ -3456,7 +3749,7 @@
         <v>392</v>
       </c>
       <c r="D28" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E28" t="s">
         <v>40</v>
@@ -3464,8 +3757,8 @@
       <c r="F28" t="s">
         <v>27</v>
       </c>
-      <c r="G28" s="30" t="s">
-        <v>13</v>
+      <c r="G28" t="s">
+        <v>28</v>
       </c>
       <c r="H28">
         <v>1</v>
@@ -3474,12 +3767,12 @@
         <v>1</v>
       </c>
       <c r="J28" s="54" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B29" t="s">
         <v>35</v>
@@ -3488,7 +3781,7 @@
         <v>392</v>
       </c>
       <c r="D29" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E29" t="s">
         <v>40</v>
@@ -3496,8 +3789,8 @@
       <c r="F29" t="s">
         <v>29</v>
       </c>
-      <c r="G29" s="30" t="s">
-        <v>13</v>
+      <c r="G29" t="s">
+        <v>28</v>
       </c>
       <c r="H29">
         <v>1</v>
@@ -3506,15 +3799,15 @@
         <v>1</v>
       </c>
       <c r="J29" s="54" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>37</v>
+        <v>384</v>
       </c>
       <c r="B30" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="C30" t="s">
         <v>392</v>
@@ -3526,7 +3819,7 @@
         <v>40</v>
       </c>
       <c r="F30" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="G30" s="30" t="s">
         <v>13</v>
@@ -3538,15 +3831,15 @@
         <v>1</v>
       </c>
       <c r="J30" s="54" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>37</v>
+        <v>384</v>
       </c>
       <c r="B31" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="C31" t="s">
         <v>392</v>
@@ -3558,7 +3851,7 @@
         <v>40</v>
       </c>
       <c r="F31" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G31" s="30" t="s">
         <v>13</v>
@@ -3570,29 +3863,29 @@
         <v>1</v>
       </c>
       <c r="J31" s="54" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>42</v>
+        <v>384</v>
       </c>
       <c r="B32" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="C32" t="s">
         <v>392</v>
       </c>
       <c r="D32" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E32" t="s">
         <v>40</v>
       </c>
       <c r="F32" t="s">
-        <v>12</v>
-      </c>
-      <c r="G32" t="s">
+        <v>29</v>
+      </c>
+      <c r="G32" s="30" t="s">
         <v>13</v>
       </c>
       <c r="H32">
@@ -3602,29 +3895,29 @@
         <v>1</v>
       </c>
       <c r="J32" s="54" t="s">
-        <v>44</v>
+        <v>386</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B33" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C33" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D33" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E33" t="s">
         <v>40</v>
       </c>
       <c r="F33" t="s">
-        <v>12</v>
-      </c>
-      <c r="G33" t="s">
+        <v>27</v>
+      </c>
+      <c r="G33" s="30" t="s">
         <v>13</v>
       </c>
       <c r="H33">
@@ -3634,29 +3927,29 @@
         <v>1</v>
       </c>
       <c r="J33" s="54" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B34" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C34" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E34" t="s">
         <v>40</v>
       </c>
       <c r="F34" t="s">
-        <v>12</v>
-      </c>
-      <c r="G34" t="s">
+        <v>29</v>
+      </c>
+      <c r="G34" s="30" t="s">
         <v>13</v>
       </c>
       <c r="H34">
@@ -3666,18 +3959,18 @@
         <v>1</v>
       </c>
       <c r="J34" s="54" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B35" t="s">
         <v>10</v>
       </c>
       <c r="C35" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="D35" t="s">
         <v>43</v>
@@ -3692,24 +3985,24 @@
         <v>13</v>
       </c>
       <c r="H35">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="I35">
         <v>1</v>
       </c>
       <c r="J35" s="54" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B36" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C36" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="D36" t="s">
         <v>43</v>
@@ -3724,24 +4017,24 @@
         <v>13</v>
       </c>
       <c r="H36">
+        <v>-1</v>
+      </c>
+      <c r="I36">
         <v>1</v>
       </c>
-      <c r="I36">
-        <v>0</v>
-      </c>
       <c r="J36" s="54" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B37" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C37" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="D37" t="s">
         <v>43</v>
@@ -3756,24 +4049,24 @@
         <v>13</v>
       </c>
       <c r="H37">
+        <v>-1</v>
+      </c>
+      <c r="I37">
         <v>1</v>
       </c>
-      <c r="I37">
-        <v>0</v>
-      </c>
       <c r="J37" s="54" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B38" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="C38" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D38" t="s">
         <v>43</v>
@@ -3788,24 +4081,24 @@
         <v>13</v>
       </c>
       <c r="H38">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="I38">
         <v>1</v>
       </c>
       <c r="J38" s="54" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="B39" t="s">
         <v>10</v>
       </c>
       <c r="C39" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D39" t="s">
         <v>43</v>
@@ -3814,30 +4107,30 @@
         <v>40</v>
       </c>
       <c r="F39" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="G39" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="H39">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="I39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J39" s="54" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B40" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="C40" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D40" t="s">
         <v>43</v>
@@ -3846,27 +4139,27 @@
         <v>40</v>
       </c>
       <c r="F40" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="G40" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="H40">
         <v>-1</v>
       </c>
       <c r="I40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J40" s="54" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="B41" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="C41" t="s">
         <v>392</v>
@@ -3878,27 +4171,27 @@
         <v>40</v>
       </c>
       <c r="F41" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="G41" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="H41">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="I41">
         <v>1</v>
       </c>
       <c r="J41" s="54" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="C42" t="s">
         <v>392</v>
@@ -3910,27 +4203,27 @@
         <v>40</v>
       </c>
       <c r="F42" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G42" t="s">
         <v>28</v>
       </c>
       <c r="H42">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="I42">
         <v>1</v>
       </c>
       <c r="J42" s="54" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>383</v>
+        <v>55</v>
       </c>
       <c r="B43" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="C43" t="s">
         <v>392</v>
@@ -3939,30 +4232,30 @@
         <v>43</v>
       </c>
       <c r="E43" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="F43" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="G43" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="H43">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="I43">
         <v>1</v>
       </c>
       <c r="J43" s="54" t="s">
-        <v>385</v>
+        <v>57</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>383</v>
+        <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="C44" t="s">
         <v>392</v>
@@ -3971,10 +4264,10 @@
         <v>43</v>
       </c>
       <c r="E44" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="F44" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G44" t="s">
         <v>28</v>
@@ -3986,15 +4279,15 @@
         <v>1</v>
       </c>
       <c r="J44" s="54" t="s">
-        <v>385</v>
+        <v>44</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>383</v>
+        <v>55</v>
       </c>
       <c r="B45" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="C45" t="s">
         <v>392</v>
@@ -4003,7 +4296,7 @@
         <v>43</v>
       </c>
       <c r="E45" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="F45" t="s">
         <v>29</v>
@@ -4012,35 +4305,35 @@
         <v>28</v>
       </c>
       <c r="H45">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="I45">
         <v>1</v>
       </c>
       <c r="J45" s="54" t="s">
-        <v>385</v>
+        <v>57</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>384</v>
+      <c r="A46" s="30" t="s">
+        <v>395</v>
       </c>
       <c r="B46" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="C46" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="D46" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E46" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="F46" t="s">
         <v>12</v>
       </c>
-      <c r="G46" s="30" t="s">
+      <c r="G46" t="s">
         <v>13</v>
       </c>
       <c r="H46">
@@ -4050,71 +4343,71 @@
         <v>1</v>
       </c>
       <c r="J46" s="54" t="s">
-        <v>386</v>
+        <v>396</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>384</v>
+      <c r="A47" s="30" t="s">
+        <v>395</v>
       </c>
       <c r="B47" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="C47" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="D47" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E47" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="F47" t="s">
-        <v>27</v>
-      </c>
-      <c r="G47" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="G47" t="s">
         <v>13</v>
       </c>
       <c r="H47">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="I47">
         <v>1</v>
       </c>
       <c r="J47" s="54" t="s">
-        <v>386</v>
+        <v>398</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>384</v>
+      <c r="A48" s="30" t="s">
+        <v>395</v>
       </c>
       <c r="B48" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="C48" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="D48" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E48" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="F48" t="s">
-        <v>29</v>
-      </c>
-      <c r="G48" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="G48" t="s">
         <v>13</v>
       </c>
       <c r="H48">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="I48">
         <v>1</v>
       </c>
       <c r="J48" s="54" t="s">
-        <v>386</v>
+        <v>397</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
@@ -4236,7 +4529,7 @@
         <v>13</v>
       </c>
       <c r="H52">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="I52">
         <v>1</v>
@@ -4268,7 +4561,7 @@
         <v>13</v>
       </c>
       <c r="H53">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="I53">
         <v>1</v>
@@ -4300,7 +4593,7 @@
         <v>13</v>
       </c>
       <c r="H54">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="I54">
         <v>1</v>
@@ -4332,7 +4625,7 @@
         <v>13</v>
       </c>
       <c r="H55">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="I55">
         <v>0</v>
@@ -4364,7 +4657,7 @@
         <v>13</v>
       </c>
       <c r="H56">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="I56">
         <v>0</v>
@@ -4844,7 +5137,7 @@
         <v>13</v>
       </c>
       <c r="H71">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="I71">
         <v>1</v>
@@ -4876,7 +5169,7 @@
         <v>13</v>
       </c>
       <c r="H72">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="I72">
         <v>1</v>
@@ -4908,7 +5201,7 @@
         <v>13</v>
       </c>
       <c r="H73">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="I73">
         <v>1</v>
@@ -4940,7 +5233,7 @@
         <v>13</v>
       </c>
       <c r="H74">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="I74">
         <v>0</v>
@@ -4972,7 +5265,7 @@
         <v>13</v>
       </c>
       <c r="H75">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="I75">
         <v>0</v>
@@ -5141,8 +5434,104 @@
         <v>57</v>
       </c>
     </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A81" s="30" t="s">
+        <v>395</v>
+      </c>
+      <c r="B81" t="s">
+        <v>10</v>
+      </c>
+      <c r="C81" t="s">
+        <v>393</v>
+      </c>
+      <c r="D81" t="s">
+        <v>43</v>
+      </c>
+      <c r="E81" t="s">
+        <v>59</v>
+      </c>
+      <c r="F81" t="s">
+        <v>12</v>
+      </c>
+      <c r="G81" t="s">
+        <v>13</v>
+      </c>
+      <c r="H81">
+        <v>1</v>
+      </c>
+      <c r="I81">
+        <v>1</v>
+      </c>
+      <c r="J81" s="54" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A82" s="30" t="s">
+        <v>395</v>
+      </c>
+      <c r="B82" t="s">
+        <v>16</v>
+      </c>
+      <c r="C82" t="s">
+        <v>393</v>
+      </c>
+      <c r="D82" t="s">
+        <v>43</v>
+      </c>
+      <c r="E82" t="s">
+        <v>59</v>
+      </c>
+      <c r="F82" t="s">
+        <v>12</v>
+      </c>
+      <c r="G82" t="s">
+        <v>13</v>
+      </c>
+      <c r="H82">
+        <v>-1</v>
+      </c>
+      <c r="I82">
+        <v>1</v>
+      </c>
+      <c r="J82" s="54" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A83" s="30" t="s">
+        <v>395</v>
+      </c>
+      <c r="B83" t="s">
+        <v>19</v>
+      </c>
+      <c r="C83" t="s">
+        <v>393</v>
+      </c>
+      <c r="D83" t="s">
+        <v>43</v>
+      </c>
+      <c r="E83" t="s">
+        <v>59</v>
+      </c>
+      <c r="F83" t="s">
+        <v>12</v>
+      </c>
+      <c r="G83" t="s">
+        <v>13</v>
+      </c>
+      <c r="H83">
+        <v>-1</v>
+      </c>
+      <c r="I83">
+        <v>1</v>
+      </c>
+      <c r="J83" s="54" t="s">
+        <v>397</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J80" xr:uid="{7838926A-4835-1A4C-A577-1C02FA1EB720}"/>
+  <autoFilter ref="A1:J83" xr:uid="{7838926A-4835-1A4C-A577-1C02FA1EB720}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
@@ -41887,10 +42276,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3AB633E-9AEE-C044-8F09-ED4F88978E4B}">
-  <dimension ref="A1:T19"/>
+  <dimension ref="A1:T20"/>
   <sheetViews>
     <sheetView zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -43094,9 +43483,71 @@
         <v>1200</v>
       </c>
     </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>394</v>
+      </c>
+      <c r="B20" t="s">
+        <v>394</v>
+      </c>
+      <c r="C20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20">
+        <v>190358223</v>
+      </c>
+      <c r="E20" s="4">
+        <v>45321</v>
+      </c>
+      <c r="F20" s="10">
+        <v>5920382423</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="H20" s="10">
+        <v>259433432</v>
+      </c>
+      <c r="I20" s="58" t="s">
+        <v>68</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>350</v>
+      </c>
+      <c r="K20" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="L20" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="M20" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="N20" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="O20" s="4">
+        <v>45321</v>
+      </c>
+      <c r="P20" s="4">
+        <v>45321</v>
+      </c>
+      <c r="Q20" s="4">
+        <v>45687</v>
+      </c>
+      <c r="R20" s="4">
+        <v>45321</v>
+      </c>
+      <c r="S20" s="4">
+        <v>45687</v>
+      </c>
+      <c r="T20" s="22">
+        <v>1200</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -43108,8 +43559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4F93C6E-21BF-4220-AF0D-6D307F3158B8}">
   <dimension ref="A1:AB21"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2:P2"/>
+    <sheetView zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -44008,26 +44459,102 @@
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-      <c r="M11"/>
-      <c r="N11"/>
-      <c r="O11" s="7"/>
-      <c r="U11" s="4"/>
-      <c r="V11" s="4"/>
-      <c r="W11" s="4"/>
-      <c r="X11" s="4"/>
-      <c r="Y11" s="4"/>
-      <c r="Z11" s="2"/>
+      <c r="A11" t="s">
+        <v>395</v>
+      </c>
+      <c r="B11" t="s">
+        <v>395</v>
+      </c>
+      <c r="C11">
+        <v>4233</v>
+      </c>
+      <c r="D11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11">
+        <v>3295423</v>
+      </c>
+      <c r="F11" t="s">
+        <v>143</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>190358223</v>
+      </c>
+      <c r="I11" s="14">
+        <v>45321</v>
+      </c>
+      <c r="J11" s="24">
+        <v>293843151242</v>
+      </c>
+      <c r="K11" s="14">
+        <v>45108</v>
+      </c>
+      <c r="L11" s="14">
+        <v>45473</v>
+      </c>
+      <c r="M11" t="s">
+        <v>399</v>
+      </c>
+      <c r="N11" s="10">
+        <v>259433432</v>
+      </c>
+      <c r="O11" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="P11" s="6" t="s">
+        <v>350</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>76</v>
+      </c>
+      <c r="R11" t="s">
+        <v>130</v>
+      </c>
+      <c r="S11" t="s">
+        <v>119</v>
+      </c>
+      <c r="T11" t="s">
+        <v>91</v>
+      </c>
+      <c r="U11" s="4">
+        <v>45245</v>
+      </c>
+      <c r="V11" s="4">
+        <v>45306</v>
+      </c>
+      <c r="W11" s="4">
+        <v>45672</v>
+      </c>
+      <c r="X11" s="4">
+        <v>45306</v>
+      </c>
+      <c r="Y11" s="4">
+        <v>45672</v>
+      </c>
+      <c r="Z11" s="2">
+        <v>1200</v>
+      </c>
+      <c r="AA11">
+        <v>600</v>
+      </c>
+      <c r="AB11" s="13">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="21" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F21" t="str">
         <f t="shared" ref="F21" si="0">+LOWER(F11)</f>
-        <v/>
+        <v>int</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="H11">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -45143,12 +45670,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7ab8c0d4-f18b-4fef-b649-c77d178c2495">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="65efab6e-20b9-465e-9733-f0c2ab732419" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -45353,20 +45882,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7ab8c0d4-f18b-4fef-b649-c77d178c2495">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="65efab6e-20b9-465e-9733-f0c2ab732419" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C685BDB-1785-4A39-A308-4CA166889A49}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE50E33B-922F-4D33-8831-2DF5BA7F11F6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="65efab6e-20b9-465e-9733-f0c2ab732419"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="7ab8c0d4-f18b-4fef-b649-c77d178c2495"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -45391,18 +45927,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE50E33B-922F-4D33-8831-2DF5BA7F11F6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C685BDB-1785-4A39-A308-4CA166889A49}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="65efab6e-20b9-465e-9733-f0c2ab732419"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="7ab8c0d4-f18b-4fef-b649-c77d178c2495"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Incluir reinstalamento en devengo NP
</commit_message>
<xml_diff>
--- a/prototipo_pcr/inputs/insumos.xlsx
+++ b/prototipo_pcr/inputs/insumos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://suramericana.sharepoint.com/sites/TraNIFF/Shared Documents/féniX/01 IFRS17/01 Archivos de Trabajo/Reservas/02 PCR_CP/03 Tecnología/01 Prototipo/prototipo_pcr/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{5053C977-F307-4044-BC63-272CFAAB14E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2543EDC1-96C8-463B-BF84-584ABCB42D0E}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{5053C977-F307-4044-BC63-272CFAAB14E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7AC59263-96F4-AD42-B848-31CEC758E388}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17340" tabRatio="959" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17340" tabRatio="959" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="param_contabilidad" sheetId="6" r:id="rId1"/>
@@ -1046,7 +1046,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8068" uniqueCount="414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8069" uniqueCount="416">
   <si>
     <t>tipo_insumo</t>
   </si>
@@ -2289,6 +2289,12 @@
   <si>
     <t>costo_contrato</t>
   </si>
+  <si>
+    <t>valor_reinstalamento</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
 </sst>
 </file>
 
@@ -6163,7 +6169,7 @@
   <sheetPr codeName="Hoja10"/>
   <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -46052,8 +46058,8 @@
   <sheetPr codeName="Hoja7"/>
   <dimension ref="A1:AB11"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" zoomScale="125" zoomScaleNormal="109" workbookViewId="0">
-      <selection activeCell="S29" sqref="S29"/>
+    <sheetView topLeftCell="X1" zoomScale="125" zoomScaleNormal="109" workbookViewId="0">
+      <selection activeCell="AB1" sqref="AB1:AB1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -47754,10 +47760,10 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8B056C4-8D76-6947-BFDD-DD6636C4305C}">
   <sheetPr codeName="Hoja9"/>
-  <dimension ref="A1:T6"/>
+  <dimension ref="A1:U6"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -47774,9 +47780,10 @@
     <col min="18" max="18" width="16" style="14" customWidth="1"/>
     <col min="19" max="19" width="18.83203125" style="13" customWidth="1"/>
     <col min="20" max="20" width="17.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.5" style="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
@@ -47837,8 +47844,11 @@
       <c r="T1" s="16" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U1" s="16" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>52</v>
       </c>
@@ -47899,8 +47909,11 @@
       <c r="T2" s="17">
         <v>7000000000</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U2" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>52</v>
       </c>
@@ -47961,8 +47974,11 @@
       <c r="T3" s="17">
         <v>7000000000</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U3" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>52</v>
       </c>
@@ -47973,7 +47989,7 @@
         <v>78</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>99</v>
+        <v>415</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>181</v>
@@ -48023,8 +48039,11 @@
       <c r="T4" s="17">
         <v>5350000000</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U4" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -48085,8 +48104,11 @@
       <c r="T5" s="17">
         <v>134000000</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U5" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>52</v>
       </c>
@@ -48148,6 +48170,9 @@
         <v>115</v>
       </c>
       <c r="T6" s="17">
+        <v>0</v>
+      </c>
+      <c r="U6" s="17">
         <v>90000000</v>
       </c>
     </row>
@@ -48159,14 +48184,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7ab8c0d4-f18b-4fef-b649-c77d178c2495">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="65efab6e-20b9-465e-9733-f0c2ab732419" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -48371,27 +48394,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7ab8c0d4-f18b-4fef-b649-c77d178c2495">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="65efab6e-20b9-465e-9733-f0c2ab732419" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE50E33B-922F-4D33-8831-2DF5BA7F11F6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C685BDB-1785-4A39-A308-4CA166889A49}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="65efab6e-20b9-465e-9733-f0c2ab732419"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="7ab8c0d4-f18b-4fef-b649-c77d178c2495"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -48416,9 +48432,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C685BDB-1785-4A39-A308-4CA166889A49}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE50E33B-922F-4D33-8831-2DF5BA7F11F6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7ab8c0d4-f18b-4fef-b649-c77d178c2495"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="65efab6e-20b9-465e-9733-f0c2ab732419"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
feat: Agregar BTs para deterioro
</commit_message>
<xml_diff>
--- a/prototipo_pcr/inputs/insumos.xlsx
+++ b/prototipo_pcr/inputs/insumos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11003"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://suramericana.sharepoint.com/sites/TraNIFF/Shared Documents/féniX/01 IFRS17/01 Archivos de Trabajo/Reservas/02 PCR_CP/03 Tecnología/01 Prototipo/prototipo_pcr/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{5053C977-F307-4044-BC63-272CFAAB14E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7AC59263-96F4-AD42-B848-31CEC758E388}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{5053C977-F307-4044-BC63-272CFAAB14E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D106FEA-1438-1743-98C7-4FEE2146C3DC}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17340" tabRatio="959" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1046,7 +1046,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8069" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8069" uniqueCount="415">
   <si>
     <t>tipo_insumo</t>
   </si>
@@ -2292,9 +2292,6 @@
   <si>
     <t>valor_reinstalamento</t>
   </si>
-  <si>
-    <t>x</t>
-  </si>
 </sst>
 </file>
 
@@ -47762,8 +47759,8 @@
   <sheetPr codeName="Hoja9"/>
   <dimension ref="A1:U6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="U1" sqref="U1"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -47989,7 +47986,7 @@
         <v>78</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>415</v>
+        <v>95</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>181</v>
@@ -48054,7 +48051,7 @@
         <v>78</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>182</v>
+        <v>349</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>181</v>
@@ -48119,7 +48116,7 @@
         <v>78</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>182</v>
+        <v>349</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>181</v>
@@ -48184,17 +48181,19 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7ab8c0d4-f18b-4fef-b649-c77d178c2495">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="65efab6e-20b9-465e-9733-f0c2ab732419" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003456B0730C78B347BD7589BC061D6E7A" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="eb47ff602caa7ec4c93498109dbc0598">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7ab8c0d4-f18b-4fef-b649-c77d178c2495" xmlns:ns3="65efab6e-20b9-465e-9733-f0c2ab732419" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="15d39866744b831c8a58edb1b96951e3" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101003456B0730C78B347BD7589BC061D6E7A" ma:contentTypeVersion="12" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="63fa1c64418ad5e2c432e8a28af753ff">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7ab8c0d4-f18b-4fef-b649-c77d178c2495" xmlns:ns3="65efab6e-20b9-465e-9733-f0c2ab732419" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0084d3678d80c20d937c1596fa80271a" ns2:_="" ns3:_="">
     <xsd:import namespace="7ab8c0d4-f18b-4fef-b649-c77d178c2495"/>
     <xsd:import namespace="65efab6e-20b9-465e-9733-f0c2ab732419"/>
     <xsd:element name="properties">
@@ -48244,7 +48243,7 @@
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="13" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="68ae7bf6-5ac9-4edb-a7e0-886d92fb71e5" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="13" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Etiquetas de imagen" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="68ae7bf6-5ac9-4edb-a7e0-886d92fb71e5" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
@@ -48303,8 +48302,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Tipo de contenido"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Título"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -48394,56 +48393,39 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7ab8c0d4-f18b-4fef-b649-c77d178c2495">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="65efab6e-20b9-465e-9733-f0c2ab732419" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C685BDB-1785-4A39-A308-4CA166889A49}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE50E33B-922F-4D33-8831-2DF5BA7F11F6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="65efab6e-20b9-465e-9733-f0c2ab732419"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="7ab8c0d4-f18b-4fef-b649-c77d178c2495"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{93DD34A5-1C6E-4C9B-84E4-5A0FA07A6638}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="7ab8c0d4-f18b-4fef-b649-c77d178c2495"/>
-    <ds:schemaRef ds:uri="65efab6e-20b9-465e-9733-f0c2ab732419"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BAD5007-D6F4-40D5-8694-BE07A7433C51}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE50E33B-922F-4D33-8831-2DF5BA7F11F6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C685BDB-1785-4A39-A308-4CA166889A49}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="7ab8c0d4-f18b-4fef-b649-c77d178c2495"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="65efab6e-20b9-465e-9733-f0c2ab732419"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
feat: Cambiar tipo de seguro para terremoto de "D" a "T"
</commit_message>
<xml_diff>
--- a/prototipo_pcr/inputs/insumos.xlsx
+++ b/prototipo_pcr/inputs/insumos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://suramericana.sharepoint.com/sites/TraNIFF/Shared Documents/féniX/01 IFRS17/01 Archivos de Trabajo/Reservas/02 PCR_CP/03 Tecnología/01 Prototipo/prototipo_pcr/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{5053C977-F307-4044-BC63-272CFAAB14E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{44F94269-7288-47D9-BB7C-1833C4A1F820}"/>
+  <xr:revisionPtr revIDLastSave="42" documentId="13_ncr:1_{5053C977-F307-4044-BC63-272CFAAB14E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{43292CAE-1619-46F8-B030-41406291816D}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17340" tabRatio="959" firstSheet="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17340" tabRatio="959" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="param_contabilidad" sheetId="6" r:id="rId1"/>
@@ -38,7 +38,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">porc_descuento!$A$1:$K$17</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">produccion_directo!$A$1:$T$18</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">produccion_rea!$A$1:$Z$10</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">tipo_seguro!$A$1:$C$61</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">tipo_seguro!$A$1:$C$1</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -590,7 +590,7 @@
     <author>tc={B4F53F10-94F2-0D4A-8418-EA623B88C944}</author>
   </authors>
   <commentList>
-    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{B4F53F10-94F2-0D4A-8418-EA623B88C944}">
+    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{B4F53F10-94F2-0D4A-8418-EA623B88C944}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -1020,7 +1020,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8029" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8029" uniqueCount="417">
   <si>
     <t>tipo_insumo</t>
   </si>
@@ -2045,31 +2045,19 @@
     <t>tipo_seguro_codigo</t>
   </si>
   <si>
-    <t>094</t>
+    <t>Personas</t>
   </si>
   <si>
-    <t>ARL</t>
+    <t>P</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>025</t>
+    <t>003</t>
   </si>
   <si>
     <t>Daños</t>
   </si>
   <si>
     <t>D</t>
-  </si>
-  <si>
-    <t>069</t>
-  </si>
-  <si>
-    <t>003</t>
-  </si>
-  <si>
-    <t>013</t>
   </si>
   <si>
     <t>006</t>
@@ -2082,6 +2070,12 @@
   </si>
   <si>
     <t>011</t>
+  </si>
+  <si>
+    <t>012</t>
+  </si>
+  <si>
+    <t>013</t>
   </si>
   <si>
     <t>015</t>
@@ -2102,7 +2096,13 @@
     <t>024</t>
   </si>
   <si>
+    <t>025</t>
+  </si>
+  <si>
     <t>028</t>
+  </si>
+  <si>
+    <t>031</t>
   </si>
   <si>
     <t>032</t>
@@ -2120,13 +2120,76 @@
     <t>039</t>
   </si>
   <si>
-    <t>012</t>
+    <t>Soat</t>
   </si>
   <si>
-    <t>031</t>
+    <t>S</t>
+  </si>
+  <si>
+    <t>069</t>
+  </si>
+  <si>
+    <t>073</t>
+  </si>
+  <si>
+    <t>074</t>
+  </si>
+  <si>
+    <t>075</t>
+  </si>
+  <si>
+    <t>081</t>
+  </si>
+  <si>
+    <t>082</t>
+  </si>
+  <si>
+    <t>084</t>
+  </si>
+  <si>
+    <t>085</t>
+  </si>
+  <si>
+    <t>086</t>
+  </si>
+  <si>
+    <t>088</t>
+  </si>
+  <si>
+    <t>092</t>
+  </si>
+  <si>
+    <t>Previsional</t>
+  </si>
+  <si>
+    <t>PR</t>
+  </si>
+  <si>
+    <t>093</t>
+  </si>
+  <si>
+    <t>094</t>
+  </si>
+  <si>
+    <t>ARL</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>096</t>
+  </si>
+  <si>
+    <t>097</t>
   </si>
   <si>
     <t>109</t>
+  </si>
+  <si>
+    <t>Terremoto</t>
+  </si>
+  <si>
+    <t>T</t>
   </si>
   <si>
     <t>128</t>
@@ -2144,52 +2207,7 @@
     <t>139</t>
   </si>
   <si>
-    <t>084</t>
-  </si>
-  <si>
-    <t>Personas</t>
-  </si>
-  <si>
-    <t>P</t>
-  </si>
-  <si>
-    <t>096</t>
-  </si>
-  <si>
-    <t>086</t>
-  </si>
-  <si>
-    <t>073</t>
-  </si>
-  <si>
-    <t>082</t>
-  </si>
-  <si>
-    <t>074</t>
-  </si>
-  <si>
-    <t>075</t>
-  </si>
-  <si>
-    <t>088</t>
-  </si>
-  <si>
-    <t>093</t>
-  </si>
-  <si>
-    <t>081</t>
-  </si>
-  <si>
-    <t>AAV</t>
-  </si>
-  <si>
-    <t>085</t>
-  </si>
-  <si>
     <t>183</t>
-  </si>
-  <si>
-    <t>097</t>
   </si>
   <si>
     <t>190</t>
@@ -2198,19 +2216,7 @@
     <t>191</t>
   </si>
   <si>
-    <t>092</t>
-  </si>
-  <si>
-    <t>Previsional</t>
-  </si>
-  <si>
-    <t>PR</t>
-  </si>
-  <si>
-    <t>Soat</t>
-  </si>
-  <si>
-    <t>S</t>
+    <t>AAV</t>
   </si>
   <si>
     <t>fecha_corte</t>
@@ -2863,7 +2869,7 @@
 
 <file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="A5" dT="2025-05-19T21:23:30.37" personId="{918B86CF-4EE8-844D-AC23-1FCD19A9DDC1}" id="{B4F53F10-94F2-0D4A-8418-EA623B88C944}">
+  <threadedComment ref="A6" dT="2025-05-19T21:23:30.37" personId="{918B86CF-4EE8-844D-AC23-1FCD19A9DDC1}" id="{B4F53F10-94F2-0D4A-8418-EA623B88C944}">
     <text>Ramo decenal</text>
   </threadedComment>
 </ThreadedComments>
@@ -14517,8 +14523,8 @@
   </sheetPr>
   <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51:B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -14538,667 +14544,672 @@
         <v>340</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.95">
-      <c r="A2" s="43" t="s">
+    <row r="2" spans="1:3">
+      <c r="A2" s="43">
+        <v>181</v>
+      </c>
+      <c r="B2" s="43" t="s">
         <v>341</v>
       </c>
-      <c r="B2" s="43" t="s">
+      <c r="C2" s="43" t="s">
         <v>342</v>
       </c>
-      <c r="C2" s="43" t="s">
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="43">
+        <v>183</v>
+      </c>
+      <c r="B3" s="43" t="s">
+        <v>341</v>
+      </c>
+      <c r="C3" s="43" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="43">
+        <v>193</v>
+      </c>
+      <c r="B4" s="43" t="s">
+        <v>341</v>
+      </c>
+      <c r="C4" s="43" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="43">
+        <v>196</v>
+      </c>
+      <c r="B5" s="43" t="s">
+        <v>341</v>
+      </c>
+      <c r="C5" s="43" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="43" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.95">
-      <c r="A3" s="43" t="s">
+      <c r="B6" s="43" t="s">
         <v>344</v>
       </c>
-      <c r="B3" s="43" t="s">
+      <c r="C6" s="43" t="s">
         <v>345</v>
       </c>
-      <c r="C3" s="43" t="s">
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="43" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.95">
-      <c r="A4" s="43" t="s">
+      <c r="B7" s="43" t="s">
+        <v>344</v>
+      </c>
+      <c r="C7" s="43" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="43" t="s">
         <v>347</v>
       </c>
-      <c r="B4" s="43" t="s">
+      <c r="B8" s="43" t="s">
+        <v>344</v>
+      </c>
+      <c r="C8" s="43" t="s">
         <v>345</v>
       </c>
-      <c r="C4" s="43" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15.95">
-      <c r="A5" s="43" t="s">
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="43" t="s">
+        <v>99</v>
+      </c>
+      <c r="B9" s="43" t="s">
+        <v>344</v>
+      </c>
+      <c r="C9" s="43" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="43" t="s">
         <v>348</v>
       </c>
-      <c r="B5" s="43" t="s">
+      <c r="B10" s="43" t="s">
+        <v>344</v>
+      </c>
+      <c r="C10" s="43" t="s">
         <v>345</v>
       </c>
-      <c r="C5" s="43" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.95">
-      <c r="A6" s="43" t="s">
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="43" t="s">
         <v>349</v>
       </c>
-      <c r="B6" s="43" t="s">
+      <c r="B11" s="43" t="s">
+        <v>344</v>
+      </c>
+      <c r="C11" s="43" t="s">
         <v>345</v>
       </c>
-      <c r="C6" s="43" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="15.95">
-      <c r="A7" s="43" t="s">
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="43" t="s">
+        <v>350</v>
+      </c>
+      <c r="B12" s="43" t="s">
+        <v>344</v>
+      </c>
+      <c r="C12" s="43" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="43" t="s">
+        <v>351</v>
+      </c>
+      <c r="B13" s="43" t="s">
+        <v>344</v>
+      </c>
+      <c r="C13" s="43" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="43" t="s">
+        <v>352</v>
+      </c>
+      <c r="B14" s="43" t="s">
+        <v>344</v>
+      </c>
+      <c r="C14" s="43" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="43" t="s">
+        <v>353</v>
+      </c>
+      <c r="B15" s="43" t="s">
+        <v>344</v>
+      </c>
+      <c r="C15" s="43" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="43" t="s">
+        <v>354</v>
+      </c>
+      <c r="B16" s="43" t="s">
+        <v>344</v>
+      </c>
+      <c r="C16" s="43" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="43" t="s">
+        <v>355</v>
+      </c>
+      <c r="B17" s="43" t="s">
+        <v>344</v>
+      </c>
+      <c r="C17" s="43" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="43" t="s">
+        <v>356</v>
+      </c>
+      <c r="B18" s="43" t="s">
+        <v>344</v>
+      </c>
+      <c r="C18" s="43" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="43" t="s">
+        <v>357</v>
+      </c>
+      <c r="B19" s="43" t="s">
+        <v>344</v>
+      </c>
+      <c r="C19" s="43" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="43" t="s">
+        <v>358</v>
+      </c>
+      <c r="B20" s="43" t="s">
+        <v>344</v>
+      </c>
+      <c r="C20" s="43" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="43" t="s">
+        <v>359</v>
+      </c>
+      <c r="B21" s="43" t="s">
+        <v>344</v>
+      </c>
+      <c r="C21" s="43" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="43" t="s">
         <v>183</v>
       </c>
-      <c r="B7" s="43" t="s">
+      <c r="B22" s="43" t="s">
+        <v>344</v>
+      </c>
+      <c r="C22" s="43" t="s">
         <v>345</v>
       </c>
-      <c r="C7" s="43" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="15.95">
-      <c r="A8" s="43" t="s">
-        <v>350</v>
-      </c>
-      <c r="B8" s="43" t="s">
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="43" t="s">
+        <v>360</v>
+      </c>
+      <c r="B23" s="43" t="s">
+        <v>344</v>
+      </c>
+      <c r="C23" s="43" t="s">
         <v>345</v>
       </c>
-      <c r="C8" s="43" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="15.95">
-      <c r="A9" s="43" t="s">
-        <v>351</v>
-      </c>
-      <c r="B9" s="43" t="s">
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="43" t="s">
+        <v>361</v>
+      </c>
+      <c r="B24" s="43" t="s">
+        <v>344</v>
+      </c>
+      <c r="C24" s="43" t="s">
         <v>345</v>
       </c>
-      <c r="C9" s="43" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="15.95">
-      <c r="A10" s="43" t="s">
-        <v>99</v>
-      </c>
-      <c r="B10" s="43" t="s">
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="43" t="s">
+        <v>362</v>
+      </c>
+      <c r="B25" s="43" t="s">
+        <v>344</v>
+      </c>
+      <c r="C25" s="43" t="s">
         <v>345</v>
       </c>
-      <c r="C10" s="43" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="15.95">
-      <c r="A11" s="43" t="s">
-        <v>352</v>
-      </c>
-      <c r="B11" s="43" t="s">
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="43" t="s">
+        <v>363</v>
+      </c>
+      <c r="B26" s="43" t="s">
+        <v>344</v>
+      </c>
+      <c r="C26" s="43" t="s">
         <v>345</v>
       </c>
-      <c r="C11" s="43" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="15.95">
-      <c r="A12" s="43" t="s">
-        <v>353</v>
-      </c>
-      <c r="B12" s="43" t="s">
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="43" t="s">
+        <v>364</v>
+      </c>
+      <c r="B27" s="43" t="s">
+        <v>344</v>
+      </c>
+      <c r="C27" s="43" t="s">
         <v>345</v>
       </c>
-      <c r="C12" s="43" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="15.95">
-      <c r="A13" s="43" t="s">
-        <v>354</v>
-      </c>
-      <c r="B13" s="43" t="s">
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="43" t="s">
+        <v>365</v>
+      </c>
+      <c r="B28" s="43" t="s">
+        <v>344</v>
+      </c>
+      <c r="C28" s="43" t="s">
         <v>345</v>
       </c>
-      <c r="C13" s="43" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="15.95">
-      <c r="A14" s="43" t="s">
-        <v>355</v>
-      </c>
-      <c r="B14" s="43" t="s">
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="43" t="s">
+        <v>79</v>
+      </c>
+      <c r="B29" s="43" t="s">
+        <v>344</v>
+      </c>
+      <c r="C29" s="43" t="s">
         <v>345</v>
       </c>
-      <c r="C14" s="43" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="15.95">
-      <c r="A15" s="43" t="s">
-        <v>356</v>
-      </c>
-      <c r="B15" s="43" t="s">
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="43" t="s">
+        <v>97</v>
+      </c>
+      <c r="B30" s="43" t="s">
+        <v>366</v>
+      </c>
+      <c r="C30" s="43" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="43" t="s">
+        <v>368</v>
+      </c>
+      <c r="B31" s="43" t="s">
+        <v>344</v>
+      </c>
+      <c r="C31" s="43" t="s">
         <v>345</v>
       </c>
-      <c r="C15" s="43" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="15.95">
-      <c r="A16" s="43" t="s">
-        <v>357</v>
-      </c>
-      <c r="B16" s="43" t="s">
-        <v>345</v>
-      </c>
-      <c r="C16" s="43" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="15.95">
-      <c r="A17" s="43" t="s">
-        <v>358</v>
-      </c>
-      <c r="B17" s="43" t="s">
-        <v>345</v>
-      </c>
-      <c r="C17" s="43" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="15.95">
-      <c r="A18" s="43" t="s">
-        <v>359</v>
-      </c>
-      <c r="B18" s="43" t="s">
-        <v>345</v>
-      </c>
-      <c r="C18" s="43" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="15.95">
-      <c r="A19" s="43" t="s">
-        <v>360</v>
-      </c>
-      <c r="B19" s="43" t="s">
-        <v>345</v>
-      </c>
-      <c r="C19" s="43" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="15.95">
-      <c r="A20" s="43" t="s">
-        <v>361</v>
-      </c>
-      <c r="B20" s="43" t="s">
-        <v>345</v>
-      </c>
-      <c r="C20" s="43" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="15.95">
-      <c r="A21" s="43" t="s">
-        <v>362</v>
-      </c>
-      <c r="B21" s="43" t="s">
-        <v>345</v>
-      </c>
-      <c r="C21" s="43" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="15.95">
-      <c r="A22" s="43" t="s">
-        <v>363</v>
-      </c>
-      <c r="B22" s="43" t="s">
-        <v>345</v>
-      </c>
-      <c r="C22" s="43" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="15.95">
-      <c r="A23" s="43" t="s">
-        <v>364</v>
-      </c>
-      <c r="B23" s="43" t="s">
-        <v>345</v>
-      </c>
-      <c r="C23" s="43" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="15.95">
-      <c r="A24" s="43" t="s">
-        <v>365</v>
-      </c>
-      <c r="B24" s="43" t="s">
-        <v>345</v>
-      </c>
-      <c r="C24" s="43" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="15.95">
-      <c r="A25" s="43" t="s">
-        <v>79</v>
-      </c>
-      <c r="B25" s="43" t="s">
-        <v>345</v>
-      </c>
-      <c r="C25" s="43" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="15.95">
-      <c r="A26" s="43" t="s">
-        <v>366</v>
-      </c>
-      <c r="B26" s="43" t="s">
-        <v>345</v>
-      </c>
-      <c r="C26" s="43" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="15.95">
-      <c r="A27" s="43" t="s">
-        <v>367</v>
-      </c>
-      <c r="B27" s="43" t="s">
-        <v>345</v>
-      </c>
-      <c r="C27" s="43" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="15.95">
-      <c r="A28" s="43" t="s">
-        <v>368</v>
-      </c>
-      <c r="B28" s="43" t="s">
-        <v>345</v>
-      </c>
-      <c r="C28" s="43" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="15.95">
-      <c r="A29" s="43" t="s">
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="43" t="s">
         <v>369</v>
       </c>
-      <c r="B29" s="43" t="s">
-        <v>345</v>
-      </c>
-      <c r="C29" s="43" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="15.95">
-      <c r="A30" s="43" t="s">
+      <c r="B32" s="43" t="s">
+        <v>341</v>
+      </c>
+      <c r="C32" s="43" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="43" t="s">
+        <v>370</v>
+      </c>
+      <c r="B33" s="43" t="s">
+        <v>341</v>
+      </c>
+      <c r="C33" s="43" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="43" t="s">
+        <v>371</v>
+      </c>
+      <c r="B34" s="43" t="s">
+        <v>341</v>
+      </c>
+      <c r="C34" s="43" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="43" t="s">
+        <v>372</v>
+      </c>
+      <c r="B35" s="43" t="s">
+        <v>341</v>
+      </c>
+      <c r="C35" s="43" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="43" t="s">
+        <v>373</v>
+      </c>
+      <c r="B36" s="43" t="s">
+        <v>341</v>
+      </c>
+      <c r="C36" s="43" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="43" t="s">
+        <v>95</v>
+      </c>
+      <c r="B37" s="43" t="s">
+        <v>341</v>
+      </c>
+      <c r="C37" s="43" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="43" t="s">
+        <v>374</v>
+      </c>
+      <c r="B38" s="43" t="s">
+        <v>341</v>
+      </c>
+      <c r="C38" s="43" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="45" t="s">
+        <v>375</v>
+      </c>
+      <c r="B39" s="43" t="s">
+        <v>341</v>
+      </c>
+      <c r="C39" s="43" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="43" t="s">
+        <v>376</v>
+      </c>
+      <c r="B40" s="43" t="s">
+        <v>341</v>
+      </c>
+      <c r="C40" s="43" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="43" t="s">
+        <v>102</v>
+      </c>
+      <c r="B41" s="43" t="s">
+        <v>341</v>
+      </c>
+      <c r="C41" s="43" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="43" t="s">
+        <v>377</v>
+      </c>
+      <c r="B42" s="43" t="s">
+        <v>341</v>
+      </c>
+      <c r="C42" s="43" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="43" t="s">
+        <v>181</v>
+      </c>
+      <c r="B43" s="43" t="s">
+        <v>341</v>
+      </c>
+      <c r="C43" s="43" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="43" t="s">
+        <v>98</v>
+      </c>
+      <c r="B44" s="43" t="s">
+        <v>341</v>
+      </c>
+      <c r="C44" s="43" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="44" t="s">
+        <v>378</v>
+      </c>
+      <c r="B45" s="43" t="s">
+        <v>379</v>
+      </c>
+      <c r="C45" s="43" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="43" t="s">
+        <v>381</v>
+      </c>
+      <c r="B46" s="43" t="s">
+        <v>341</v>
+      </c>
+      <c r="C46" s="43" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="43" t="s">
+        <v>382</v>
+      </c>
+      <c r="B47" s="43" t="s">
+        <v>383</v>
+      </c>
+      <c r="C47" s="43" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="43" t="s">
+        <v>161</v>
+      </c>
+      <c r="B48" s="43" t="s">
+        <v>341</v>
+      </c>
+      <c r="C48" s="43" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="43" t="s">
+        <v>385</v>
+      </c>
+      <c r="B49" s="43" t="s">
+        <v>341</v>
+      </c>
+      <c r="C49" s="43" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="46" t="s">
+        <v>386</v>
+      </c>
+      <c r="B50" s="46" t="s">
+        <v>341</v>
+      </c>
+      <c r="C50" s="43" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="43" t="s">
+        <v>387</v>
+      </c>
+      <c r="B51" s="43" t="s">
+        <v>388</v>
+      </c>
+      <c r="C51" s="43" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="43" t="s">
+        <v>390</v>
+      </c>
+      <c r="B52" s="43" t="s">
+        <v>388</v>
+      </c>
+      <c r="C52" s="43" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="43" t="s">
         <v>101</v>
       </c>
-      <c r="B30" s="43" t="s">
-        <v>345</v>
-      </c>
-      <c r="C30" s="43" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="15.95">
-      <c r="A31" s="43" t="s">
-        <v>370</v>
-      </c>
-      <c r="B31" s="43" t="s">
-        <v>345</v>
-      </c>
-      <c r="C31" s="43" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="15.95">
-      <c r="A32" s="43" t="s">
-        <v>371</v>
-      </c>
-      <c r="B32" s="43" t="s">
-        <v>345</v>
-      </c>
-      <c r="C32" s="43" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="15.95">
-      <c r="A33" s="43" t="s">
-        <v>372</v>
-      </c>
-      <c r="B33" s="43" t="s">
-        <v>345</v>
-      </c>
-      <c r="C33" s="43" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="15.95">
-      <c r="A34" s="43" t="s">
-        <v>373</v>
-      </c>
-      <c r="B34" s="43" t="s">
-        <v>345</v>
-      </c>
-      <c r="C34" s="43" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="15.95">
-      <c r="A35" s="43" t="s">
-        <v>374</v>
-      </c>
-      <c r="B35" s="43" t="s">
-        <v>375</v>
-      </c>
-      <c r="C35" s="43" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="15.95">
-      <c r="A36" s="43" t="s">
-        <v>377</v>
-      </c>
-      <c r="B36" s="43" t="s">
-        <v>375</v>
-      </c>
-      <c r="C36" s="43" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="15.95">
-      <c r="A37" s="43" t="s">
-        <v>378</v>
-      </c>
-      <c r="B37" s="43" t="s">
-        <v>375</v>
-      </c>
-      <c r="C37" s="43" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="15.95">
-      <c r="A38" s="43" t="s">
-        <v>379</v>
-      </c>
-      <c r="B38" s="43" t="s">
-        <v>375</v>
-      </c>
-      <c r="C38" s="43" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="15.95">
-      <c r="A39" s="43" t="s">
-        <v>380</v>
-      </c>
-      <c r="B39" s="43" t="s">
-        <v>375</v>
-      </c>
-      <c r="C39" s="43" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="15.95">
-      <c r="A40" s="43" t="s">
-        <v>381</v>
-      </c>
-      <c r="B40" s="43" t="s">
-        <v>375</v>
-      </c>
-      <c r="C40" s="43" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="15.95">
-      <c r="A41" s="43" t="s">
-        <v>382</v>
-      </c>
-      <c r="B41" s="43" t="s">
-        <v>375</v>
-      </c>
-      <c r="C41" s="43" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="15.95">
-      <c r="A42" s="43">
-        <v>181</v>
-      </c>
-      <c r="B42" s="43" t="s">
-        <v>375</v>
-      </c>
-      <c r="C42" s="43" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="15.95">
-      <c r="A43" s="43" t="s">
-        <v>102</v>
-      </c>
-      <c r="B43" s="43" t="s">
-        <v>375</v>
-      </c>
-      <c r="C43" s="43" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="15.95">
-      <c r="A44" s="43" t="s">
-        <v>383</v>
-      </c>
-      <c r="B44" s="43" t="s">
-        <v>375</v>
-      </c>
-      <c r="C44" s="43" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="15.95">
-      <c r="A45" s="43" t="s">
-        <v>384</v>
-      </c>
-      <c r="B45" s="43" t="s">
-        <v>375</v>
-      </c>
-      <c r="C45" s="43" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="15.95">
-      <c r="A46" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="B46" s="43" t="s">
-        <v>375</v>
-      </c>
-      <c r="C46" s="43" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="15.95">
-      <c r="A47" s="43">
-        <v>196</v>
-      </c>
-      <c r="B47" s="43" t="s">
-        <v>375</v>
-      </c>
-      <c r="C47" s="43" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="15.95">
-      <c r="A48" s="43">
-        <v>193</v>
-      </c>
-      <c r="B48" s="43" t="s">
-        <v>375</v>
-      </c>
-      <c r="C48" s="43" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="15.95">
-      <c r="A49" s="43">
-        <v>183</v>
-      </c>
-      <c r="B49" s="43" t="s">
-        <v>375</v>
-      </c>
-      <c r="C49" s="43" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="15.95">
-      <c r="A50" s="43" t="s">
-        <v>95</v>
-      </c>
-      <c r="B50" s="43" t="s">
-        <v>375</v>
-      </c>
-      <c r="C50" s="43" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="15.95">
-      <c r="A51" s="43" t="s">
-        <v>385</v>
-      </c>
-      <c r="B51" s="43" t="s">
-        <v>375</v>
-      </c>
-      <c r="C51" s="43" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="15.95">
-      <c r="A52" s="43" t="s">
-        <v>386</v>
-      </c>
-      <c r="B52" s="43" t="s">
-        <v>375</v>
-      </c>
-      <c r="C52" s="43" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="15.95">
-      <c r="A53" s="45" t="s">
-        <v>387</v>
-      </c>
       <c r="B53" s="43" t="s">
-        <v>375</v>
+        <v>388</v>
       </c>
       <c r="C53" s="43" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="15.95">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
       <c r="A54" s="43" t="s">
-        <v>98</v>
+        <v>391</v>
       </c>
       <c r="B54" s="43" t="s">
-        <v>375</v>
+        <v>388</v>
       </c>
       <c r="C54" s="43" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="15.95">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
       <c r="A55" s="43" t="s">
-        <v>181</v>
+        <v>392</v>
       </c>
       <c r="B55" s="43" t="s">
-        <v>375</v>
+        <v>388</v>
       </c>
       <c r="C55" s="43" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="15.95">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
       <c r="A56" s="43" t="s">
+        <v>393</v>
+      </c>
+      <c r="B56" s="43" t="s">
         <v>388</v>
       </c>
-      <c r="B56" s="43" t="s">
-        <v>375</v>
-      </c>
       <c r="C56" s="43" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="15.95">
-      <c r="A57" s="46" t="s">
         <v>389</v>
       </c>
-      <c r="B57" s="46" t="s">
-        <v>375</v>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="43" t="s">
+        <v>394</v>
+      </c>
+      <c r="B57" s="43" t="s">
+        <v>388</v>
       </c>
       <c r="C57" s="43" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" ht="15.95">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
       <c r="A58" s="43" t="s">
-        <v>390</v>
+        <v>395</v>
       </c>
       <c r="B58" s="43" t="s">
-        <v>375</v>
+        <v>341</v>
       </c>
       <c r="C58" s="43" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" ht="15.95">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
       <c r="A59" s="43" t="s">
-        <v>391</v>
+        <v>396</v>
       </c>
       <c r="B59" s="43" t="s">
-        <v>375</v>
+        <v>341</v>
       </c>
       <c r="C59" s="43" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="15.95">
-      <c r="A60" s="44" t="s">
-        <v>392</v>
+        <v>342</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="43" t="s">
+        <v>397</v>
       </c>
       <c r="B60" s="43" t="s">
-        <v>393</v>
+        <v>341</v>
       </c>
       <c r="C60" s="43" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" ht="15.95">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
       <c r="A61" s="43" t="s">
-        <v>97</v>
+        <v>398</v>
       </c>
       <c r="B61" s="43" t="s">
-        <v>395</v>
+        <v>341</v>
       </c>
       <c r="C61" s="43" t="s">
-        <v>396</v>
+        <v>342</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C1" xr:uid="{04FB4049-F651-384C-8DCF-CEAFB17703EB}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C61">
+      <sortCondition ref="A1"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
@@ -15229,7 +15240,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>1</v>
@@ -15259,18 +15270,18 @@
         <v>134</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="B2" s="14">
         <v>45322</v>
       </c>
       <c r="C2" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="D2" t="s">
         <v>238</v>
@@ -15302,13 +15313,13 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="B3" s="14">
         <v>45322</v>
       </c>
       <c r="C3" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="D3" t="s">
         <v>238</v>
@@ -15379,7 +15390,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>162</v>
@@ -15388,7 +15399,7 @@
         <v>163</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>4</v>
@@ -15397,10 +15408,10 @@
         <v>3</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>73</v>
@@ -15415,27 +15426,27 @@
         <v>134</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="B2" s="14">
         <v>45657</v>
       </c>
       <c r="F2" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="G2" t="s">
         <v>46</v>
       </c>
       <c r="H2" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="I2" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="J2" s="7" t="s">
         <v>81</v>
@@ -15455,22 +15466,22 @@
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="B3" s="14">
         <v>45657</v>
       </c>
       <c r="F3" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="G3" t="s">
         <v>46</v>
       </c>
       <c r="H3" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="I3" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="J3" s="7" t="s">
         <v>81</v>
@@ -15490,22 +15501,22 @@
     </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="B4" s="14">
         <v>45657</v>
       </c>
       <c r="F4" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="G4" t="s">
         <v>50</v>
       </c>
       <c r="H4" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="I4" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="J4" s="7" t="s">
         <v>81</v>
@@ -47995,12 +48006,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7ab8c0d4-f18b-4fef-b649-c77d178c2495">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="65efab6e-20b9-465e-9733-f0c2ab732419" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -48205,26 +48218,24 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7ab8c0d4-f18b-4fef-b649-c77d178c2495">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="65efab6e-20b9-465e-9733-f0c2ab732419" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C685BDB-1785-4A39-A308-4CA166889A49}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE50E33B-922F-4D33-8831-2DF5BA7F11F6}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2447AA2-4D77-4E90-A16B-99E3B284965B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D43FA500-B4BA-4DED-8DE0-EA4A442F0F3F}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE50E33B-922F-4D33-8831-2DF5BA7F11F6}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C685BDB-1785-4A39-A308-4CA166889A49}"/>
 </file>
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
refactor: Ajustar BTs de costo de contrato para evitar duplicados
</commit_message>
<xml_diff>
--- a/prototipo_pcr/inputs/insumos.xlsx
+++ b/prototipo_pcr/inputs/insumos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebatoec/projects/prototipo_pcr/prototipo_pcr/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3CCCAC6-2E4C-9E42-B118-98D87A784CE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C56FCB9C-595C-B944-BC2C-0BF9E44F43AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17340" tabRatio="959" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17340" tabRatio="959" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="param_contabilidad" sheetId="6" r:id="rId1"/>
@@ -2903,8 +2903,8 @@
   </sheetPr>
   <dimension ref="A1:K98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView topLeftCell="A25" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B88" sqref="B88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4112,7 +4112,7 @@
         <v>52</v>
       </c>
       <c r="B38" t="s">
-        <v>11</v>
+        <v>414</v>
       </c>
       <c r="C38" t="s">
         <v>12</v>
@@ -4144,7 +4144,7 @@
         <v>52</v>
       </c>
       <c r="B39" t="s">
-        <v>11</v>
+        <v>414</v>
       </c>
       <c r="C39" t="s">
         <v>12</v>
@@ -4816,7 +4816,7 @@
         <v>52</v>
       </c>
       <c r="B60" t="s">
-        <v>11</v>
+        <v>414</v>
       </c>
       <c r="C60" t="s">
         <v>12</v>
@@ -4848,7 +4848,7 @@
         <v>52</v>
       </c>
       <c r="B61" t="s">
-        <v>11</v>
+        <v>414</v>
       </c>
       <c r="C61" t="s">
         <v>12</v>
@@ -5360,7 +5360,7 @@
         <v>52</v>
       </c>
       <c r="B77" t="s">
-        <v>11</v>
+        <v>414</v>
       </c>
       <c r="C77" t="s">
         <v>12</v>
@@ -5392,7 +5392,7 @@
         <v>52</v>
       </c>
       <c r="B78" t="s">
-        <v>11</v>
+        <v>414</v>
       </c>
       <c r="C78" t="s">
         <v>12</v>
@@ -46143,7 +46143,7 @@
   <dimension ref="A1:T20"/>
   <sheetViews>
     <sheetView zoomScale="180" zoomScaleNormal="109" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -47352,7 +47352,7 @@
         <v>159</v>
       </c>
       <c r="B20" t="s">
-        <v>159</v>
+        <v>38</v>
       </c>
       <c r="C20" t="s">
         <v>13</v>
@@ -47424,8 +47424,8 @@
   <sheetPr codeName="Hoja7"/>
   <dimension ref="A1:AB11"/>
   <sheetViews>
-    <sheetView topLeftCell="X1" zoomScale="125" zoomScaleNormal="109" workbookViewId="0">
-      <selection activeCell="AB1" sqref="AB1"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="109" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -48328,7 +48328,7 @@
         <v>172</v>
       </c>
       <c r="B11" t="s">
-        <v>172</v>
+        <v>70</v>
       </c>
       <c r="C11">
         <v>4233</v>
@@ -49129,7 +49129,7 @@
   <dimension ref="A1:U6"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
feat: Incorporar produccion de ARL
</commit_message>
<xml_diff>
--- a/prototipo_pcr/inputs/insumos.xlsx
+++ b/prototipo_pcr/inputs/insumos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11003"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11018"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebatoec/projects/prototipo_pcr/prototipo_pcr/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C56FCB9C-595C-B944-BC2C-0BF9E44F43AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E903877-2835-8C4F-B292-31BF135DA88A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17340" tabRatio="959" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17340" tabRatio="959" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="param_contabilidad" sheetId="6" r:id="rId1"/>
@@ -2903,8 +2903,8 @@
   </sheetPr>
   <dimension ref="A1:K98"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B88" sqref="B88"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -47424,7 +47424,7 @@
   <sheetPr codeName="Hoja7"/>
   <dimension ref="A1:AB11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="109" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="109" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
feat: Incorporar cuenta corriente
</commit_message>
<xml_diff>
--- a/prototipo_pcr/inputs/insumos.xlsx
+++ b/prototipo_pcr/inputs/insumos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebatoec/projects/prototipo_pcr/prototipo_pcr/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91D6187A-069A-F54F-8C74-A9E988BCE096}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{479EE68D-D8AF-BF44-9FD8-EC4C63CAF015}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17340" tabRatio="959" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17340" tabRatio="959" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="param_contabilidad" sheetId="6" r:id="rId1"/>
@@ -28,13 +28,12 @@
     <sheet name="map_bt" sheetId="20" r:id="rId13"/>
     <sheet name="tipo_seguro" sheetId="21" r:id="rId14"/>
     <sheet name="cuenta_cobrar_directo" sheetId="23" r:id="rId15"/>
-    <sheet name="cuenta_corriente_rea" sheetId="25" r:id="rId16"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">comision_rea!$A$1:$V$9</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">gastos!$B$1:$K$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">map_bt!$A$1:$I$261</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">param_contabilidad!$A$1:$J$98</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">param_contabilidad!$A$1:$J$102</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">porc_descuento!$A$1:$K$17</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">produccion_directo!$A$1:$T$18</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">produccion_rea!$A$1:$Z$10</definedName>
@@ -209,7 +208,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G36" authorId="0" shapeId="0" xr:uid="{60704782-0207-754E-8C3D-579B8D19FB81}">
+    <comment ref="G40" authorId="0" shapeId="0" xr:uid="{60704782-0207-754E-8C3D-579B8D19FB81}">
       <text>
         <r>
           <rPr>
@@ -222,7 +221,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G37" authorId="0" shapeId="0" xr:uid="{79E1C198-5A7C-3E4A-B967-D774BDD95BB9}">
+    <comment ref="G41" authorId="0" shapeId="0" xr:uid="{79E1C198-5A7C-3E4A-B967-D774BDD95BB9}">
       <text>
         <r>
           <rPr>
@@ -235,7 +234,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G38" authorId="0" shapeId="0" xr:uid="{E2EB6F16-7DC2-B547-9D29-6287117B6B6D}">
+    <comment ref="G42" authorId="0" shapeId="0" xr:uid="{E2EB6F16-7DC2-B547-9D29-6287117B6B6D}">
       <text>
         <r>
           <rPr>
@@ -248,7 +247,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G39" authorId="0" shapeId="0" xr:uid="{CADF5D80-B324-BD4D-83EF-7103C7C4BCDC}">
+    <comment ref="G43" authorId="0" shapeId="0" xr:uid="{CADF5D80-B324-BD4D-83EF-7103C7C4BCDC}">
       <text>
         <r>
           <rPr>
@@ -261,7 +260,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A51" authorId="1" shapeId="0" xr:uid="{EEFD83EE-3C57-0040-A776-C6A8CAEFDA01}">
+    <comment ref="A55" authorId="1" shapeId="0" xr:uid="{EEFD83EE-3C57-0040-A776-C6A8CAEFDA01}">
       <text>
         <r>
           <rPr>
@@ -294,7 +293,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A52" authorId="1" shapeId="0" xr:uid="{1C6775A6-7A61-FC47-AD2D-7B8B13898F2C}">
+    <comment ref="A56" authorId="1" shapeId="0" xr:uid="{1C6775A6-7A61-FC47-AD2D-7B8B13898F2C}">
       <text>
         <r>
           <rPr>
@@ -327,7 +326,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A53" authorId="1" shapeId="0" xr:uid="{FB267839-4FB3-E246-A4AB-DE20DBF48B28}">
+    <comment ref="A57" authorId="1" shapeId="0" xr:uid="{FB267839-4FB3-E246-A4AB-DE20DBF48B28}">
       <text>
         <r>
           <rPr>
@@ -360,7 +359,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G60" authorId="0" shapeId="0" xr:uid="{7D06FA4A-5748-C349-AE6A-6BF22180618F}">
+    <comment ref="G64" authorId="0" shapeId="0" xr:uid="{7D06FA4A-5748-C349-AE6A-6BF22180618F}">
       <text>
         <r>
           <rPr>
@@ -373,7 +372,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G61" authorId="0" shapeId="0" xr:uid="{60B7F3D0-2F4A-0645-8858-314766FA3CB7}">
+    <comment ref="G65" authorId="0" shapeId="0" xr:uid="{60B7F3D0-2F4A-0645-8858-314766FA3CB7}">
       <text>
         <r>
           <rPr>
@@ -386,7 +385,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G75" authorId="0" shapeId="0" xr:uid="{E6330DC2-B24F-ED40-95D8-2DAC8AE12089}">
+    <comment ref="G79" authorId="0" shapeId="0" xr:uid="{E6330DC2-B24F-ED40-95D8-2DAC8AE12089}">
       <text>
         <r>
           <rPr>
@@ -399,7 +398,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G76" authorId="0" shapeId="0" xr:uid="{92BF18EE-22AE-B144-9B75-E64D6C7556B1}">
+    <comment ref="G80" authorId="0" shapeId="0" xr:uid="{92BF18EE-22AE-B144-9B75-E64D6C7556B1}">
       <text>
         <r>
           <rPr>
@@ -412,7 +411,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G77" authorId="0" shapeId="0" xr:uid="{03FC245B-BB84-D04E-951E-37009D11D476}">
+    <comment ref="G81" authorId="0" shapeId="0" xr:uid="{03FC245B-BB84-D04E-951E-37009D11D476}">
       <text>
         <r>
           <rPr>
@@ -425,7 +424,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G78" authorId="0" shapeId="0" xr:uid="{F47F6BE0-1988-7A49-8D44-80895B191E26}">
+    <comment ref="G82" authorId="0" shapeId="0" xr:uid="{F47F6BE0-1988-7A49-8D44-80895B191E26}">
       <text>
         <r>
           <rPr>
@@ -438,7 +437,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A90" authorId="1" shapeId="0" xr:uid="{960598ED-127D-444A-AE38-C3AFAA411D4A}">
+    <comment ref="A94" authorId="1" shapeId="0" xr:uid="{960598ED-127D-444A-AE38-C3AFAA411D4A}">
       <text>
         <r>
           <rPr>
@@ -471,7 +470,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A91" authorId="1" shapeId="0" xr:uid="{AF9ED192-6F2B-9A4A-ABFC-F6E0AB6DC88B}">
+    <comment ref="A95" authorId="1" shapeId="0" xr:uid="{AF9ED192-6F2B-9A4A-ABFC-F6E0AB6DC88B}">
       <text>
         <r>
           <rPr>
@@ -504,7 +503,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A92" authorId="1" shapeId="0" xr:uid="{DB8EB780-29ED-0A4F-AD19-96C9969B2ED2}">
+    <comment ref="A96" authorId="1" shapeId="0" xr:uid="{DB8EB780-29ED-0A4F-AD19-96C9969B2ED2}">
       <text>
         <r>
           <rPr>
@@ -1020,7 +1019,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8292" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8283" uniqueCount="420">
   <si>
     <t>tipo_insumo</t>
   </si>
@@ -2228,39 +2227,6 @@
     <t>cuenta_cobrar_noexigible_directo</t>
   </si>
   <si>
-    <t>fe_ini_vigencia_contrato_rea</t>
-  </si>
-  <si>
-    <t>concepto</t>
-  </si>
-  <si>
-    <t>tipo_cuenta</t>
-  </si>
-  <si>
-    <t>cuenta_pagar_prima_rea</t>
-  </si>
-  <si>
-    <t>cedido</t>
-  </si>
-  <si>
-    <t>prima_cedida</t>
-  </si>
-  <si>
-    <t>pasivo</t>
-  </si>
-  <si>
-    <t>cuenta_cobrar_comision_rea</t>
-  </si>
-  <si>
-    <t>comisiones_reaseguro</t>
-  </si>
-  <si>
-    <t>activo</t>
-  </si>
-  <si>
-    <t>cuenta_pagar_costo_rea</t>
-  </si>
-  <si>
     <t>costo_contrato</t>
   </si>
   <si>
@@ -2289,6 +2255,30 @@
   </si>
   <si>
     <t>cartera_no_exigible</t>
+  </si>
+  <si>
+    <t>cuenta_pagar_contratos_np</t>
+  </si>
+  <si>
+    <t>cuenta_pagar_contratos_pp</t>
+  </si>
+  <si>
+    <t>cuenta_cobrar_comisiones_pp</t>
+  </si>
+  <si>
+    <t>cuenta_cobrar_comisiones_np</t>
+  </si>
+  <si>
+    <t>saldo/movimiento de la cuenta corriente por concepto de primas</t>
+  </si>
+  <si>
+    <t>saldo/movimiento de la cuenta corriente por concepto de costos de contrato</t>
+  </si>
+  <si>
+    <t>saldo/movimiento de la cuenta corriente por concepto de comisiones de contratos proporcionales</t>
+  </si>
+  <si>
+    <t>saldo/movimiento de la cuenta corriente por concepto de comisiones de contratos no proporcionales</t>
   </si>
 </sst>
 </file>
@@ -2898,10 +2888,10 @@
   <sheetPr codeName="Hoja1">
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:K98"/>
+  <dimension ref="A1:K102"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3920,7 +3910,7 @@
         <v>11</v>
       </c>
       <c r="C32" t="s">
-        <v>421</v>
+        <v>410</v>
       </c>
       <c r="D32" t="s">
         <v>13</v>
@@ -3941,7 +3931,7 @@
         <v>1</v>
       </c>
       <c r="J32" s="54" t="s">
-        <v>414</v>
+        <v>403</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
@@ -3952,7 +3942,7 @@
         <v>11</v>
       </c>
       <c r="C33" t="s">
-        <v>422</v>
+        <v>411</v>
       </c>
       <c r="D33" t="s">
         <v>13</v>
@@ -3973,27 +3963,27 @@
         <v>1</v>
       </c>
       <c r="J33" s="54" t="s">
-        <v>415</v>
+        <v>404</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>45</v>
+        <v>413</v>
       </c>
       <c r="B34" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="C34" t="s">
-        <v>12</v>
+        <v>410</v>
       </c>
       <c r="D34" t="s">
         <v>46</v>
       </c>
       <c r="E34" t="s">
-        <v>47</v>
+        <v>240</v>
       </c>
       <c r="F34" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G34" t="s">
         <v>31</v>
@@ -4005,24 +3995,24 @@
         <v>1</v>
       </c>
       <c r="J34" s="54" t="s">
-        <v>48</v>
+        <v>416</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>45</v>
+        <v>412</v>
       </c>
       <c r="B35" t="s">
-        <v>43</v>
+        <v>402</v>
       </c>
       <c r="C35" t="s">
-        <v>12</v>
+        <v>410</v>
       </c>
       <c r="D35" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E35" t="s">
-        <v>47</v>
+        <v>240</v>
       </c>
       <c r="F35" t="s">
         <v>32</v>
@@ -4037,85 +4027,85 @@
         <v>1</v>
       </c>
       <c r="J35" s="54" t="s">
-        <v>48</v>
+        <v>417</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>49</v>
+        <v>414</v>
       </c>
       <c r="B36" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="C36" t="s">
-        <v>12</v>
+        <v>410</v>
       </c>
       <c r="D36" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E36" t="s">
-        <v>47</v>
+        <v>240</v>
       </c>
       <c r="F36" t="s">
-        <v>30</v>
-      </c>
-      <c r="G36" s="30" t="s">
-        <v>15</v>
+        <v>32</v>
+      </c>
+      <c r="G36" t="s">
+        <v>31</v>
       </c>
       <c r="H36">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="I36">
         <v>1</v>
       </c>
       <c r="J36" s="54" t="s">
-        <v>51</v>
+        <v>418</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>49</v>
+        <v>415</v>
       </c>
       <c r="B37" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="C37" t="s">
-        <v>12</v>
+        <v>410</v>
       </c>
       <c r="D37" t="s">
         <v>50</v>
       </c>
       <c r="E37" t="s">
-        <v>47</v>
+        <v>240</v>
       </c>
       <c r="F37" t="s">
         <v>32</v>
       </c>
-      <c r="G37" s="30" t="s">
-        <v>15</v>
+      <c r="G37" t="s">
+        <v>31</v>
       </c>
       <c r="H37">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="I37">
         <v>1</v>
       </c>
       <c r="J37" s="54" t="s">
-        <v>51</v>
+        <v>419</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B38" t="s">
-        <v>413</v>
+        <v>43</v>
       </c>
       <c r="C38" t="s">
         <v>12</v>
       </c>
       <c r="D38" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E38" t="s">
         <v>47</v>
@@ -4123,8 +4113,8 @@
       <c r="F38" t="s">
         <v>30</v>
       </c>
-      <c r="G38" s="30" t="s">
-        <v>15</v>
+      <c r="G38" t="s">
+        <v>31</v>
       </c>
       <c r="H38">
         <v>1</v>
@@ -4133,21 +4123,21 @@
         <v>1</v>
       </c>
       <c r="J38" s="54" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B39" t="s">
-        <v>413</v>
+        <v>43</v>
       </c>
       <c r="C39" t="s">
         <v>12</v>
       </c>
       <c r="D39" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E39" t="s">
         <v>47</v>
@@ -4155,8 +4145,8 @@
       <c r="F39" t="s">
         <v>32</v>
       </c>
-      <c r="G39" s="30" t="s">
-        <v>15</v>
+      <c r="G39" t="s">
+        <v>31</v>
       </c>
       <c r="H39">
         <v>1</v>
@@ -4165,29 +4155,29 @@
         <v>1</v>
       </c>
       <c r="J39" s="54" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B40" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="C40" t="s">
         <v>12</v>
       </c>
       <c r="D40" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E40" t="s">
         <v>47</v>
       </c>
       <c r="F40" t="s">
-        <v>14</v>
-      </c>
-      <c r="G40" t="s">
+        <v>30</v>
+      </c>
+      <c r="G40" s="30" t="s">
         <v>15</v>
       </c>
       <c r="H40">
@@ -4197,93 +4187,93 @@
         <v>1</v>
       </c>
       <c r="J40" s="54" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B41" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="C41" t="s">
-        <v>57</v>
+        <v>12</v>
       </c>
       <c r="D41" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E41" t="s">
         <v>47</v>
       </c>
       <c r="F41" t="s">
-        <v>14</v>
-      </c>
-      <c r="G41" t="s">
+        <v>32</v>
+      </c>
+      <c r="G41" s="30" t="s">
         <v>15</v>
       </c>
       <c r="H41">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="I41">
         <v>1</v>
       </c>
       <c r="J41" s="54" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B42" t="s">
-        <v>21</v>
+        <v>402</v>
       </c>
       <c r="C42" t="s">
-        <v>57</v>
+        <v>12</v>
       </c>
       <c r="D42" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E42" t="s">
         <v>47</v>
       </c>
       <c r="F42" t="s">
-        <v>14</v>
-      </c>
-      <c r="G42" t="s">
+        <v>30</v>
+      </c>
+      <c r="G42" s="30" t="s">
         <v>15</v>
       </c>
       <c r="H42">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="I42">
         <v>1</v>
       </c>
       <c r="J42" s="54" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B43" t="s">
-        <v>11</v>
+        <v>402</v>
       </c>
       <c r="C43" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D43" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E43" t="s">
         <v>47</v>
       </c>
       <c r="F43" t="s">
-        <v>14</v>
-      </c>
-      <c r="G43" t="s">
+        <v>32</v>
+      </c>
+      <c r="G43" s="30" t="s">
         <v>15</v>
       </c>
       <c r="H43">
@@ -4293,18 +4283,18 @@
         <v>1</v>
       </c>
       <c r="J43" s="54" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B44" t="s">
         <v>11</v>
       </c>
       <c r="C44" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D44" t="s">
         <v>46</v>
@@ -4319,24 +4309,24 @@
         <v>15</v>
       </c>
       <c r="H44">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="I44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J44" s="54" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B45" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C45" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="D45" t="s">
         <v>46</v>
@@ -4354,21 +4344,21 @@
         <v>-1</v>
       </c>
       <c r="I45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J45" s="54" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B46" t="s">
-        <v>68</v>
+        <v>21</v>
       </c>
       <c r="C46" t="s">
-        <v>12</v>
+        <v>57</v>
       </c>
       <c r="D46" t="s">
         <v>46</v>
@@ -4389,18 +4379,18 @@
         <v>1</v>
       </c>
       <c r="J46" s="54" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="B47" t="s">
         <v>11</v>
       </c>
       <c r="C47" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="D47" t="s">
         <v>46</v>
@@ -4409,10 +4399,10 @@
         <v>47</v>
       </c>
       <c r="F47" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="G47" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="H47">
         <v>1</v>
@@ -4421,18 +4411,18 @@
         <v>1</v>
       </c>
       <c r="J47" s="54" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B48" t="s">
-        <v>68</v>
+        <v>11</v>
       </c>
       <c r="C48" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="D48" t="s">
         <v>46</v>
@@ -4441,30 +4431,30 @@
         <v>47</v>
       </c>
       <c r="F48" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="G48" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="H48">
         <v>-1</v>
       </c>
       <c r="I48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J48" s="54" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="B49" t="s">
         <v>11</v>
       </c>
       <c r="C49" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="D49" t="s">
         <v>46</v>
@@ -4473,19 +4463,19 @@
         <v>47</v>
       </c>
       <c r="F49" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="G49" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="H49">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="I49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J49" s="54" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
@@ -4505,10 +4495,10 @@
         <v>47</v>
       </c>
       <c r="F50" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="G50" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="H50">
         <v>-1</v>
@@ -4521,14 +4511,14 @@
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A51" s="30" t="s">
-        <v>70</v>
+      <c r="A51" t="s">
+        <v>54</v>
       </c>
       <c r="B51" t="s">
         <v>11</v>
       </c>
       <c r="C51" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="D51" t="s">
         <v>46</v>
@@ -4537,10 +4527,10 @@
         <v>47</v>
       </c>
       <c r="F51" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="G51" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="H51">
         <v>1</v>
@@ -4549,18 +4539,18 @@
         <v>1</v>
       </c>
       <c r="J51" s="54" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A52" s="30" t="s">
-        <v>70</v>
+      <c r="A52" t="s">
+        <v>67</v>
       </c>
       <c r="B52" t="s">
-        <v>18</v>
+        <v>68</v>
       </c>
       <c r="C52" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="D52" t="s">
         <v>46</v>
@@ -4569,10 +4559,10 @@
         <v>47</v>
       </c>
       <c r="F52" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="G52" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="H52">
         <v>-1</v>
@@ -4581,18 +4571,18 @@
         <v>1</v>
       </c>
       <c r="J52" s="54" t="s">
-        <v>41</v>
+        <v>69</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A53" s="30" t="s">
-        <v>70</v>
+      <c r="A53" t="s">
+        <v>54</v>
       </c>
       <c r="B53" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C53" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="D53" t="s">
         <v>46</v>
@@ -4601,30 +4591,30 @@
         <v>47</v>
       </c>
       <c r="F53" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="G53" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="H53">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="I53">
         <v>1</v>
       </c>
       <c r="J53" s="54" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A54" s="30" t="s">
-        <v>70</v>
+      <c r="A54" t="s">
+        <v>67</v>
       </c>
       <c r="B54" t="s">
-        <v>11</v>
+        <v>68</v>
       </c>
       <c r="C54" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="D54" t="s">
         <v>46</v>
@@ -4633,19 +4623,19 @@
         <v>47</v>
       </c>
       <c r="F54" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G54" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="H54">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="I54">
         <v>1</v>
       </c>
       <c r="J54" s="54" t="s">
-        <v>40</v>
+        <v>69</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
@@ -4653,7 +4643,7 @@
         <v>70</v>
       </c>
       <c r="B55" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C55" t="s">
         <v>39</v>
@@ -4665,19 +4655,19 @@
         <v>47</v>
       </c>
       <c r="F55" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="G55" t="s">
         <v>15</v>
       </c>
       <c r="H55">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="I55">
         <v>1</v>
       </c>
       <c r="J55" s="54" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
@@ -4685,7 +4675,7 @@
         <v>70</v>
       </c>
       <c r="B56" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C56" t="s">
         <v>39</v>
@@ -4697,7 +4687,7 @@
         <v>47</v>
       </c>
       <c r="F56" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="G56" t="s">
         <v>15</v>
@@ -4709,7 +4699,7 @@
         <v>1</v>
       </c>
       <c r="J56" s="54" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.2">
@@ -4717,10 +4707,10 @@
         <v>70</v>
       </c>
       <c r="B57" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C57" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="D57" t="s">
         <v>46</v>
@@ -4729,19 +4719,19 @@
         <v>47</v>
       </c>
       <c r="F57" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="G57" t="s">
         <v>15</v>
       </c>
       <c r="H57">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="I57">
         <v>1</v>
       </c>
       <c r="J57" s="54" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
@@ -4749,10 +4739,10 @@
         <v>70</v>
       </c>
       <c r="B58" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C58" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="D58" t="s">
         <v>46</v>
@@ -4761,19 +4751,19 @@
         <v>47</v>
       </c>
       <c r="F58" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G58" t="s">
         <v>15</v>
       </c>
       <c r="H58">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="I58">
         <v>1</v>
       </c>
       <c r="J58" s="54" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
@@ -4781,10 +4771,10 @@
         <v>70</v>
       </c>
       <c r="B59" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C59" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="D59" t="s">
         <v>46</v>
@@ -4793,7 +4783,7 @@
         <v>47</v>
       </c>
       <c r="F59" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G59" t="s">
         <v>15</v>
@@ -4805,29 +4795,29 @@
         <v>1</v>
       </c>
       <c r="J59" s="54" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>52</v>
+      <c r="A60" s="30" t="s">
+        <v>70</v>
       </c>
       <c r="B60" t="s">
-        <v>413</v>
+        <v>21</v>
       </c>
       <c r="C60" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="D60" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E60" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
       <c r="F60" t="s">
         <v>30</v>
       </c>
-      <c r="G60" s="30" t="s">
+      <c r="G60" t="s">
         <v>15</v>
       </c>
       <c r="H60">
@@ -4837,47 +4827,47 @@
         <v>1</v>
       </c>
       <c r="J60" s="54" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>52</v>
+      <c r="A61" s="30" t="s">
+        <v>70</v>
       </c>
       <c r="B61" t="s">
-        <v>413</v>
+        <v>11</v>
       </c>
       <c r="C61" t="s">
         <v>12</v>
       </c>
       <c r="D61" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E61" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
       <c r="F61" t="s">
         <v>32</v>
       </c>
-      <c r="G61" s="30" t="s">
+      <c r="G61" t="s">
         <v>15</v>
       </c>
       <c r="H61">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="I61">
         <v>1</v>
       </c>
       <c r="J61" s="54" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>54</v>
+      <c r="A62" s="30" t="s">
+        <v>70</v>
       </c>
       <c r="B62" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C62" t="s">
         <v>12</v>
@@ -4886,10 +4876,10 @@
         <v>46</v>
       </c>
       <c r="E62" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
       <c r="F62" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="G62" t="s">
         <v>15</v>
@@ -4901,93 +4891,93 @@
         <v>1</v>
       </c>
       <c r="J62" s="54" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>56</v>
+      <c r="A63" s="30" t="s">
+        <v>70</v>
       </c>
       <c r="B63" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C63" t="s">
-        <v>57</v>
+        <v>12</v>
       </c>
       <c r="D63" t="s">
         <v>46</v>
       </c>
       <c r="E63" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
       <c r="F63" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="G63" t="s">
         <v>15</v>
       </c>
       <c r="H63">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="I63">
         <v>1</v>
       </c>
       <c r="J63" s="54" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B64" t="s">
-        <v>21</v>
+        <v>402</v>
       </c>
       <c r="C64" t="s">
-        <v>57</v>
+        <v>12</v>
       </c>
       <c r="D64" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E64" t="s">
         <v>71</v>
       </c>
       <c r="F64" t="s">
-        <v>14</v>
-      </c>
-      <c r="G64" t="s">
+        <v>30</v>
+      </c>
+      <c r="G64" s="30" t="s">
         <v>15</v>
       </c>
       <c r="H64">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="I64">
         <v>1</v>
       </c>
       <c r="J64" s="54" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B65" t="s">
-        <v>11</v>
+        <v>402</v>
       </c>
       <c r="C65" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D65" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E65" t="s">
         <v>71</v>
       </c>
       <c r="F65" t="s">
-        <v>14</v>
-      </c>
-      <c r="G65" t="s">
+        <v>32</v>
+      </c>
+      <c r="G65" s="30" t="s">
         <v>15</v>
       </c>
       <c r="H65">
@@ -4997,18 +4987,18 @@
         <v>1</v>
       </c>
       <c r="J65" s="54" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B66" t="s">
         <v>11</v>
       </c>
       <c r="C66" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D66" t="s">
         <v>46</v>
@@ -5023,24 +5013,24 @@
         <v>15</v>
       </c>
       <c r="H66">
+        <v>-1</v>
+      </c>
+      <c r="I66">
         <v>1</v>
       </c>
-      <c r="I66">
-        <v>0</v>
-      </c>
       <c r="J66" s="54" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B67" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C67" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="D67" t="s">
         <v>46</v>
@@ -5058,21 +5048,21 @@
         <v>1</v>
       </c>
       <c r="I67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J67" s="54" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B68" t="s">
-        <v>68</v>
+        <v>21</v>
       </c>
       <c r="C68" t="s">
-        <v>12</v>
+        <v>57</v>
       </c>
       <c r="D68" t="s">
         <v>46</v>
@@ -5093,18 +5083,18 @@
         <v>1</v>
       </c>
       <c r="J68" s="54" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="B69" t="s">
         <v>11</v>
       </c>
       <c r="C69" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="D69" t="s">
         <v>46</v>
@@ -5113,10 +5103,10 @@
         <v>71</v>
       </c>
       <c r="F69" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="G69" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="H69">
         <v>-1</v>
@@ -5125,18 +5115,18 @@
         <v>1</v>
       </c>
       <c r="J69" s="54" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B70" t="s">
-        <v>68</v>
+        <v>11</v>
       </c>
       <c r="C70" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="D70" t="s">
         <v>46</v>
@@ -5145,30 +5135,30 @@
         <v>71</v>
       </c>
       <c r="F70" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="G70" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="H70">
         <v>1</v>
       </c>
       <c r="I70">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J70" s="54" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="B71" t="s">
         <v>11</v>
       </c>
       <c r="C71" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="D71" t="s">
         <v>46</v>
@@ -5177,19 +5167,19 @@
         <v>71</v>
       </c>
       <c r="F71" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="G71" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="H71">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="I71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J71" s="54" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.2">
@@ -5209,10 +5199,10 @@
         <v>71</v>
       </c>
       <c r="F72" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="G72" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="H72">
         <v>1</v>
@@ -5226,10 +5216,10 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="B73" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="C73" t="s">
         <v>12</v>
@@ -5238,7 +5228,7 @@
         <v>46</v>
       </c>
       <c r="E73" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F73" t="s">
         <v>30</v>
@@ -5247,21 +5237,21 @@
         <v>31</v>
       </c>
       <c r="H73">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="I73">
         <v>1</v>
       </c>
       <c r="J73" s="54" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="B74" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="C74" t="s">
         <v>12</v>
@@ -5270,10 +5260,10 @@
         <v>46</v>
       </c>
       <c r="E74" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F74" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G74" t="s">
         <v>31</v>
@@ -5285,62 +5275,62 @@
         <v>1</v>
       </c>
       <c r="J74" s="54" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B75" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="C75" t="s">
         <v>12</v>
       </c>
       <c r="D75" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E75" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F75" t="s">
-        <v>30</v>
-      </c>
-      <c r="G75" s="30" t="s">
-        <v>15</v>
+        <v>32</v>
+      </c>
+      <c r="G75" t="s">
+        <v>31</v>
       </c>
       <c r="H75">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="I75">
         <v>1</v>
       </c>
       <c r="J75" s="54" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="B76" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="C76" t="s">
         <v>12</v>
       </c>
       <c r="D76" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E76" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F76" t="s">
         <v>32</v>
       </c>
-      <c r="G76" s="30" t="s">
-        <v>15</v>
+      <c r="G76" t="s">
+        <v>31</v>
       </c>
       <c r="H76">
         <v>1</v>
@@ -5349,21 +5339,21 @@
         <v>1</v>
       </c>
       <c r="J76" s="54" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B77" t="s">
-        <v>413</v>
+        <v>43</v>
       </c>
       <c r="C77" t="s">
         <v>12</v>
       </c>
       <c r="D77" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E77" t="s">
         <v>72</v>
@@ -5371,8 +5361,8 @@
       <c r="F77" t="s">
         <v>30</v>
       </c>
-      <c r="G77" s="30" t="s">
-        <v>15</v>
+      <c r="G77" t="s">
+        <v>31</v>
       </c>
       <c r="H77">
         <v>1</v>
@@ -5381,21 +5371,21 @@
         <v>1</v>
       </c>
       <c r="J77" s="54" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B78" t="s">
-        <v>413</v>
+        <v>43</v>
       </c>
       <c r="C78" t="s">
         <v>12</v>
       </c>
       <c r="D78" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E78" t="s">
         <v>72</v>
@@ -5403,8 +5393,8 @@
       <c r="F78" t="s">
         <v>32</v>
       </c>
-      <c r="G78" s="30" t="s">
-        <v>15</v>
+      <c r="G78" t="s">
+        <v>31</v>
       </c>
       <c r="H78">
         <v>1</v>
@@ -5413,29 +5403,29 @@
         <v>1</v>
       </c>
       <c r="J78" s="54" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B79" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="C79" t="s">
         <v>12</v>
       </c>
       <c r="D79" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E79" t="s">
         <v>72</v>
       </c>
       <c r="F79" t="s">
-        <v>14</v>
-      </c>
-      <c r="G79" t="s">
+        <v>30</v>
+      </c>
+      <c r="G79" s="30" t="s">
         <v>15</v>
       </c>
       <c r="H79">
@@ -5445,93 +5435,93 @@
         <v>1</v>
       </c>
       <c r="J79" s="54" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B80" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="C80" t="s">
-        <v>57</v>
+        <v>12</v>
       </c>
       <c r="D80" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E80" t="s">
         <v>72</v>
       </c>
       <c r="F80" t="s">
-        <v>14</v>
-      </c>
-      <c r="G80" t="s">
+        <v>32</v>
+      </c>
+      <c r="G80" s="30" t="s">
         <v>15</v>
       </c>
       <c r="H80">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="I80">
         <v>1</v>
       </c>
       <c r="J80" s="54" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B81" t="s">
-        <v>21</v>
+        <v>402</v>
       </c>
       <c r="C81" t="s">
-        <v>57</v>
+        <v>12</v>
       </c>
       <c r="D81" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E81" t="s">
         <v>72</v>
       </c>
       <c r="F81" t="s">
-        <v>14</v>
-      </c>
-      <c r="G81" t="s">
+        <v>30</v>
+      </c>
+      <c r="G81" s="30" t="s">
         <v>15</v>
       </c>
       <c r="H81">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="I81">
         <v>1</v>
       </c>
       <c r="J81" s="54" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B82" t="s">
-        <v>11</v>
+        <v>402</v>
       </c>
       <c r="C82" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D82" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E82" t="s">
         <v>72</v>
       </c>
       <c r="F82" t="s">
-        <v>14</v>
-      </c>
-      <c r="G82" t="s">
+        <v>32</v>
+      </c>
+      <c r="G82" s="30" t="s">
         <v>15</v>
       </c>
       <c r="H82">
@@ -5541,18 +5531,18 @@
         <v>1</v>
       </c>
       <c r="J82" s="54" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B83" t="s">
         <v>11</v>
       </c>
       <c r="C83" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D83" t="s">
         <v>46</v>
@@ -5567,24 +5557,24 @@
         <v>15</v>
       </c>
       <c r="H83">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="I83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J83" s="54" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B84" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C84" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="D84" t="s">
         <v>46</v>
@@ -5602,21 +5592,21 @@
         <v>-1</v>
       </c>
       <c r="I84">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J84" s="54" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B85" t="s">
-        <v>68</v>
+        <v>21</v>
       </c>
       <c r="C85" t="s">
-        <v>12</v>
+        <v>57</v>
       </c>
       <c r="D85" t="s">
         <v>46</v>
@@ -5637,18 +5627,18 @@
         <v>1</v>
       </c>
       <c r="J85" s="54" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="B86" t="s">
         <v>11</v>
       </c>
       <c r="C86" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="D86" t="s">
         <v>46</v>
@@ -5657,10 +5647,10 @@
         <v>72</v>
       </c>
       <c r="F86" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="G86" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="H86">
         <v>1</v>
@@ -5669,18 +5659,18 @@
         <v>1</v>
       </c>
       <c r="J86" s="54" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B87" t="s">
-        <v>68</v>
+        <v>11</v>
       </c>
       <c r="C87" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="D87" t="s">
         <v>46</v>
@@ -5689,30 +5679,30 @@
         <v>72</v>
       </c>
       <c r="F87" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="G87" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="H87">
         <v>-1</v>
       </c>
       <c r="I87">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J87" s="54" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="B88" t="s">
         <v>11</v>
       </c>
       <c r="C88" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="D88" t="s">
         <v>46</v>
@@ -5721,19 +5711,19 @@
         <v>72</v>
       </c>
       <c r="F88" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="G88" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="H88">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="I88">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J88" s="54" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.2">
@@ -5753,10 +5743,10 @@
         <v>72</v>
       </c>
       <c r="F89" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="G89" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="H89">
         <v>-1</v>
@@ -5769,14 +5759,14 @@
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A90" s="30" t="s">
-        <v>70</v>
+      <c r="A90" t="s">
+        <v>54</v>
       </c>
       <c r="B90" t="s">
         <v>11</v>
       </c>
       <c r="C90" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="D90" t="s">
         <v>46</v>
@@ -5785,10 +5775,10 @@
         <v>72</v>
       </c>
       <c r="F90" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="G90" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="H90">
         <v>1</v>
@@ -5797,18 +5787,18 @@
         <v>1</v>
       </c>
       <c r="J90" s="54" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A91" s="30" t="s">
-        <v>70</v>
+      <c r="A91" t="s">
+        <v>67</v>
       </c>
       <c r="B91" t="s">
-        <v>18</v>
+        <v>68</v>
       </c>
       <c r="C91" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="D91" t="s">
         <v>46</v>
@@ -5817,10 +5807,10 @@
         <v>72</v>
       </c>
       <c r="F91" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="G91" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="H91">
         <v>-1</v>
@@ -5829,18 +5819,18 @@
         <v>1</v>
       </c>
       <c r="J91" s="54" t="s">
-        <v>41</v>
+        <v>69</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A92" s="30" t="s">
-        <v>70</v>
+      <c r="A92" t="s">
+        <v>54</v>
       </c>
       <c r="B92" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C92" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="D92" t="s">
         <v>46</v>
@@ -5849,30 +5839,30 @@
         <v>72</v>
       </c>
       <c r="F92" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="G92" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="H92">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="I92">
         <v>1</v>
       </c>
       <c r="J92" s="54" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A93" s="30" t="s">
-        <v>70</v>
+      <c r="A93" t="s">
+        <v>67</v>
       </c>
       <c r="B93" t="s">
-        <v>11</v>
+        <v>68</v>
       </c>
       <c r="C93" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="D93" t="s">
         <v>46</v>
@@ -5881,19 +5871,19 @@
         <v>72</v>
       </c>
       <c r="F93" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G93" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="H93">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="I93">
         <v>1</v>
       </c>
       <c r="J93" s="54" t="s">
-        <v>40</v>
+        <v>69</v>
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.2">
@@ -5901,7 +5891,7 @@
         <v>70</v>
       </c>
       <c r="B94" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C94" t="s">
         <v>39</v>
@@ -5913,19 +5903,19 @@
         <v>72</v>
       </c>
       <c r="F94" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="G94" t="s">
         <v>15</v>
       </c>
       <c r="H94">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="I94">
         <v>1</v>
       </c>
       <c r="J94" s="54" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.2">
@@ -5933,7 +5923,7 @@
         <v>70</v>
       </c>
       <c r="B95" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C95" t="s">
         <v>39</v>
@@ -5945,7 +5935,7 @@
         <v>72</v>
       </c>
       <c r="F95" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="G95" t="s">
         <v>15</v>
@@ -5957,7 +5947,7 @@
         <v>1</v>
       </c>
       <c r="J95" s="54" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.2">
@@ -5965,10 +5955,10 @@
         <v>70</v>
       </c>
       <c r="B96" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C96" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="D96" t="s">
         <v>46</v>
@@ -5977,19 +5967,19 @@
         <v>72</v>
       </c>
       <c r="F96" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="G96" t="s">
         <v>15</v>
       </c>
       <c r="H96">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="I96">
         <v>1</v>
       </c>
       <c r="J96" s="54" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.2">
@@ -5997,10 +5987,10 @@
         <v>70</v>
       </c>
       <c r="B97" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C97" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="D97" t="s">
         <v>46</v>
@@ -6009,19 +5999,19 @@
         <v>72</v>
       </c>
       <c r="F97" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G97" t="s">
         <v>15</v>
       </c>
       <c r="H97">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="I97">
         <v>1</v>
       </c>
       <c r="J97" s="54" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.2">
@@ -6029,10 +6019,10 @@
         <v>70</v>
       </c>
       <c r="B98" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C98" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="D98" t="s">
         <v>46</v>
@@ -6041,7 +6031,7 @@
         <v>72</v>
       </c>
       <c r="F98" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G98" t="s">
         <v>15</v>
@@ -6053,11 +6043,139 @@
         <v>1</v>
       </c>
       <c r="J98" s="54" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A99" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="B99" t="s">
+        <v>21</v>
+      </c>
+      <c r="C99" t="s">
+        <v>39</v>
+      </c>
+      <c r="D99" t="s">
+        <v>46</v>
+      </c>
+      <c r="E99" t="s">
+        <v>72</v>
+      </c>
+      <c r="F99" t="s">
+        <v>30</v>
+      </c>
+      <c r="G99" t="s">
+        <v>15</v>
+      </c>
+      <c r="H99">
+        <v>-1</v>
+      </c>
+      <c r="I99">
+        <v>1</v>
+      </c>
+      <c r="J99" s="54" t="s">
         <v>42</v>
       </c>
     </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A100" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="B100" t="s">
+        <v>11</v>
+      </c>
+      <c r="C100" t="s">
+        <v>12</v>
+      </c>
+      <c r="D100" t="s">
+        <v>46</v>
+      </c>
+      <c r="E100" t="s">
+        <v>72</v>
+      </c>
+      <c r="F100" t="s">
+        <v>32</v>
+      </c>
+      <c r="G100" t="s">
+        <v>15</v>
+      </c>
+      <c r="H100">
+        <v>1</v>
+      </c>
+      <c r="I100">
+        <v>1</v>
+      </c>
+      <c r="J100" s="54" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A101" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="B101" t="s">
+        <v>18</v>
+      </c>
+      <c r="C101" t="s">
+        <v>12</v>
+      </c>
+      <c r="D101" t="s">
+        <v>46</v>
+      </c>
+      <c r="E101" t="s">
+        <v>72</v>
+      </c>
+      <c r="F101" t="s">
+        <v>32</v>
+      </c>
+      <c r="G101" t="s">
+        <v>15</v>
+      </c>
+      <c r="H101">
+        <v>-1</v>
+      </c>
+      <c r="I101">
+        <v>1</v>
+      </c>
+      <c r="J101" s="54" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A102" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="B102" t="s">
+        <v>21</v>
+      </c>
+      <c r="C102" t="s">
+        <v>12</v>
+      </c>
+      <c r="D102" t="s">
+        <v>46</v>
+      </c>
+      <c r="E102" t="s">
+        <v>72</v>
+      </c>
+      <c r="F102" t="s">
+        <v>32</v>
+      </c>
+      <c r="G102" t="s">
+        <v>15</v>
+      </c>
+      <c r="H102">
+        <v>-1</v>
+      </c>
+      <c r="I102">
+        <v>1</v>
+      </c>
+      <c r="J102" s="54" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J98" xr:uid="{7838926A-4835-1A4C-A577-1C02FA1EB720}"/>
+  <autoFilter ref="A1:J102" xr:uid="{7838926A-4835-1A4C-A577-1C02FA1EB720}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
@@ -15305,7 +15423,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15429,7 +15547,7 @@
         <v>45688</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>240</v>
@@ -15464,7 +15582,7 @@
         <v>45688</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>240</v>
@@ -15499,7 +15617,7 @@
         <v>45716</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>240</v>
@@ -15534,7 +15652,7 @@
         <v>45716</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>240</v>
@@ -15565,190 +15683,6 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C59D3D0B-BDA7-C849-9A02-F348974FBECC}">
-  <sheetPr codeName="Hoja16">
-    <tabColor rgb="FFC00000"/>
-  </sheetPr>
-  <dimension ref="A1:N4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.1640625" customWidth="1"/>
-    <col min="10" max="10" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.83203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>398</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>402</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>403</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>404</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>405</v>
-      </c>
-      <c r="B2" s="14">
-        <v>45657</v>
-      </c>
-      <c r="F2" t="s">
-        <v>406</v>
-      </c>
-      <c r="G2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H2" t="s">
-        <v>407</v>
-      </c>
-      <c r="I2" t="s">
-        <v>408</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="L2" t="s">
-        <v>154</v>
-      </c>
-      <c r="M2" t="s">
-        <v>115</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>409</v>
-      </c>
-      <c r="B3" s="14">
-        <v>45657</v>
-      </c>
-      <c r="F3" t="s">
-        <v>406</v>
-      </c>
-      <c r="G3" t="s">
-        <v>46</v>
-      </c>
-      <c r="H3" t="s">
-        <v>410</v>
-      </c>
-      <c r="I3" t="s">
-        <v>411</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="L3" t="s">
-        <v>154</v>
-      </c>
-      <c r="M3" t="s">
-        <v>115</v>
-      </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>412</v>
-      </c>
-      <c r="B4" s="14">
-        <v>45657</v>
-      </c>
-      <c r="F4" t="s">
-        <v>406</v>
-      </c>
-      <c r="G4" t="s">
-        <v>50</v>
-      </c>
-      <c r="H4" t="s">
-        <v>413</v>
-      </c>
-      <c r="I4" t="s">
-        <v>408</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="L4" t="s">
-        <v>154</v>
-      </c>
-      <c r="M4" t="s">
-        <v>115</v>
-      </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -15928,7 +15862,7 @@
   <sheetData>
     <row r="1" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>416</v>
+        <v>405</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>83</v>
@@ -15955,7 +15889,7 @@
         <v>87</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>417</v>
+        <v>406</v>
       </c>
       <c r="K1" s="5" t="s">
         <v>88</v>
@@ -15996,7 +15930,7 @@
         <v>92</v>
       </c>
       <c r="J2" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K2" s="9">
         <v>0.1</v>
@@ -16037,7 +15971,7 @@
         <v>92</v>
       </c>
       <c r="J3" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K3" s="9">
         <v>0.2</v>
@@ -16078,7 +16012,7 @@
         <v>92</v>
       </c>
       <c r="J4" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K4" s="9">
         <v>1.1000000000000001</v>
@@ -16119,7 +16053,7 @@
         <v>92</v>
       </c>
       <c r="J5" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K5" s="9">
         <v>0.13</v>
@@ -16160,7 +16094,7 @@
         <v>92</v>
       </c>
       <c r="J6" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K6" s="9">
         <v>0.15</v>
@@ -16201,7 +16135,7 @@
         <v>92</v>
       </c>
       <c r="J7" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K7" s="9">
         <v>0.7</v>
@@ -16242,7 +16176,7 @@
         <v>92</v>
       </c>
       <c r="J8" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K8" s="9">
         <v>0.1</v>
@@ -16283,7 +16217,7 @@
         <v>92</v>
       </c>
       <c r="J9" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K9" s="9">
         <v>0.2</v>
@@ -16324,7 +16258,7 @@
         <v>92</v>
       </c>
       <c r="J10" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K10" s="9">
         <v>1.1000000000000001</v>
@@ -16365,7 +16299,7 @@
         <v>92</v>
       </c>
       <c r="J11" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K11" s="9">
         <v>0.13</v>
@@ -16406,7 +16340,7 @@
         <v>92</v>
       </c>
       <c r="J12" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K12" s="9">
         <v>0.15</v>
@@ -16447,7 +16381,7 @@
         <v>92</v>
       </c>
       <c r="J13" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K13" s="9">
         <v>0.7</v>
@@ -16488,7 +16422,7 @@
         <v>92</v>
       </c>
       <c r="J14" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K14" s="9">
         <v>0.1</v>
@@ -16529,7 +16463,7 @@
         <v>92</v>
       </c>
       <c r="J15" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K15" s="9">
         <v>0.2</v>
@@ -16570,7 +16504,7 @@
         <v>92</v>
       </c>
       <c r="J16" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K16" s="9">
         <v>1.1000000000000001</v>
@@ -16611,7 +16545,7 @@
         <v>92</v>
       </c>
       <c r="J17" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K17" s="9">
         <v>0.13</v>
@@ -16652,7 +16586,7 @@
         <v>92</v>
       </c>
       <c r="J18" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K18" s="9">
         <v>0.15</v>
@@ -16693,7 +16627,7 @@
         <v>92</v>
       </c>
       <c r="J19" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K19" s="9">
         <v>0.7</v>
@@ -16734,7 +16668,7 @@
         <v>92</v>
       </c>
       <c r="J20" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K20" s="9">
         <v>0.1</v>
@@ -16775,7 +16709,7 @@
         <v>92</v>
       </c>
       <c r="J21" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K21" s="9">
         <v>0.2</v>
@@ -16816,7 +16750,7 @@
         <v>92</v>
       </c>
       <c r="J22" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K22" s="9">
         <v>1.1000000000000001</v>
@@ -16857,7 +16791,7 @@
         <v>92</v>
       </c>
       <c r="J23" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K23" s="9">
         <v>0.13</v>
@@ -16898,7 +16832,7 @@
         <v>92</v>
       </c>
       <c r="J24" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K24" s="9">
         <v>0.15</v>
@@ -16939,7 +16873,7 @@
         <v>92</v>
       </c>
       <c r="J25" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K25" s="9">
         <v>0.7</v>
@@ -16980,7 +16914,7 @@
         <v>92</v>
       </c>
       <c r="J26" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K26" s="9">
         <v>0</v>
@@ -17021,7 +16955,7 @@
         <v>92</v>
       </c>
       <c r="J27" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K27" s="9">
         <v>0</v>
@@ -17062,7 +16996,7 @@
         <v>92</v>
       </c>
       <c r="J28" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K28" s="9">
         <v>0</v>
@@ -17103,7 +17037,7 @@
         <v>92</v>
       </c>
       <c r="J29" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K29" s="9">
         <v>0</v>
@@ -17144,7 +17078,7 @@
         <v>92</v>
       </c>
       <c r="J30" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K30" s="9">
         <v>0.1</v>
@@ -17185,7 +17119,7 @@
         <v>92</v>
       </c>
       <c r="J31" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K31" s="9">
         <v>0.2</v>
@@ -17226,7 +17160,7 @@
         <v>92</v>
       </c>
       <c r="J32" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K32" s="9">
         <v>1.1000000000000001</v>
@@ -17267,7 +17201,7 @@
         <v>92</v>
       </c>
       <c r="J33" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K33" s="9">
         <v>0.13</v>
@@ -17308,7 +17242,7 @@
         <v>92</v>
       </c>
       <c r="J34" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K34" s="9">
         <v>0.15</v>
@@ -17349,7 +17283,7 @@
         <v>92</v>
       </c>
       <c r="J35" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K35" s="9">
         <v>0.7</v>
@@ -17390,7 +17324,7 @@
         <v>92</v>
       </c>
       <c r="J36" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K36" s="9">
         <v>0.1</v>
@@ -17431,7 +17365,7 @@
         <v>92</v>
       </c>
       <c r="J37" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K37" s="9">
         <v>0.2</v>
@@ -17472,7 +17406,7 @@
         <v>92</v>
       </c>
       <c r="J38" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K38" s="9">
         <v>1.1000000000000001</v>
@@ -17513,7 +17447,7 @@
         <v>92</v>
       </c>
       <c r="J39" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K39" s="9">
         <v>0.13</v>
@@ -17554,7 +17488,7 @@
         <v>92</v>
       </c>
       <c r="J40" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K40" s="9">
         <v>0.15</v>
@@ -17595,7 +17529,7 @@
         <v>92</v>
       </c>
       <c r="J41" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K41" s="9">
         <v>0.7</v>
@@ -17636,7 +17570,7 @@
         <v>92</v>
       </c>
       <c r="J42" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K42" s="9">
         <v>0.1</v>
@@ -17677,7 +17611,7 @@
         <v>92</v>
       </c>
       <c r="J43" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K43" s="9">
         <v>0.2</v>
@@ -17718,7 +17652,7 @@
         <v>92</v>
       </c>
       <c r="J44" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K44" s="9">
         <v>1.1000000000000001</v>
@@ -17759,7 +17693,7 @@
         <v>92</v>
       </c>
       <c r="J45" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K45" s="9">
         <v>0.13</v>
@@ -17800,7 +17734,7 @@
         <v>92</v>
       </c>
       <c r="J46" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K46" s="9">
         <v>0.15</v>
@@ -17841,7 +17775,7 @@
         <v>92</v>
       </c>
       <c r="J47" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K47" s="9">
         <v>0.7</v>
@@ -17882,7 +17816,7 @@
         <v>92</v>
       </c>
       <c r="J48" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K48" s="9">
         <v>0.1</v>
@@ -17923,7 +17857,7 @@
         <v>92</v>
       </c>
       <c r="J49" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K49" s="9">
         <v>0.2</v>
@@ -17964,7 +17898,7 @@
         <v>92</v>
       </c>
       <c r="J50" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K50" s="9">
         <v>1.1000000000000001</v>
@@ -18005,7 +17939,7 @@
         <v>92</v>
       </c>
       <c r="J51" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K51" s="9">
         <v>0.13</v>
@@ -18046,7 +17980,7 @@
         <v>92</v>
       </c>
       <c r="J52" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K52" s="9">
         <v>0.15</v>
@@ -18087,7 +18021,7 @@
         <v>92</v>
       </c>
       <c r="J53" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K53" s="9">
         <v>0.7</v>
@@ -18128,7 +18062,7 @@
         <v>92</v>
       </c>
       <c r="J54" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K54" s="9">
         <v>0</v>
@@ -18169,7 +18103,7 @@
         <v>92</v>
       </c>
       <c r="J55" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K55" s="9">
         <v>0</v>
@@ -18210,7 +18144,7 @@
         <v>92</v>
       </c>
       <c r="J56" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K56" s="9">
         <v>0</v>
@@ -18251,7 +18185,7 @@
         <v>92</v>
       </c>
       <c r="J57" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K57" s="9">
         <v>0</v>
@@ -18292,7 +18226,7 @@
         <v>92</v>
       </c>
       <c r="J58" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K58" s="9">
         <v>0.1</v>
@@ -18333,7 +18267,7 @@
         <v>92</v>
       </c>
       <c r="J59" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K59" s="9">
         <v>0.2</v>
@@ -18374,7 +18308,7 @@
         <v>92</v>
       </c>
       <c r="J60" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K60" s="9">
         <v>1.1000000000000001</v>
@@ -18415,7 +18349,7 @@
         <v>92</v>
       </c>
       <c r="J61" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K61" s="9">
         <v>0.13</v>
@@ -18456,7 +18390,7 @@
         <v>92</v>
       </c>
       <c r="J62" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K62" s="9">
         <v>0.15</v>
@@ -18497,7 +18431,7 @@
         <v>92</v>
       </c>
       <c r="J63" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K63" s="9">
         <v>0.7</v>
@@ -18538,7 +18472,7 @@
         <v>92</v>
       </c>
       <c r="J64" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K64" s="9">
         <v>0.1</v>
@@ -18579,7 +18513,7 @@
         <v>92</v>
       </c>
       <c r="J65" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K65" s="9">
         <v>0.2</v>
@@ -18620,7 +18554,7 @@
         <v>92</v>
       </c>
       <c r="J66" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K66" s="9">
         <v>1.1000000000000001</v>
@@ -18661,7 +18595,7 @@
         <v>92</v>
       </c>
       <c r="J67" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K67" s="9">
         <v>0.13</v>
@@ -18702,7 +18636,7 @@
         <v>92</v>
       </c>
       <c r="J68" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K68" s="9">
         <v>0.15</v>
@@ -18743,7 +18677,7 @@
         <v>92</v>
       </c>
       <c r="J69" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K69" s="9">
         <v>0.7</v>
@@ -18784,7 +18718,7 @@
         <v>92</v>
       </c>
       <c r="J70" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K70" s="9">
         <v>0.1</v>
@@ -18825,7 +18759,7 @@
         <v>92</v>
       </c>
       <c r="J71" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K71" s="9">
         <v>0.2</v>
@@ -18866,7 +18800,7 @@
         <v>92</v>
       </c>
       <c r="J72" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K72" s="9">
         <v>1.1000000000000001</v>
@@ -18907,7 +18841,7 @@
         <v>92</v>
       </c>
       <c r="J73" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K73" s="9">
         <v>0.13</v>
@@ -18948,7 +18882,7 @@
         <v>92</v>
       </c>
       <c r="J74" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K74" s="9">
         <v>0.15</v>
@@ -18989,7 +18923,7 @@
         <v>92</v>
       </c>
       <c r="J75" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K75" s="9">
         <v>0.7</v>
@@ -19030,7 +18964,7 @@
         <v>92</v>
       </c>
       <c r="J76" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K76" s="9">
         <v>0.1</v>
@@ -19071,7 +19005,7 @@
         <v>92</v>
       </c>
       <c r="J77" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K77" s="9">
         <v>0.2</v>
@@ -19112,7 +19046,7 @@
         <v>92</v>
       </c>
       <c r="J78" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K78" s="9">
         <v>1.1000000000000001</v>
@@ -19153,7 +19087,7 @@
         <v>92</v>
       </c>
       <c r="J79" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K79" s="9">
         <v>0.13</v>
@@ -19194,7 +19128,7 @@
         <v>92</v>
       </c>
       <c r="J80" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K80" s="9">
         <v>0.15</v>
@@ -19235,7 +19169,7 @@
         <v>92</v>
       </c>
       <c r="J81" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K81" s="9">
         <v>0.7</v>
@@ -19276,7 +19210,7 @@
         <v>92</v>
       </c>
       <c r="J82" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K82" s="9">
         <v>0.15</v>
@@ -19317,7 +19251,7 @@
         <v>92</v>
       </c>
       <c r="J83" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K83" s="9">
         <v>0.15</v>
@@ -19358,7 +19292,7 @@
         <v>92</v>
       </c>
       <c r="J84" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K84" s="9">
         <v>0.16</v>
@@ -19399,7 +19333,7 @@
         <v>92</v>
       </c>
       <c r="J85" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K85" s="9">
         <v>0.16500000000000001</v>
@@ -19440,7 +19374,7 @@
         <v>100</v>
       </c>
       <c r="J86" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K86" s="9">
         <v>0.5</v>
@@ -19481,7 +19415,7 @@
         <v>100</v>
       </c>
       <c r="J87" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K87" s="9">
         <v>0.1</v>
@@ -19522,7 +19456,7 @@
         <v>100</v>
       </c>
       <c r="J88" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K88" s="9">
         <v>0.6</v>
@@ -19563,7 +19497,7 @@
         <v>100</v>
       </c>
       <c r="J89" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K89" s="9">
         <v>7.0000000000000007E-2</v>
@@ -19604,7 +19538,7 @@
         <v>100</v>
       </c>
       <c r="J90" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K90" s="9">
         <v>0.8</v>
@@ -19645,7 +19579,7 @@
         <v>100</v>
       </c>
       <c r="J91" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K91" s="9">
         <v>0.3</v>
@@ -19686,7 +19620,7 @@
         <v>100</v>
       </c>
       <c r="J92" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K92" s="9">
         <v>0.5</v>
@@ -19727,7 +19661,7 @@
         <v>100</v>
       </c>
       <c r="J93" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K93" s="9">
         <v>0.1</v>
@@ -19768,7 +19702,7 @@
         <v>100</v>
       </c>
       <c r="J94" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K94" s="9">
         <v>0.6</v>
@@ -19809,7 +19743,7 @@
         <v>100</v>
       </c>
       <c r="J95" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K95" s="9">
         <v>7.0000000000000007E-2</v>
@@ -19850,7 +19784,7 @@
         <v>100</v>
       </c>
       <c r="J96" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K96" s="9">
         <v>0.8</v>
@@ -19891,7 +19825,7 @@
         <v>100</v>
       </c>
       <c r="J97" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K97" s="9">
         <v>0.3</v>
@@ -19932,7 +19866,7 @@
         <v>100</v>
       </c>
       <c r="J98" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K98" s="9">
         <v>0.5</v>
@@ -19973,7 +19907,7 @@
         <v>100</v>
       </c>
       <c r="J99" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K99" s="9">
         <v>0.1</v>
@@ -20014,7 +19948,7 @@
         <v>100</v>
       </c>
       <c r="J100" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K100" s="9">
         <v>0.6</v>
@@ -20055,7 +19989,7 @@
         <v>100</v>
       </c>
       <c r="J101" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K101" s="9">
         <v>7.0000000000000007E-2</v>
@@ -20096,7 +20030,7 @@
         <v>100</v>
       </c>
       <c r="J102" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K102" s="9">
         <v>0.8</v>
@@ -20137,7 +20071,7 @@
         <v>100</v>
       </c>
       <c r="J103" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K103" s="9">
         <v>0.3</v>
@@ -20178,7 +20112,7 @@
         <v>100</v>
       </c>
       <c r="J104" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K104" s="9">
         <v>0.5</v>
@@ -20219,7 +20153,7 @@
         <v>100</v>
       </c>
       <c r="J105" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K105" s="9">
         <v>0.1</v>
@@ -20260,7 +20194,7 @@
         <v>100</v>
       </c>
       <c r="J106" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K106" s="9">
         <v>0.6</v>
@@ -20301,7 +20235,7 @@
         <v>100</v>
       </c>
       <c r="J107" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K107" s="9">
         <v>7.0000000000000007E-2</v>
@@ -20342,7 +20276,7 @@
         <v>100</v>
       </c>
       <c r="J108" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K108" s="9">
         <v>0.8</v>
@@ -20383,7 +20317,7 @@
         <v>100</v>
       </c>
       <c r="J109" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K109" s="9">
         <v>0.3</v>
@@ -20424,7 +20358,7 @@
         <v>100</v>
       </c>
       <c r="J110" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K110" s="9">
         <v>0.21</v>
@@ -20465,7 +20399,7 @@
         <v>100</v>
       </c>
       <c r="J111" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K111" s="9">
         <v>0.2</v>
@@ -20506,7 +20440,7 @@
         <v>100</v>
       </c>
       <c r="J112" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K112" s="9">
         <v>0.23</v>
@@ -20547,7 +20481,7 @@
         <v>100</v>
       </c>
       <c r="J113" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K113" s="9">
         <v>0.22</v>
@@ -20588,7 +20522,7 @@
         <v>100</v>
       </c>
       <c r="J114" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K114" s="9">
         <v>0.5</v>
@@ -20629,7 +20563,7 @@
         <v>100</v>
       </c>
       <c r="J115" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K115" s="9">
         <v>0.1</v>
@@ -20670,7 +20604,7 @@
         <v>100</v>
       </c>
       <c r="J116" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K116" s="9">
         <v>0.6</v>
@@ -20711,7 +20645,7 @@
         <v>100</v>
       </c>
       <c r="J117" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K117" s="9">
         <v>7.0000000000000007E-2</v>
@@ -20752,7 +20686,7 @@
         <v>100</v>
       </c>
       <c r="J118" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K118" s="9">
         <v>0.8</v>
@@ -20793,7 +20727,7 @@
         <v>100</v>
       </c>
       <c r="J119" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K119" s="9">
         <v>0.3</v>
@@ -20834,7 +20768,7 @@
         <v>100</v>
       </c>
       <c r="J120" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K120" s="9">
         <v>0.5</v>
@@ -20875,7 +20809,7 @@
         <v>100</v>
       </c>
       <c r="J121" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K121" s="9">
         <v>0.1</v>
@@ -20916,7 +20850,7 @@
         <v>100</v>
       </c>
       <c r="J122" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K122" s="9">
         <v>0.6</v>
@@ -20957,7 +20891,7 @@
         <v>100</v>
       </c>
       <c r="J123" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K123" s="9">
         <v>7.0000000000000007E-2</v>
@@ -20998,7 +20932,7 @@
         <v>100</v>
       </c>
       <c r="J124" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K124" s="9">
         <v>0.8</v>
@@ -21039,7 +20973,7 @@
         <v>100</v>
       </c>
       <c r="J125" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K125" s="9">
         <v>0.3</v>
@@ -21080,7 +21014,7 @@
         <v>100</v>
       </c>
       <c r="J126" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K126" s="9">
         <v>0.5</v>
@@ -21121,7 +21055,7 @@
         <v>100</v>
       </c>
       <c r="J127" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K127" s="9">
         <v>0.1</v>
@@ -21162,7 +21096,7 @@
         <v>100</v>
       </c>
       <c r="J128" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K128" s="9">
         <v>0.6</v>
@@ -21203,7 +21137,7 @@
         <v>100</v>
       </c>
       <c r="J129" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K129" s="9">
         <v>7.0000000000000007E-2</v>
@@ -21244,7 +21178,7 @@
         <v>100</v>
       </c>
       <c r="J130" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K130" s="9">
         <v>0.8</v>
@@ -21285,7 +21219,7 @@
         <v>100</v>
       </c>
       <c r="J131" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K131" s="9">
         <v>0.3</v>
@@ -21326,7 +21260,7 @@
         <v>100</v>
       </c>
       <c r="J132" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K132" s="9">
         <v>0.5</v>
@@ -21367,7 +21301,7 @@
         <v>100</v>
       </c>
       <c r="J133" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K133" s="9">
         <v>0.1</v>
@@ -21408,7 +21342,7 @@
         <v>100</v>
       </c>
       <c r="J134" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K134" s="9">
         <v>0.6</v>
@@ -21449,7 +21383,7 @@
         <v>100</v>
       </c>
       <c r="J135" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K135" s="9">
         <v>7.0000000000000007E-2</v>
@@ -21490,7 +21424,7 @@
         <v>100</v>
       </c>
       <c r="J136" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K136" s="9">
         <v>0.8</v>
@@ -21531,7 +21465,7 @@
         <v>100</v>
       </c>
       <c r="J137" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K137" s="9">
         <v>0.3</v>
@@ -21572,7 +21506,7 @@
         <v>100</v>
       </c>
       <c r="J138" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K138" s="9">
         <v>0.11</v>
@@ -21613,7 +21547,7 @@
         <v>100</v>
       </c>
       <c r="J139" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K139" s="9">
         <v>0.13</v>
@@ -21654,7 +21588,7 @@
         <v>100</v>
       </c>
       <c r="J140" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K140" s="9">
         <v>0.14000000000000001</v>
@@ -21695,7 +21629,7 @@
         <v>100</v>
       </c>
       <c r="J141" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K141" s="9">
         <v>0.14000000000000001</v>
@@ -21736,7 +21670,7 @@
         <v>100</v>
       </c>
       <c r="J142" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K142" s="9">
         <v>0.5</v>
@@ -21777,7 +21711,7 @@
         <v>100</v>
       </c>
       <c r="J143" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K143" s="9">
         <v>0.1</v>
@@ -21818,7 +21752,7 @@
         <v>100</v>
       </c>
       <c r="J144" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K144" s="9">
         <v>0.6</v>
@@ -21859,7 +21793,7 @@
         <v>100</v>
       </c>
       <c r="J145" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K145" s="9">
         <v>7.0000000000000007E-2</v>
@@ -21900,7 +21834,7 @@
         <v>100</v>
       </c>
       <c r="J146" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K146" s="9">
         <v>0.8</v>
@@ -21941,7 +21875,7 @@
         <v>100</v>
       </c>
       <c r="J147" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K147" s="9">
         <v>0.3</v>
@@ -21982,7 +21916,7 @@
         <v>100</v>
       </c>
       <c r="J148" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K148" s="9">
         <v>0.5</v>
@@ -22023,7 +21957,7 @@
         <v>100</v>
       </c>
       <c r="J149" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K149" s="9">
         <v>0.1</v>
@@ -22064,7 +21998,7 @@
         <v>100</v>
       </c>
       <c r="J150" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K150" s="9">
         <v>0.6</v>
@@ -22105,7 +22039,7 @@
         <v>100</v>
       </c>
       <c r="J151" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K151" s="9">
         <v>7.0000000000000007E-2</v>
@@ -22146,7 +22080,7 @@
         <v>100</v>
       </c>
       <c r="J152" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K152" s="9">
         <v>0.8</v>
@@ -22187,7 +22121,7 @@
         <v>100</v>
       </c>
       <c r="J153" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K153" s="9">
         <v>0.3</v>
@@ -22228,7 +22162,7 @@
         <v>100</v>
       </c>
       <c r="J154" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K154" s="9">
         <v>0.5</v>
@@ -22269,7 +22203,7 @@
         <v>100</v>
       </c>
       <c r="J155" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K155" s="9">
         <v>0.1</v>
@@ -22310,7 +22244,7 @@
         <v>100</v>
       </c>
       <c r="J156" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K156" s="9">
         <v>0.6</v>
@@ -22351,7 +22285,7 @@
         <v>100</v>
       </c>
       <c r="J157" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K157" s="9">
         <v>7.0000000000000007E-2</v>
@@ -22392,7 +22326,7 @@
         <v>100</v>
       </c>
       <c r="J158" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K158" s="9">
         <v>0.8</v>
@@ -22433,7 +22367,7 @@
         <v>100</v>
       </c>
       <c r="J159" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K159" s="9">
         <v>0.3</v>
@@ -22474,7 +22408,7 @@
         <v>100</v>
       </c>
       <c r="J160" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K160" s="9">
         <v>0.5</v>
@@ -22515,7 +22449,7 @@
         <v>100</v>
       </c>
       <c r="J161" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K161" s="9">
         <v>0.1</v>
@@ -22556,7 +22490,7 @@
         <v>100</v>
       </c>
       <c r="J162" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K162" s="9">
         <v>0.6</v>
@@ -22597,7 +22531,7 @@
         <v>100</v>
       </c>
       <c r="J163" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K163" s="9">
         <v>7.0000000000000007E-2</v>
@@ -22638,7 +22572,7 @@
         <v>100</v>
       </c>
       <c r="J164" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K164" s="9">
         <v>0.8</v>
@@ -22679,7 +22613,7 @@
         <v>100</v>
       </c>
       <c r="J165" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K165" s="9">
         <v>0.3</v>
@@ -22720,7 +22654,7 @@
         <v>100</v>
       </c>
       <c r="J166" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K166" s="9">
         <v>0.11</v>
@@ -22761,7 +22695,7 @@
         <v>100</v>
       </c>
       <c r="J167" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K167" s="9">
         <v>0.13</v>
@@ -22802,7 +22736,7 @@
         <v>100</v>
       </c>
       <c r="J168" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K168" s="9">
         <v>0.14000000000000001</v>
@@ -22843,7 +22777,7 @@
         <v>100</v>
       </c>
       <c r="J169" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K169" s="9">
         <v>0.14000000000000001</v>
@@ -22884,7 +22818,7 @@
         <v>33</v>
       </c>
       <c r="J170" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K170" s="9">
         <v>0.89</v>
@@ -22925,7 +22859,7 @@
         <v>35</v>
       </c>
       <c r="J171" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K171" s="9">
         <v>0.11</v>
@@ -22966,7 +22900,7 @@
         <v>92</v>
       </c>
       <c r="J172" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K172" s="9">
         <v>0.04</v>
@@ -23007,7 +22941,7 @@
         <v>100</v>
       </c>
       <c r="J173" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K173" s="9">
         <v>0.04</v>
@@ -23048,7 +22982,7 @@
         <v>33</v>
       </c>
       <c r="J174" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K174" s="9">
         <v>0.89</v>
@@ -23089,7 +23023,7 @@
         <v>35</v>
       </c>
       <c r="J175" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K175" s="9">
         <v>0.11</v>
@@ -23130,7 +23064,7 @@
         <v>92</v>
       </c>
       <c r="J176" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K176" s="9">
         <v>0.04</v>
@@ -23171,7 +23105,7 @@
         <v>100</v>
       </c>
       <c r="J177" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K177" s="9">
         <v>0.04</v>
@@ -23212,7 +23146,7 @@
         <v>92</v>
       </c>
       <c r="J178" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K178" s="9">
         <v>0.04</v>
@@ -23253,7 +23187,7 @@
         <v>100</v>
       </c>
       <c r="J179" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K179" s="9">
         <v>0.04</v>
@@ -23294,7 +23228,7 @@
         <v>33</v>
       </c>
       <c r="J180" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K180" s="9">
         <v>0.89</v>
@@ -23335,7 +23269,7 @@
         <v>35</v>
       </c>
       <c r="J181" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K181" s="9">
         <v>0.11</v>
@@ -23376,7 +23310,7 @@
         <v>92</v>
       </c>
       <c r="J182" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K182" s="9">
         <v>0.04</v>
@@ -23417,7 +23351,7 @@
         <v>100</v>
       </c>
       <c r="J183" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K183" s="9">
         <v>0.04</v>
@@ -23458,7 +23392,7 @@
         <v>33</v>
       </c>
       <c r="J184" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K184" s="9">
         <v>0.89</v>
@@ -23499,7 +23433,7 @@
         <v>35</v>
       </c>
       <c r="J185" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K185" s="9">
         <v>0.11</v>
@@ -23540,7 +23474,7 @@
         <v>92</v>
       </c>
       <c r="J186" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K186" s="9">
         <v>0.04</v>
@@ -23581,7 +23515,7 @@
         <v>100</v>
       </c>
       <c r="J187" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K187" s="9">
         <v>0.04</v>
@@ -23622,7 +23556,7 @@
         <v>92</v>
       </c>
       <c r="J188" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K188" s="9">
         <v>0.04</v>
@@ -23663,7 +23597,7 @@
         <v>100</v>
       </c>
       <c r="J189" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K189" s="9">
         <v>0.04</v>
@@ -23704,7 +23638,7 @@
         <v>33</v>
       </c>
       <c r="J190" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K190" s="9">
         <v>0.89</v>
@@ -23745,7 +23679,7 @@
         <v>35</v>
       </c>
       <c r="J191" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K191" s="9">
         <v>0.11</v>
@@ -23786,7 +23720,7 @@
         <v>92</v>
       </c>
       <c r="J192" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K192" s="9">
         <v>0.04</v>
@@ -23827,7 +23761,7 @@
         <v>100</v>
       </c>
       <c r="J193" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K193" s="9">
         <v>0.04</v>
@@ -23868,7 +23802,7 @@
         <v>33</v>
       </c>
       <c r="J194" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K194" s="9">
         <v>0.89</v>
@@ -23909,7 +23843,7 @@
         <v>35</v>
       </c>
       <c r="J195" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K195" s="9">
         <v>0.11</v>
@@ -23950,7 +23884,7 @@
         <v>92</v>
       </c>
       <c r="J196" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K196" s="9">
         <v>0.04</v>
@@ -23991,7 +23925,7 @@
         <v>100</v>
       </c>
       <c r="J197" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K197" s="9">
         <v>0.04</v>
@@ -24032,7 +23966,7 @@
         <v>92</v>
       </c>
       <c r="J198" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K198" s="9">
         <v>0.04</v>
@@ -24073,7 +24007,7 @@
         <v>100</v>
       </c>
       <c r="J199" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K199" s="9">
         <v>0.04</v>
@@ -24114,7 +24048,7 @@
         <v>33</v>
       </c>
       <c r="J200" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K200" s="9">
         <v>0.89</v>
@@ -24155,7 +24089,7 @@
         <v>35</v>
       </c>
       <c r="J201" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K201" s="9">
         <v>0.11</v>
@@ -24196,7 +24130,7 @@
         <v>92</v>
       </c>
       <c r="J202" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K202" s="9">
         <v>0.04</v>
@@ -24237,7 +24171,7 @@
         <v>100</v>
       </c>
       <c r="J203" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K203" s="9">
         <v>0.04</v>
@@ -24278,7 +24212,7 @@
         <v>33</v>
       </c>
       <c r="J204" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K204" s="9">
         <v>0.89</v>
@@ -24319,7 +24253,7 @@
         <v>35</v>
       </c>
       <c r="J205" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K205" s="9">
         <v>0.11</v>
@@ -24360,7 +24294,7 @@
         <v>92</v>
       </c>
       <c r="J206" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K206" s="9">
         <v>0.04</v>
@@ -24401,7 +24335,7 @@
         <v>100</v>
       </c>
       <c r="J207" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K207" s="9">
         <v>0.04</v>
@@ -24442,7 +24376,7 @@
         <v>92</v>
       </c>
       <c r="J208" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K208" s="9">
         <v>0.04</v>
@@ -24483,7 +24417,7 @@
         <v>100</v>
       </c>
       <c r="J209" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K209" s="9">
         <v>0.04</v>
@@ -24524,7 +24458,7 @@
         <v>103</v>
       </c>
       <c r="J210" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K210" s="9">
         <v>0.1</v>
@@ -24565,7 +24499,7 @@
         <v>105</v>
       </c>
       <c r="J211" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K211" s="9">
         <v>0.2</v>
@@ -24606,7 +24540,7 @@
         <v>92</v>
       </c>
       <c r="J212" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="K212" s="9">
         <v>0</v>
@@ -24647,7 +24581,7 @@
         <v>100</v>
       </c>
       <c r="J213" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="K213" s="9">
         <v>0</v>
@@ -24688,7 +24622,7 @@
         <v>92</v>
       </c>
       <c r="J214" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="K214" s="9">
         <v>0</v>
@@ -24729,7 +24663,7 @@
         <v>100</v>
       </c>
       <c r="J215" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="K215" s="9">
         <v>0</v>
@@ -24770,7 +24704,7 @@
         <v>106</v>
       </c>
       <c r="J216" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="K216" s="9">
         <v>0</v>
@@ -24811,7 +24745,7 @@
         <v>108</v>
       </c>
       <c r="J217" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="K217" s="9">
         <v>0</v>
@@ -24852,7 +24786,7 @@
         <v>106</v>
       </c>
       <c r="J218" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="K218" s="9">
         <v>0</v>
@@ -24893,7 +24827,7 @@
         <v>108</v>
       </c>
       <c r="J219" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="K219" s="9">
         <v>0</v>
@@ -24934,7 +24868,7 @@
         <v>106</v>
       </c>
       <c r="J220" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K220" s="9">
         <v>0.1</v>
@@ -24975,7 +24909,7 @@
         <v>108</v>
       </c>
       <c r="J221" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="K221" s="9">
         <v>0.2</v>
@@ -48422,7 +48356,7 @@
   <sheetPr codeName="Hoja8"/>
   <dimension ref="A1:X9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="109" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="109" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
@@ -49547,6 +49481,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="7ab8c0d4-f18b-4fef-b649-c77d178c2495">
@@ -49557,7 +49500,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003456B0730C78B347BD7589BC061D6E7A" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="eb47ff602caa7ec4c93498109dbc0598">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7ab8c0d4-f18b-4fef-b649-c77d178c2495" xmlns:ns3="65efab6e-20b9-465e-9733-f0c2ab732419" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="15d39866744b831c8a58edb1b96951e3" ns2:_="" ns3:_="">
     <xsd:import namespace="7ab8c0d4-f18b-4fef-b649-c77d178c2495"/>
@@ -49758,16 +49701,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C685BDB-1785-4A39-A308-4CA166889A49}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE50E33B-922F-4D33-8831-2DF5BA7F11F6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -49778,7 +49720,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D43FA500-B4BA-4DED-8DE0-EA4A442F0F3F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -49797,14 +49739,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C685BDB-1785-4A39-A308-4CA166889A49}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{3c0bd4fe-1111-4d13-8e0c-7c33b9eb7581}" enabled="0" method="" siteId="{3c0bd4fe-1111-4d13-8e0c-7c33b9eb7581}" removed="1"/>

</xml_diff>